<commit_message>
20200817 21.41 for lathe model and gui
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86137\Desktop\micro_machinery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D212F4B-0699-4FA2-9583-EF325555B2BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91C096-208F-4E37-8327-B49CA0335BAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1066,9 +1066,6 @@
     <t>石砧</t>
   </si>
   <si>
-    <t>手持物品（1个）右键放置在砧上，手持锤子左键3次，产出成品，空手右键取下</t>
-  </si>
-  <si>
     <t>原矿→粉碎矿石</t>
   </si>
   <si>
@@ -1099,9 +1096,6 @@
     <t>车床</t>
   </si>
   <si>
-    <t>车削加工，5个按钮，根据顺序点击可以产出成品，否则产出粉末</t>
-  </si>
-  <si>
     <t>齿轮坯→齿轮</t>
   </si>
   <si>
@@ -1109,9 +1103,6 @@
   </si>
   <si>
     <t>锭→杆</t>
-  </si>
-  <si>
-    <t>杆→线</t>
   </si>
   <si>
     <t>杆→2螺丝</t>
@@ -2440,6 +2431,41 @@
   </si>
   <si>
     <t>fusing_machine</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>车削加工，选择加工项目：齿轮、杆、辊、螺丝，根据加工项目收取材料）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>手持物品（1个）右键放置在砧上，手持锤子</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>右</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>键3次，产出成品，空手右键取下</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>杆→线</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2498,12 +2524,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2518,7 +2550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2555,6 +2587,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2833,8 +2868,8 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P2" sqref="P2:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2894,49 +2929,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -2950,49 +2985,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3006,49 +3041,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3062,49 +3097,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3118,43 +3153,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3168,37 +3203,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3212,37 +3247,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3256,37 +3291,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3300,25 +3335,25 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3332,25 +3367,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3364,25 +3399,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3396,19 +3431,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3422,19 +3457,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3448,19 +3483,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3474,19 +3509,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3500,19 +3535,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3523,22 +3558,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3552,13 +3587,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3572,10 +3607,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3586,7 +3621,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -3735,109 +3770,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -3848,109 +3883,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -3961,109 +3996,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>188</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AH4" t="s">
         <v>189</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>190</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4074,109 +4109,109 @@
         <v>191</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>199</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>206</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AH5" t="s">
         <v>207</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>208</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4187,103 +4222,103 @@
         <v>209</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>217</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>218</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>225</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4294,37 +4329,37 @@
         <v>226</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>231</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4332,19 +4367,19 @@
         <v>232</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>233</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>234</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4352,31 +4387,31 @@
         <v>235</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>239</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4387,37 +4422,37 @@
         <v>240</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>245</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4425,19 +4460,19 @@
         <v>246</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>247</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>248</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
@@ -4445,31 +4480,31 @@
         <v>249</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>253</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4480,37 +4515,37 @@
         <v>254</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>259</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4518,19 +4553,19 @@
         <v>260</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>261</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="T9" s="9" t="s">
         <v>262</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4538,31 +4573,31 @@
         <v>263</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>267</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4573,37 +4608,37 @@
         <v>268</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>273</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -4611,13 +4646,13 @@
         <v>274</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>275</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
@@ -4627,31 +4662,31 @@
         <v>276</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>280</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -4662,37 +4697,37 @@
         <v>281</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>286</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -4700,13 +4735,13 @@
         <v>287</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>288</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
@@ -4716,13 +4751,13 @@
         <v>289</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>290</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -4730,13 +4765,13 @@
         <v>291</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>292</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -4747,37 +4782,37 @@
         <v>293</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>298</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -4787,7 +4822,7 @@
         <v>299</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
@@ -4797,13 +4832,13 @@
         <v>300</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>301</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -4811,13 +4846,13 @@
         <v>302</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>303</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -4828,37 +4863,37 @@
         <v>304</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -4880,7 +4915,7 @@
         <v>310</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -4891,31 +4926,31 @@
         <v>311</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>315</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -4939,7 +4974,7 @@
         <v>316</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -4954,19 +4989,19 @@
         <v>317</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>319</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -4990,7 +5025,7 @@
         <v>320</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5005,19 +5040,19 @@
         <v>321</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>323</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5041,7 +5076,7 @@
         <v>324</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5056,19 +5091,19 @@
         <v>325</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>327</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5089,10 +5124,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5107,19 +5142,19 @@
         <v>328</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>330</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5140,10 +5175,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5158,19 +5193,19 @@
         <v>331</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>333</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5191,10 +5226,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5209,13 +5244,13 @@
         <v>334</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>335</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5238,10 +5273,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5256,13 +5291,13 @@
         <v>336</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>337</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5285,10 +5320,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5305,7 +5340,7 @@
         <v>338</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5342,7 +5377,7 @@
         <v>339</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5379,7 +5414,7 @@
         <v>340</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5416,7 +5451,7 @@
         <v>341</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5453,7 +5488,7 @@
         <v>342</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5546,8 +5581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5582,25 +5617,28 @@
         <v>346</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>760</v>
-      </c>
-      <c r="D2" t="s">
+        <v>757</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>784</v>
+      </c>
+      <c r="E2" t="s">
         <v>347</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>348</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>349</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>350</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>351</v>
       </c>
-      <c r="I2" t="s">
-        <v>352</v>
+      <c r="J2" s="11" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5608,13 +5646,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>761</v>
-      </c>
-      <c r="D3" t="s">
-        <v>347</v>
+        <v>758</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5622,13 +5660,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>762</v>
-      </c>
-      <c r="D4" t="s">
-        <v>347</v>
+        <v>759</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5636,13 +5674,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>754</v>
+      </c>
+      <c r="D5" t="s">
         <v>355</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>757</v>
-      </c>
-      <c r="D5" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5650,31 +5688,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>755</v>
+      </c>
+      <c r="D6" t="s">
+        <v>783</v>
+      </c>
+      <c r="E6" t="s">
         <v>357</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>758</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>358</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>359</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
+        <v>361</v>
+      </c>
+      <c r="I6" t="s">
         <v>360</v>
-      </c>
-      <c r="G6" t="s">
-        <v>361</v>
-      </c>
-      <c r="H6" t="s">
-        <v>362</v>
-      </c>
-      <c r="I6" t="s">
-        <v>363</v>
-      </c>
-      <c r="J6" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5682,22 +5717,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>756</v>
+      </c>
+      <c r="D7" t="s">
+        <v>363</v>
+      </c>
+      <c r="E7" t="s">
+        <v>364</v>
+      </c>
+      <c r="F7" t="s">
         <v>365</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>759</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>366</v>
-      </c>
-      <c r="E7" t="s">
-        <v>367</v>
-      </c>
-      <c r="F7" t="s">
-        <v>368</v>
-      </c>
-      <c r="G7" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5705,13 +5740,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5719,13 +5754,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="E9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5733,19 +5768,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="E10" t="s">
+        <v>372</v>
+      </c>
+      <c r="F10" t="s">
+        <v>373</v>
+      </c>
+      <c r="G10" t="s">
         <v>374</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>765</v>
-      </c>
-      <c r="E10" t="s">
-        <v>375</v>
-      </c>
-      <c r="F10" t="s">
-        <v>376</v>
-      </c>
-      <c r="G10" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5753,13 +5788,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="E11" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5767,13 +5802,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="D12" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5781,10 +5816,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="E13" t="s">
         <v>134</v>
@@ -5802,10 +5837,10 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="K13" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5813,13 +5848,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="E14" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5827,13 +5862,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="E15" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5841,17 +5876,17 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G17" t="s">
         <v>345</v>
@@ -5861,17 +5896,17 @@
       <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>393</v>
+      <c r="B18" s="16" t="s">
+        <v>390</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -5879,23 +5914,23 @@
       <c r="A19" s="2">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>772</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="G19" t="s">
         <v>397</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="G19" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -5903,66 +5938,66 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>773</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>776</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="G20" t="s">
         <v>402</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="G20" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>4</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="G21" t="s">
         <v>406</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>777</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="G21" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="98" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>5</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>410</v>
+      <c r="B22" s="16" t="s">
+        <v>407</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.3">
@@ -5970,13 +6005,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -5986,43 +6021,43 @@
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>8</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>780</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="G25" s="8" t="s">
         <v>420</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6030,18 +6065,18 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="8" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
@@ -6049,20 +6084,20 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6070,20 +6105,20 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="168" x14ac:dyDescent="0.3">
@@ -6091,22 +6126,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>781</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>432</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>784</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6114,58 +6149,59 @@
         <v>13</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F30" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>14</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>439</v>
+      <c r="B31" s="16" t="s">
+        <v>436</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>15</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>442</v>
+      <c r="B32" s="16" t="s">
+        <v>439</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6184,7 +6220,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6192,7 +6228,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20200823 22.05 for qihua
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86137\Desktop\micro_machinery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91C096-208F-4E37-8327-B49CA0335BAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A6FC1-12C9-4112-BD97-692CA7B6C992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,9 +1198,6 @@
     <t>火电厂</t>
   </si>
   <si>
-    <t>根据机械方块等级，最高温度不同；温度提升机制：每20tick+1度，停止运行后每1tick-1度，最低温度24度；温度低于300度则不发电，300度以上效率为0.3，400度以上效率为0.7，500度以上效率为1.0,600度以上效率为1.8,750度以上效率为3.0；最高水量320桶，最低运行水量80桶，当前水量低于最低运行水量将强制停机；最高存电量10mFE，单口最高输出效率80kFE/tick；燃料消耗速度（提供的燃烧时间）：煤粉：200-190-170-130-80-20tick，IE生物柴油10mb：40-38-34-26-16-4，其他联动；最终耗水量=（当前温度-300）/当前水量百分比；最终发电量=最终耗水量*35*发电效率</t>
-  </si>
-  <si>
     <t>电量指示、温度指示、水量指示、启动拉杆、运行警示灯</t>
   </si>
   <si>
@@ -1214,9 +1211,6 @@
   </si>
   <si>
     <t>锤头</t>
-  </si>
-  <si>
-    <t>圆形铸件→1轴；锭→2线；锭→板；锭→2杆；4板→1管道</t>
   </si>
   <si>
     <t>浇注机</t>
@@ -2381,12 +2375,6 @@
   </si>
   <si>
     <t>thermal_power_plant</t>
-  </si>
-  <si>
-    <t>forging_press</t>
-  </si>
-  <si>
-    <t>reaction_still</t>
   </si>
   <si>
     <t>spherical_tank</t>
@@ -2466,6 +2454,22 @@
   </si>
   <si>
     <t>杆→线</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>reaction_still</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>forging_press</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆形铸件→1轴；锭→板；4板→1管道</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据机械方块等级，最高温度不同；温度提升机制：每10tick+1度，停止运行后每2tick-1度，最低温度24度；温度低于300度则不发电，300度以上效率为0.3，400度以上效率为0.5，500度以上效率为0.8,600度以上效率为1.2,750度以上效率为3.0；最高水量320桶，最低运行水量80桶，当前水量低于最低运行水量将强制停机；最高存电量100mFE，单口最高输出效率24kFE/tick；燃料消耗速度（提供的燃烧时间）：煤粉：25-22-19-14-10-5tick，IE生物柴油每tick消耗mb：1-2-5-10-15-20，其他联动；最终耗水量=（当前温度-300）/当前水量百分比；最终发电量=最终耗水量*8*发电效率</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2550,7 +2554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2590,6 +2594,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2929,49 +2934,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -2985,49 +2990,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3041,49 +3046,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3097,49 +3102,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3153,43 +3158,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3203,37 +3208,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3247,37 +3252,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3291,37 +3296,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="L9" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="M9" s="12" t="s">
         <v>523</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>525</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3335,25 +3340,25 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3367,25 +3372,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3399,25 +3404,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3431,19 +3436,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3457,19 +3462,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3483,19 +3488,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3509,19 +3514,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3535,19 +3540,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3558,22 +3563,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3587,13 +3592,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3607,10 +3612,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3621,7 +3626,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -3770,109 +3775,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -3883,109 +3888,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -3996,109 +4001,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>188</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AH4" t="s">
         <v>189</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>190</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4109,109 +4114,109 @@
         <v>191</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>199</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>206</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AH5" t="s">
         <v>207</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>208</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4222,103 +4227,103 @@
         <v>209</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>217</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>218</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>225</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4329,37 +4334,37 @@
         <v>226</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>231</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4367,19 +4372,19 @@
         <v>232</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>233</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>234</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4387,31 +4392,31 @@
         <v>235</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>239</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4422,37 +4427,37 @@
         <v>240</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>245</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4460,19 +4465,19 @@
         <v>246</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>247</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>248</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
@@ -4480,31 +4485,31 @@
         <v>249</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>253</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4515,37 +4520,37 @@
         <v>254</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>259</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4553,19 +4558,19 @@
         <v>260</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>261</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="T9" s="9" t="s">
         <v>262</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4573,31 +4578,31 @@
         <v>263</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>267</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4608,37 +4613,37 @@
         <v>268</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>273</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -4646,13 +4651,13 @@
         <v>274</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>275</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
@@ -4662,31 +4667,31 @@
         <v>276</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>280</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -4697,37 +4702,37 @@
         <v>281</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>286</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -4735,13 +4740,13 @@
         <v>287</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>288</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
@@ -4751,13 +4756,13 @@
         <v>289</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>290</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -4765,13 +4770,13 @@
         <v>291</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>292</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -4782,37 +4787,37 @@
         <v>293</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>298</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -4822,7 +4827,7 @@
         <v>299</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
@@ -4832,13 +4837,13 @@
         <v>300</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>301</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -4846,13 +4851,13 @@
         <v>302</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>303</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -4863,37 +4868,37 @@
         <v>304</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -4915,7 +4920,7 @@
         <v>310</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -4926,31 +4931,31 @@
         <v>311</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>315</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -4974,7 +4979,7 @@
         <v>316</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -4989,19 +4994,19 @@
         <v>317</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>319</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5025,7 +5030,7 @@
         <v>320</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5040,19 +5045,19 @@
         <v>321</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>323</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5076,7 +5081,7 @@
         <v>324</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5091,19 +5096,19 @@
         <v>325</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>327</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5124,10 +5129,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5142,19 +5147,19 @@
         <v>328</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>330</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5175,10 +5180,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5193,19 +5198,19 @@
         <v>331</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>333</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5226,10 +5231,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5244,13 +5249,13 @@
         <v>334</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>335</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5273,10 +5278,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5291,13 +5296,13 @@
         <v>336</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>337</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5320,10 +5325,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5340,7 +5345,7 @@
         <v>338</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5377,7 +5382,7 @@
         <v>339</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5414,7 +5419,7 @@
         <v>340</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5451,7 +5456,7 @@
         <v>341</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5488,7 +5493,7 @@
         <v>342</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5581,8 +5586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5613,14 +5618,14 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="17" t="s">
         <v>346</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="E2" t="s">
         <v>347</v>
@@ -5638,46 +5643,46 @@
         <v>351</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="17" t="s">
         <v>352</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="17" t="s">
         <v>353</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="17" t="s">
         <v>354</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D5" t="s">
         <v>355</v>
@@ -5687,14 +5692,14 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="17" t="s">
         <v>356</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D6" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="E6" t="s">
         <v>357</v>
@@ -5716,11 +5721,11 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="17" t="s">
         <v>362</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D7" t="s">
         <v>363</v>
@@ -5743,7 +5748,7 @@
         <v>367</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E8" t="s">
         <v>368</v>
@@ -5757,7 +5762,7 @@
         <v>369</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E9" t="s">
         <v>370</v>
@@ -5771,7 +5776,7 @@
         <v>371</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E10" t="s">
         <v>372</v>
@@ -5791,7 +5796,7 @@
         <v>375</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E11" t="s">
         <v>376</v>
@@ -5805,7 +5810,7 @@
         <v>377</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D12" t="s">
         <v>378</v>
@@ -5819,7 +5824,7 @@
         <v>379</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E13" t="s">
         <v>134</v>
@@ -5851,7 +5856,7 @@
         <v>382</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E14" t="s">
         <v>383</v>
@@ -5865,7 +5870,7 @@
         <v>384</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E15" t="s">
         <v>385</v>
@@ -5900,13 +5905,13 @@
         <v>390</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>391</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>392</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -5915,22 +5920,22 @@
         <v>2</v>
       </c>
       <c r="B19" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>783</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>769</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>396</v>
-      </c>
       <c r="G19" t="s">
-        <v>397</v>
+        <v>784</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -5938,22 +5943,22 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>773</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="F20" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="G20" t="s">
         <v>400</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="G20" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -5961,22 +5966,22 @@
         <v>4</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>770</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>774</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="G21" t="s">
         <v>404</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="G21" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="98" x14ac:dyDescent="0.3">
@@ -5984,20 +5989,20 @@
         <v>5</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>770</v>
+        <v>782</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.3">
@@ -6005,13 +6010,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -6021,20 +6026,20 @@
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>772</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>776</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>414</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="8" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.3">
@@ -6042,22 +6047,22 @@
         <v>8</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>773</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>777</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="F25" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="G25" s="8" t="s">
         <v>418</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6065,18 +6070,18 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
@@ -6084,20 +6089,20 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6105,20 +6110,20 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="168" x14ac:dyDescent="0.3">
@@ -6126,22 +6131,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>781</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="G29" s="8" t="s">
         <v>430</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6149,19 +6154,19 @@
         <v>13</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>778</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="F30" t="s">
         <v>433</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>782</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F30" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6169,16 +6174,16 @@
         <v>14</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>434</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>767</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>436</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>771</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6186,16 +6191,16 @@
         <v>15</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>772</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -6220,7 +6225,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6228,7 +6233,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20200829 17.21 for recipe
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86137\Desktop\micro_machinery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A6FC1-12C9-4112-BD97-692CA7B6C992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E0F998-836F-4C8E-8EA8-4568C22760A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -22,8 +22,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>胡清源</author>
+  </authors>
+  <commentList>
+    <comment ref="AG13" authorId="0" shapeId="0" xr:uid="{E6B9CEB0-A8B1-4AB6-8F78-859BBD03C147}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>hqyzsy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+探测右键的方块下方半径32格内的矿石，仅支持mm的矿石和原版铁矿煤矿金矿，数量大于4就在聊天栏里显示“下方微弱反馈”，大于16显示“下方较弱反馈”，大于32显示“下方明显反馈”，大于64显示“下方强烈反馈”</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="792">
   <si>
     <t>矿石</t>
   </si>
@@ -572,9 +608,6 @@
   </si>
   <si>
     <t>青铜轴</t>
-  </si>
-  <si>
-    <t>铁辊</t>
   </si>
   <si>
     <t>铁齿轮</t>
@@ -2013,9 +2046,6 @@
   </si>
   <si>
     <t>roll_hss</t>
-  </si>
-  <si>
-    <t>roll_iron</t>
   </si>
   <si>
     <t>slag</t>
@@ -2472,12 +2502,43 @@
     <t>根据机械方块等级，最高温度不同；温度提升机制：每10tick+1度，停止运行后每2tick-1度，最低温度24度；温度低于300度则不发电，300度以上效率为0.3，400度以上效率为0.5，500度以上效率为0.8,600度以上效率为1.2,750度以上效率为3.0；最高水量320桶，最低运行水量80桶，当前水量低于最低运行水量将强制停机；最高存电量100mFE，单口最高输出效率24kFE/tick；燃料消耗速度（提供的燃烧时间）：煤粉：25-22-19-14-10-5tick，IE生物柴油每tick消耗mb：1-2-5-10-15-20，其他联动；最终耗水量=（当前温度-300）/当前水量百分比；最终发电量=最终耗水量*8*发电效率</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>勘矿镐</t>
+  </si>
+  <si>
+    <t>prospector</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢辊</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>roll_steel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>铬轴</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>钴轴</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_chromium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_cobalt</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2526,6 +2587,21 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2874,7 +2950,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P2" sqref="P2:Q4"/>
+      <selection pane="topRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2934,49 +3010,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -2990,49 +3066,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3046,49 +3122,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3102,49 +3178,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3158,43 +3234,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3208,37 +3284,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3252,37 +3328,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3296,37 +3372,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3340,25 +3416,25 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3372,25 +3448,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3404,25 +3480,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3436,19 +3512,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3462,19 +3538,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3488,19 +3564,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3514,19 +3590,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3540,19 +3616,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3563,22 +3639,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>456</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>457</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3592,13 +3668,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3612,10 +3688,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3626,7 +3702,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -3664,12 +3740,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3775,109 +3851,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>666</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>148</v>
+        <v>667</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>786</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>651</v>
+        <v>787</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -3888,109 +3964,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>164</v>
+        <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="V3" s="9" t="s">
-        <v>165</v>
+        <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4001,109 +4077,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
         <v>664</v>
       </c>
       <c r="V4" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="W4" s="12" t="s">
-        <v>654</v>
-      </c>
-      <c r="X4" s="9" t="s">
+      <c r="Y4" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="Y4" s="12" t="s">
-        <v>691</v>
-      </c>
-      <c r="Z4" s="9" t="s">
+      <c r="AA4" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="AA4" s="12" t="s">
-        <v>680</v>
-      </c>
-      <c r="AB4" s="9" t="s">
+      <c r="AC4" s="12" t="s">
+        <v>656</v>
+      </c>
+      <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="AC4" s="12" t="s">
-        <v>658</v>
-      </c>
-      <c r="AD4" s="9" t="s">
+      <c r="AE4" s="12" t="s">
+        <v>707</v>
+      </c>
+      <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="AE4" s="12" t="s">
-        <v>709</v>
-      </c>
-      <c r="AF4" s="9" t="s">
+      <c r="AG4" s="12" t="s">
+        <v>537</v>
+      </c>
+      <c r="AH4" t="s">
         <v>188</v>
       </c>
-      <c r="AG4" s="12" t="s">
-        <v>538</v>
-      </c>
-      <c r="AH4" t="s">
+      <c r="AI4" s="12" t="s">
+        <v>549</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="AI4" s="12" t="s">
-        <v>550</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>190</v>
-      </c>
       <c r="AK4" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4111,112 +4187,112 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>697</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="12" t="s">
+        <v>713</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>715</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="12" t="s">
+        <v>553</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>554</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>574</v>
-      </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="K5" s="12" t="s">
-        <v>620</v>
-      </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>597</v>
-      </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="12" t="s">
+        <v>636</v>
+      </c>
+      <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="O5" s="12" t="s">
-        <v>637</v>
-      </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="Q5" s="12" t="s">
-        <v>642</v>
-      </c>
-      <c r="R5" s="9" t="s">
-        <v>199</v>
-      </c>
       <c r="S5" s="12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="T5" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>665</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="U5" s="12" t="s">
-        <v>669</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="W5" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="W5" s="12" t="s">
-        <v>652</v>
-      </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="Y5" s="12" t="s">
-        <v>687</v>
-      </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="12" t="s">
+        <v>674</v>
+      </c>
+      <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="AA5" s="12" t="s">
-        <v>676</v>
-      </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="AC5" s="12" t="s">
-        <v>659</v>
-      </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AE5" s="12" t="s">
+        <v>708</v>
+      </c>
+      <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="AE5" s="12" t="s">
-        <v>710</v>
-      </c>
-      <c r="AF5" s="10" t="s">
+      <c r="AG5" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="AH5" t="s">
         <v>206</v>
       </c>
-      <c r="AG5" s="12" t="s">
-        <v>539</v>
-      </c>
-      <c r="AH5" t="s">
+      <c r="AI5" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="AI5" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="AJ5" s="9" t="s">
-        <v>208</v>
-      </c>
       <c r="AK5" s="12" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4224,106 +4300,106 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>696</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>698</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="12" t="s">
+        <v>714</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>716</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="12" t="s">
+        <v>555</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>556</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>576</v>
-      </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>622</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>599</v>
-      </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="12" t="s">
+        <v>637</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="O6" s="12" t="s">
-        <v>638</v>
-      </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="Q6" s="12" t="s">
-        <v>648</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>217</v>
-      </c>
       <c r="S6" s="12" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>218</v>
+        <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="V6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="W6" s="12" t="s">
-        <v>650</v>
-      </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="12" t="s">
+        <v>682</v>
+      </c>
+      <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="Y6" s="12" t="s">
-        <v>684</v>
-      </c>
-      <c r="Z6" s="9" t="s">
+      <c r="AA6" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="AA6" s="12" t="s">
-        <v>673</v>
-      </c>
-      <c r="AB6" s="9" t="s">
+      <c r="AC6" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="AC6" s="12" t="s">
-        <v>656</v>
-      </c>
-      <c r="AD6" s="9" t="s">
+      <c r="AE6" s="12" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="AE6" s="12" t="s">
-        <v>711</v>
-      </c>
-      <c r="AF6" s="9" t="s">
+      <c r="AG6" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="AG6" s="12" t="s">
-        <v>540</v>
-      </c>
-      <c r="AJ6" s="9" t="s">
-        <v>225</v>
-      </c>
       <c r="AK6" s="12" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4331,92 +4407,92 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>697</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>699</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="12" t="s">
+        <v>716</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>718</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>557</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="I7" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>577</v>
-      </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="12" t="s">
+        <v>627</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>628</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>231</v>
-      </c>
       <c r="M7" s="12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>642</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="Q7" s="12" t="s">
-        <v>643</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>233</v>
-      </c>
       <c r="S7" s="13" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>234</v>
+        <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
       <c r="X7" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="Y7" s="12" t="s">
-        <v>692</v>
-      </c>
-      <c r="Z7" s="9" t="s">
+      <c r="AA7" s="12" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="AA7" s="12" t="s">
-        <v>681</v>
-      </c>
-      <c r="AB7" s="9" t="s">
+      <c r="AC7" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="AC7" s="12" t="s">
-        <v>661</v>
-      </c>
-      <c r="AF7" s="9" t="s">
+      <c r="AG7" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="AG7" s="12" t="s">
-        <v>542</v>
-      </c>
-      <c r="AJ7" s="9" t="s">
-        <v>239</v>
-      </c>
       <c r="AK7" s="12" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4424,92 +4500,92 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>698</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>700</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="12" t="s">
+        <v>717</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>719</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>563</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>584</v>
-      </c>
-      <c r="J8" s="9" t="s">
+      <c r="K8" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>621</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>245</v>
-      </c>
       <c r="M8" s="12" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="Q8" s="12" t="s">
-        <v>644</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>247</v>
-      </c>
       <c r="S8" s="12" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="T8" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="U8" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="V8" s="9"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="U8" s="12" t="s">
-        <v>667</v>
-      </c>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9" t="s">
+      <c r="Y8" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="Y8" s="12" t="s">
-        <v>690</v>
-      </c>
-      <c r="Z8" s="9" t="s">
+      <c r="AA8" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="AA8" s="12" t="s">
-        <v>679</v>
-      </c>
-      <c r="AB8" s="9" t="s">
+      <c r="AC8" s="12" t="s">
+        <v>660</v>
+      </c>
+      <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="AC8" s="12" t="s">
-        <v>662</v>
-      </c>
-      <c r="AF8" s="9" t="s">
+      <c r="AG8" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="AG8" s="12" t="s">
-        <v>541</v>
-      </c>
-      <c r="AJ8" s="9" t="s">
-        <v>253</v>
-      </c>
       <c r="AK8" s="12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4517,92 +4593,92 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>699</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>701</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="12" t="s">
+        <v>718</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>720</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>555</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="J9" s="9" t="s">
+      <c r="K9" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>623</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>259</v>
-      </c>
       <c r="M9" s="12" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>644</v>
+      </c>
+      <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="Q9" s="12" t="s">
-        <v>645</v>
-      </c>
-      <c r="R9" s="9" t="s">
-        <v>261</v>
-      </c>
       <c r="S9" s="12" t="s">
-        <v>613</v>
-      </c>
-      <c r="T9" s="9" t="s">
-        <v>262</v>
+        <v>612</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>788</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>665</v>
+        <v>790</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
       <c r="X9" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y9" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="Y9" s="12" t="s">
-        <v>688</v>
-      </c>
-      <c r="Z9" s="9" t="s">
+      <c r="AA9" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="AA9" s="12" t="s">
-        <v>677</v>
-      </c>
-      <c r="AB9" s="9" t="s">
+      <c r="AC9" s="12" t="s">
+        <v>661</v>
+      </c>
+      <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="AC9" s="12" t="s">
-        <v>663</v>
-      </c>
-      <c r="AF9" s="9" t="s">
+      <c r="AG9" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="AG9" s="12" t="s">
-        <v>543</v>
-      </c>
-      <c r="AJ9" s="9" t="s">
-        <v>267</v>
-      </c>
       <c r="AK9" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4610,88 +4686,92 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>700</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>702</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="12" t="s">
+        <v>719</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>721</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>558</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="I10" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>578</v>
-      </c>
-      <c r="J10" s="9" t="s">
+      <c r="K10" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="K10" s="12" t="s">
-        <v>624</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>273</v>
-      </c>
       <c r="M10" s="12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>645</v>
+      </c>
+      <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="Q10" s="12" t="s">
-        <v>646</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>275</v>
-      </c>
       <c r="S10" s="12" t="s">
-        <v>614</v>
-      </c>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
+        <v>613</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>668</v>
+      </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y10" s="12" t="s">
+        <v>683</v>
+      </c>
+      <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="Y10" s="12" t="s">
-        <v>685</v>
-      </c>
-      <c r="Z10" s="9" t="s">
+      <c r="AA10" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="AA10" s="12" t="s">
-        <v>674</v>
-      </c>
-      <c r="AB10" s="9" t="s">
+      <c r="AC10" s="12" t="s">
+        <v>658</v>
+      </c>
+      <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="AC10" s="12" t="s">
-        <v>660</v>
-      </c>
-      <c r="AF10" s="9" t="s">
+      <c r="AG10" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="AG10" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="AJ10" s="9" t="s">
-        <v>280</v>
-      </c>
       <c r="AK10" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -4699,84 +4779,88 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>701</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>703</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="12" t="s">
+        <v>720</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>722</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>579</v>
-      </c>
-      <c r="J11" s="9" t="s">
+      <c r="K11" s="12" t="s">
+        <v>625</v>
+      </c>
+      <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>626</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>286</v>
-      </c>
       <c r="M11" s="12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>646</v>
+      </c>
+      <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="Q11" s="12" t="s">
-        <v>647</v>
-      </c>
-      <c r="R11" s="9" t="s">
-        <v>288</v>
-      </c>
       <c r="S11" s="12" t="s">
-        <v>615</v>
-      </c>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
+        <v>614</v>
+      </c>
+      <c r="T11" s="14" t="s">
+        <v>789</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>791</v>
+      </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y11" s="12" t="s">
+        <v>684</v>
+      </c>
+      <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="Y11" s="12" t="s">
-        <v>686</v>
-      </c>
-      <c r="Z11" s="9" t="s">
-        <v>290</v>
-      </c>
       <c r="AA11" s="12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
       <c r="AF11" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="AG11" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="AG11" s="12" t="s">
-        <v>544</v>
-      </c>
-      <c r="AJ11" s="9" t="s">
-        <v>292</v>
-      </c>
       <c r="AK11" s="12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -4784,80 +4868,78 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>702</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>704</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="12" t="s">
+        <v>721</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>723</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="G12" s="12" t="s">
+        <v>559</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>560</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>581</v>
-      </c>
-      <c r="J12" s="9" t="s">
+      <c r="K12" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>627</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>298</v>
-      </c>
       <c r="M12" s="12" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>616</v>
-      </c>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
+        <v>615</v>
+      </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y12" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="Y12" s="12" t="s">
-        <v>689</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>301</v>
-      </c>
       <c r="AA12" s="12" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
       <c r="AF12" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG12" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="AG12" s="12" t="s">
-        <v>546</v>
-      </c>
-      <c r="AJ12" s="9" t="s">
-        <v>303</v>
-      </c>
       <c r="AK12" s="12" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -4865,40 +4947,40 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>704</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>706</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="12" t="s">
+        <v>715</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>717</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>561</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="I13" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>582</v>
-      </c>
-      <c r="J13" s="9" t="s">
+      <c r="K13" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="K13" s="12" t="s">
-        <v>629</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>309</v>
-      </c>
       <c r="M13" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -4916,11 +4998,17 @@
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
+      <c r="AF13" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="AG13" s="12" t="s">
+        <v>785</v>
+      </c>
       <c r="AJ13" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -4928,34 +5016,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>703</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>705</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="12" t="s">
+        <v>722</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>724</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="12" t="s">
+        <v>561</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>562</v>
-      </c>
-      <c r="H14" s="9" t="s">
+      <c r="I14" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>583</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>315</v>
-      </c>
       <c r="K14" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -4975,11 +5063,12 @@
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
       <c r="AC14" s="9"/>
+      <c r="AF14" s="10"/>
       <c r="AJ14" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -4991,22 +5080,22 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>564</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="I15" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>585</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>319</v>
-      </c>
       <c r="K15" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5027,10 +5116,10 @@
       <c r="AB15" s="9"/>
       <c r="AC15" s="9"/>
       <c r="AJ15" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5042,22 +5131,22 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>565</v>
-      </c>
-      <c r="H16" s="9" t="s">
+      <c r="I16" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>586</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>323</v>
-      </c>
       <c r="K16" s="12" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5078,10 +5167,10 @@
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
       <c r="AJ16" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5093,22 +5182,22 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>566</v>
-      </c>
-      <c r="H17" s="9" t="s">
+      <c r="I17" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>587</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>327</v>
-      </c>
       <c r="K17" s="12" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5129,10 +5218,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5144,22 +5233,22 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>567</v>
-      </c>
-      <c r="H18" s="9" t="s">
+      <c r="I18" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="I18" s="12" t="s">
-        <v>588</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>330</v>
-      </c>
       <c r="K18" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5180,10 +5269,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5195,22 +5284,22 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>568</v>
-      </c>
-      <c r="H19" s="9" t="s">
+      <c r="I19" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>589</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>333</v>
-      </c>
       <c r="K19" s="12" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5231,10 +5320,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5246,16 +5335,16 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>569</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>335</v>
-      </c>
       <c r="I20" s="12" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5278,10 +5367,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5293,16 +5382,16 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="G21" s="12" t="s">
-        <v>570</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>337</v>
-      </c>
       <c r="I21" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5325,10 +5414,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5342,10 +5431,10 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5379,10 +5468,10 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5416,10 +5505,10 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5453,10 +5542,10 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5490,10 +5579,10 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5579,6 +5668,8 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5586,7 +5677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -5604,14 +5695,14 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5619,31 +5710,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>753</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>778</v>
+      </c>
+      <c r="E2" t="s">
         <v>346</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>755</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>780</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>347</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>348</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>349</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>350</v>
       </c>
-      <c r="I2" t="s">
-        <v>351</v>
-      </c>
       <c r="J2" s="11" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5651,13 +5742,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5665,13 +5756,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5679,13 +5770,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>750</v>
+      </c>
+      <c r="D5" t="s">
         <v>354</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>752</v>
-      </c>
-      <c r="D5" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5693,28 +5784,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>751</v>
+      </c>
+      <c r="D6" t="s">
+        <v>777</v>
+      </c>
+      <c r="E6" t="s">
         <v>356</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>753</v>
-      </c>
-      <c r="D6" t="s">
-        <v>779</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>357</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>358</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>360</v>
+      </c>
+      <c r="I6" t="s">
         <v>359</v>
-      </c>
-      <c r="H6" t="s">
-        <v>361</v>
-      </c>
-      <c r="I6" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5722,22 +5813,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>752</v>
+      </c>
+      <c r="D7" t="s">
         <v>362</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>754</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>363</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>364</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>365</v>
-      </c>
-      <c r="G7" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5745,13 +5836,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>756</v>
+      </c>
+      <c r="E8" t="s">
         <v>367</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>758</v>
-      </c>
-      <c r="E8" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5759,13 +5850,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>368</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>757</v>
+      </c>
+      <c r="E9" t="s">
         <v>369</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>759</v>
-      </c>
-      <c r="E9" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5773,19 +5864,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>758</v>
+      </c>
+      <c r="E10" t="s">
         <v>371</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>760</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>372</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>373</v>
-      </c>
-      <c r="G10" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5793,13 +5884,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>374</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>759</v>
+      </c>
+      <c r="E11" t="s">
         <v>375</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>761</v>
-      </c>
-      <c r="E11" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5807,13 +5898,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>376</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>760</v>
+      </c>
+      <c r="D12" t="s">
         <v>377</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>762</v>
-      </c>
-      <c r="D12" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5821,16 +5912,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E13" t="s">
         <v>134</v>
       </c>
       <c r="F13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
@@ -5842,10 +5933,10 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
+        <v>379</v>
+      </c>
+      <c r="K13" t="s">
         <v>380</v>
-      </c>
-      <c r="K13" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5853,13 +5944,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>381</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="E14" t="s">
         <v>382</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>764</v>
-      </c>
-      <c r="E14" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5867,13 +5958,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>383</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>763</v>
+      </c>
+      <c r="E15" t="s">
         <v>384</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>765</v>
-      </c>
-      <c r="E15" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5881,20 +5972,20 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>389</v>
-      </c>
       <c r="G17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="138" customHeight="1" x14ac:dyDescent="0.3">
@@ -5902,16 +5993,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>764</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>390</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>766</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>785</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>391</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -5920,22 +6011,22 @@
         <v>2</v>
       </c>
       <c r="B19" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>781</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>783</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>395</v>
-      </c>
       <c r="G19" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -5943,22 +6034,22 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>767</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>769</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" t="s">
         <v>399</v>
-      </c>
-      <c r="G20" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -5966,22 +6057,22 @@
         <v>4</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>770</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="G21" t="s">
         <v>403</v>
-      </c>
-      <c r="G21" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="98" x14ac:dyDescent="0.3">
@@ -5989,20 +6080,20 @@
         <v>5</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>780</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>782</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>406</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.3">
@@ -6010,13 +6101,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>408</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>771</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -6026,20 +6117,20 @@
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>770</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>772</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>412</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.3">
@@ -6047,22 +6138,22 @@
         <v>8</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>771</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>773</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="8" t="s">
         <v>417</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6070,18 +6161,18 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
@@ -6089,20 +6180,20 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>773</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>775</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>422</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6110,20 +6201,20 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>776</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>425</v>
-      </c>
       <c r="E28" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="168" x14ac:dyDescent="0.3">
@@ -6131,22 +6222,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>777</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="8" t="s">
         <v>429</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6154,19 +6245,19 @@
         <v>13</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>776</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>778</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="F30" t="s">
         <v>432</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="F30" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6174,16 +6265,16 @@
         <v>14</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>765</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>767</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6191,16 +6282,16 @@
         <v>15</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>766</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>768</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -6225,7 +6316,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6233,7 +6324,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20200830 14.00 for vein
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86137\Desktop\micro_machinery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E0F998-836F-4C8E-8EA8-4568C22760A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F15BF0-9EB6-4052-8466-D27520059410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-探测右键的方块下方半径32格内的矿石，仅支持mm的矿石和原版铁矿煤矿金矿，数量大于4就在聊天栏里显示“下方微弱反馈”，大于16显示“下方较弱反馈”，大于32显示“下方明显反馈”，大于64显示“下方强烈反馈”</t>
+探测右键的方块下方半径16格内的矿石，仅支持mm的矿石和原版铁矿煤矿金矿，数量大于4就在聊天栏里显示“下方微弱反馈”，大于16显示“下方较弱反馈”，大于32显示“下方明显反馈”，大于64显示“下方强烈反馈”</t>
         </r>
       </text>
     </comment>
@@ -3743,9 +3743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
20200906 13.41 for resource
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F15BF0-9EB6-4052-8466-D27520059410}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15E1B17-47B2-4E58-9B12-ECDA8BCBA56E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -3743,7 +3743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
@@ -5677,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
20200911 11.21 for many things
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15E1B17-47B2-4E58-9B12-ECDA8BCBA56E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B60C39A-DA94-4096-9591-0832868EBC61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1669,26 +1669,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>lead_copper</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>lead_nickel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>lead_aluminum</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>lead_tungsten</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>lead_cobalt</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>logistics_steel</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2532,6 +2512,26 @@
   <si>
     <t>axis_cobalt</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>copper_cable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>nickel_cable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>aluminum_cable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tungsten_cable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cobalt_cable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2948,9 +2948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I3" sqref="I3"/>
+      <selection pane="topRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3108,7 +3108,7 @@
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3358,7 +3358,7 @@
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>529</v>
+        <v>787</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3402,7 +3402,7 @@
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>530</v>
+        <v>788</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3434,7 +3434,7 @@
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>531</v>
+        <v>789</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3466,7 +3466,7 @@
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>532</v>
+        <v>790</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3498,7 +3498,7 @@
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>533</v>
+        <v>791</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3743,7 +3743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AJ14" sqref="AJ14"/>
     </sheetView>
@@ -3851,109 +3851,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -3964,109 +3964,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4077,109 +4077,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4190,109 +4190,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4303,103 +4303,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4410,37 +4410,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4448,19 +4448,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4468,31 +4468,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4503,37 +4503,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4541,19 +4541,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4561,31 +4561,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4596,37 +4596,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4634,19 +4634,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4654,31 +4654,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4689,37 +4689,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -4727,19 +4727,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -4747,31 +4747,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -4782,37 +4782,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -4820,19 +4820,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -4840,13 +4840,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -4854,13 +4854,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -4871,37 +4871,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -4911,7 +4911,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -4919,13 +4919,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -4933,13 +4933,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -4950,37 +4950,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -4999,16 +4999,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5019,31 +5019,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5068,7 +5068,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5083,19 +5083,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5119,7 +5119,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5134,19 +5134,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5170,7 +5170,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5185,19 +5185,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5218,10 +5218,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5236,19 +5236,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5269,10 +5269,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5287,19 +5287,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5320,10 +5320,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5338,13 +5338,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5367,10 +5367,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5385,13 +5385,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5414,10 +5414,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5434,7 +5434,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5471,7 +5471,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5508,7 +5508,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5545,7 +5545,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5582,7 +5582,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5677,7 +5677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5713,10 +5713,10 @@
         <v>345</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="E2" t="s">
         <v>346</v>
@@ -5734,7 +5734,7 @@
         <v>350</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5745,10 +5745,10 @@
         <v>351</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5759,10 +5759,10 @@
         <v>352</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5773,7 +5773,7 @@
         <v>353</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="D5" t="s">
         <v>354</v>
@@ -5787,10 +5787,10 @@
         <v>355</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="D6" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="E6" t="s">
         <v>356</v>
@@ -5816,7 +5816,7 @@
         <v>361</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="D7" t="s">
         <v>362</v>
@@ -5839,7 +5839,7 @@
         <v>366</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="E8" t="s">
         <v>367</v>
@@ -5853,7 +5853,7 @@
         <v>368</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="E9" t="s">
         <v>369</v>
@@ -5867,7 +5867,7 @@
         <v>370</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="E10" t="s">
         <v>371</v>
@@ -5887,7 +5887,7 @@
         <v>374</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="E11" t="s">
         <v>375</v>
@@ -5901,7 +5901,7 @@
         <v>376</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="D12" t="s">
         <v>377</v>
@@ -5915,7 +5915,7 @@
         <v>378</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="E13" t="s">
         <v>134</v>
@@ -5947,7 +5947,7 @@
         <v>381</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="E14" t="s">
         <v>382</v>
@@ -5961,7 +5961,7 @@
         <v>383</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="E15" t="s">
         <v>384</v>
@@ -5996,10 +5996,10 @@
         <v>389</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>390</v>
@@ -6014,7 +6014,7 @@
         <v>391</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>392</v>
@@ -6026,7 +6026,7 @@
         <v>394</v>
       </c>
       <c r="G19" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6037,7 +6037,7 @@
         <v>395</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>396</v>
@@ -6060,7 +6060,7 @@
         <v>400</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>401</v>
@@ -6083,7 +6083,7 @@
         <v>404</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>405</v>
@@ -6104,7 +6104,7 @@
         <v>407</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>408</v>
@@ -6120,7 +6120,7 @@
         <v>409</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>410</v>
@@ -6141,7 +6141,7 @@
         <v>413</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>414</v>
@@ -6164,7 +6164,7 @@
         <v>418</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
@@ -6183,7 +6183,7 @@
         <v>420</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>421</v>
@@ -6204,7 +6204,7 @@
         <v>423</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>424</v>
@@ -6225,7 +6225,7 @@
         <v>426</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>427</v>
@@ -6248,7 +6248,7 @@
         <v>430</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>431</v>
@@ -6268,7 +6268,7 @@
         <v>433</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>434</v>
@@ -6285,7 +6285,7 @@
         <v>436</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>437</v>

</xml_diff>

<commit_message>
20200923 21.44 for 设定
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B60C39A-DA94-4096-9591-0832868EBC61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A223CAB-1983-47B4-9FE0-CABD9F2A70C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="798">
   <si>
     <t>矿石</t>
   </si>
@@ -1123,33 +1123,12 @@
     <t>窑</t>
   </si>
   <si>
-    <t>金属产出率90%，具有三个模板，可以熔炼青铜合金【锭160mb、杆80mb、板160mb】</t>
-  </si>
-  <si>
     <t>车床</t>
   </si>
   <si>
-    <t>齿轮坯→齿轮</t>
-  </si>
-  <si>
-    <t>5锭→齿轮</t>
-  </si>
-  <si>
-    <t>锭→杆</t>
-  </si>
-  <si>
-    <t>杆→2螺丝</t>
-  </si>
-  <si>
-    <t>轴→辊</t>
-  </si>
-  <si>
     <t>切割机</t>
   </si>
   <si>
-    <t>切断整材</t>
-  </si>
-  <si>
     <t>块→8板</t>
   </si>
   <si>
@@ -1192,9 +1171,6 @@
     <t>电动泵</t>
   </si>
   <si>
-    <t>可以抽取正下方的液体，若泵正下方为2*2的水源方块，不抽取世界水，直接生成水</t>
-  </si>
-  <si>
     <t>焊接室</t>
   </si>
   <si>
@@ -1237,9 +1213,6 @@
     <t>锻压机</t>
   </si>
   <si>
-    <t>所有工作时间相同（便于动画效果实现）正在运行的配方将会把物品渲染在操作台上，然后锤头压下去完成工作</t>
-  </si>
-  <si>
     <t>电量指示、启动拉杆、运行警示灯</t>
   </si>
   <si>
@@ -1249,9 +1222,6 @@
     <t>浇注机</t>
   </si>
   <si>
-    <t>浇筑开启后，钢包倾斜，流体块渲染，模具液面提升；随后钢包回归位置，浇筑完成后模具液面消失</t>
-  </si>
-  <si>
     <t>电量指示、启动拉杆、运行警示灯、清空拉杆</t>
   </si>
   <si>
@@ -1264,9 +1234,6 @@
     <t>连铸轧钢厂</t>
   </si>
   <si>
-    <t>钢包液面根据容量确定高度，开始工作后，金属条抽出，移动到轧钢滚轮处，生成一块块金属板</t>
-  </si>
-  <si>
     <t>钢包液面，金属条，轧钢滚轮，金属板</t>
   </si>
   <si>
@@ -1276,9 +1243,6 @@
     <t>反应釜</t>
   </si>
   <si>
-    <t>四个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）；</t>
-  </si>
-  <si>
     <t>苹果+水→苹果汁；烈焰粉+苹果汁→苹果糖；金锭+苹果汁→金苹果汁；紫颂花+金苹果汁→金苹果糖；腐化蜘蛛眼+苹果汁→乙烯；烈焰粉+乙烯→聚乙烯片</t>
   </si>
   <si>
@@ -1291,9 +1255,6 @@
     <t>电力高炉</t>
   </si>
   <si>
-    <t>温度提升速度和耗电速度根据线圈材料决定，最高温度根据机械方块决定，高炉温度-产物流体温度≥0时，配方开启运行，运行时间为额定热量/升温速度，运行期间高炉温度不增加，停止运行时，温度每tick-10度（即检测到可运行配方时开启升温）</t>
-  </si>
-  <si>
     <t>电量指示、启动拉杆、运行警示灯、温度指示</t>
   </si>
   <si>
@@ -1303,9 +1264,6 @@
     <t>破碎机</t>
   </si>
   <si>
-    <t>最高转速根据机械方块等级不同，配方实际工作时间=设计工作时间/(10/转速)，转速每10tick+20，不工作时每tick-20；工作时，转轴每秒转一圈</t>
-  </si>
-  <si>
     <t>电量指示、启动拉杆、运行警示灯、转速表</t>
   </si>
   <si>
@@ -1322,9 +1280,6 @@
   </si>
   <si>
     <t>单晶炉</t>
-  </si>
-  <si>
-    <t>根据投入的籽晶不同，产物不同</t>
   </si>
   <si>
     <t>硅锭+64硅粉→1单晶硅；石英+64硅粉→64石英；钻石+64碳粉→2钻石；石墨锭+32碳粉→2石墨锭</t>
@@ -2250,10 +2205,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>齿轮模具</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>剑模具</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2264,9 +2215,6 @@
     <t>cast_stick</t>
   </si>
   <si>
-    <t>cast_gear</t>
-  </si>
-  <si>
     <t>cast_sword</t>
   </si>
   <si>
@@ -2429,10 +2377,6 @@
   </si>
   <si>
     <t>fusing_machine</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>车削加工，选择加工项目：齿轮、杆、辊、螺丝，根据加工项目收取材料）</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -2532,6 +2476,307 @@
   <si>
     <t>cobalt_cable</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>齿轮坯模具</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>cast_gear_blank</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>齿轮坯→齿轮（钻削，镗孔</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>锭→杆（刨削，磨削</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>轴→辊（钻削，车削</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>杆→2螺丝（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>铣削，车削</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>金属产出率90%，具有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>四</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>个模板，可以熔炼青铜合金【锭160mb、杆80mb、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>齿轮坯640</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mb、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>剑刃320mb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>】</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>每tick发电</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>车削加工，选择加工项目：齿轮、杆、辊、螺丝，根据加工项目收取材料）钻削-5，车削-10，铣削-7，磨削-2，刨削-4，镗孔-3，车床最大电容量40000fe，每次加工消耗6400fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>最大电容量80000fe，每tick消耗80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>可以抽取正下方的液体，若泵正下方为2*2的水源方块，不抽取世界水，直接生成水（最大电容量3200fe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，每</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tick</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>消耗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>最大电容量32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000fe，每tick消耗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4096fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有工作时间相同（便于动画效果实现）正在运行的配方将会把物品渲染在操作台上，然后锤头压下去完成工作</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>浇筑开启后，钢包倾斜，流体块渲染，模具液面提升；随后钢包回归位置，浇筑完成后模具液面消失</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢包液面根据容量确定高度，开始工作后，金属条抽出，移动到轧钢滚轮处，生成一块块金属板</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>四个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>温度提升速度和耗电速度根据线圈材料决定，最高温度根据机械方块决定，高炉温度-产物流体温度≥0时，配方开启运行，运行时间为额定热量/升温速度，运行期间高炉温度不增加，停止运行时，温度每tick-10度（即检测到可运行配方时开启升温）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高转速根据机械方块等级不同，配方实际工作时间=设计工作时间/(10/转速)，转速每10tick+20，不工作时每tick-20；工作时，转轴每秒转一圈</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据投入的籽晶不同，产物不同</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大电容量120000fe，每tick消耗1024fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大电容量40000fe，每tick消耗128fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>最大电容量8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000fe，每tick消耗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>256fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>切断整材，最大电容量40000fe，每tick消耗128fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大电容40000fe，每tick发电16fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2630,7 +2875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2671,6 +2916,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2949,7 +3203,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -3010,49 +3264,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>524</v>
+        <v>509</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3066,49 +3320,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>529</v>
+        <v>514</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3122,49 +3376,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>509</v>
+        <v>494</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>525</v>
+        <v>510</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3178,49 +3432,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>516</v>
+        <v>501</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>510</v>
+        <v>495</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>526</v>
+        <v>511</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3234,43 +3488,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>521</v>
+        <v>506</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>527</v>
+        <v>512</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3284,37 +3538,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>523</v>
+        <v>508</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>528</v>
+        <v>513</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3328,37 +3582,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>515</v>
+        <v>500</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>513</v>
+        <v>498</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>787</v>
+        <v>769</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3372,37 +3626,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>504</v>
+        <v>489</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>520</v>
+        <v>505</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>514</v>
+        <v>499</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>788</v>
+        <v>770</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3416,25 +3670,25 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>789</v>
+        <v>771</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3448,25 +3702,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>790</v>
+        <v>772</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3480,25 +3734,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>791</v>
+        <v>773</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3512,19 +3766,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3538,19 +3792,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3564,19 +3818,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3590,19 +3844,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3616,19 +3870,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>502</v>
+        <v>487</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3639,22 +3893,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>503</v>
+        <v>488</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3668,13 +3922,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3688,10 +3942,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3702,7 +3956,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -3745,7 +3999,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ14" sqref="AJ14"/>
+      <selection pane="topRight" activeCell="AK19" sqref="AK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3851,109 +4105,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>687</v>
+        <v>672</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>705</v>
+        <v>690</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>611</v>
+        <v>596</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>588</v>
+        <v>573</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>629</v>
+        <v>614</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>600</v>
+        <v>585</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>781</v>
+        <v>763</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>782</v>
+        <v>764</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>726</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -3964,109 +4218,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>706</v>
+        <v>691</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>546</v>
+        <v>531</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>612</v>
+        <v>597</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>601</v>
+        <v>586</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>701</v>
+        <v>686</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>541</v>
+        <v>526</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>727</v>
+        <v>710</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4077,109 +4331,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>707</v>
+        <v>692</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>567</v>
+        <v>552</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>613</v>
+        <v>598</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>590</v>
+        <v>575</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>630</v>
+        <v>615</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>643</v>
+        <v>628</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>602</v>
+        <v>587</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>659</v>
+        <v>644</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>684</v>
+        <v>669</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>673</v>
+        <v>658</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>702</v>
+        <v>687</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>532</v>
+        <v>517</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>544</v>
+        <v>529</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>728</v>
+        <v>711</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4190,109 +4444,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>708</v>
+        <v>693</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>548</v>
+        <v>533</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>614</v>
+        <v>599</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>591</v>
+        <v>576</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>603</v>
+        <v>588</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>680</v>
+        <v>665</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>669</v>
+        <v>654</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>703</v>
+        <v>688</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>542</v>
+        <v>527</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>729</v>
+        <v>712</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4303,103 +4557,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>691</v>
+        <v>676</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>709</v>
+        <v>694</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>550</v>
+        <v>535</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>616</v>
+        <v>601</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>593</v>
+        <v>578</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>604</v>
+        <v>589</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>661</v>
+        <v>646</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>677</v>
+        <v>662</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>704</v>
+        <v>689</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>730</v>
+        <v>713</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4410,37 +4664,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>692</v>
+        <v>677</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>711</v>
+        <v>696</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>571</v>
+        <v>556</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>592</v>
+        <v>577</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4448,19 +4702,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>637</v>
+        <v>622</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>605</v>
+        <v>590</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>657</v>
+        <v>642</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4468,31 +4722,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>654</v>
+        <v>639</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>731</v>
+        <v>714</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4503,37 +4757,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>712</v>
+        <v>697</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>578</v>
+        <v>563</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>615</v>
+        <v>600</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>594</v>
+        <v>579</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4541,19 +4795,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>606</v>
+        <v>591</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>664</v>
+        <v>649</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4561,31 +4815,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>683</v>
+        <v>668</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>655</v>
+        <v>640</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>732</v>
+        <v>715</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4596,37 +4850,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>694</v>
+        <v>679</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>713</v>
+        <v>698</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>549</v>
+        <v>534</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>617</v>
+        <v>602</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>595</v>
+        <v>580</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4634,19 +4888,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>783</v>
+        <v>765</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>785</v>
+        <v>767</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4654,31 +4908,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>681</v>
+        <v>666</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>537</v>
+        <v>522</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>733</v>
+        <v>716</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4689,37 +4943,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>695</v>
+        <v>680</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>714</v>
+        <v>699</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>552</v>
+        <v>537</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>618</v>
+        <v>603</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>597</v>
+        <v>582</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -4727,19 +4981,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>608</v>
+        <v>593</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>663</v>
+        <v>648</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -4747,31 +5001,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>678</v>
+        <v>663</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>734</v>
+        <v>717</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -4782,37 +5036,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>696</v>
+        <v>681</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>715</v>
+        <v>700</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>553</v>
+        <v>538</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>620</v>
+        <v>605</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>598</v>
+        <v>583</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -4820,19 +5074,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>784</v>
+        <v>766</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>786</v>
+        <v>768</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -4840,13 +5094,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>679</v>
+        <v>664</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -4854,13 +5108,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>538</v>
+        <v>523</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>735</v>
+        <v>718</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -4871,37 +5125,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>697</v>
+        <v>682</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>716</v>
+        <v>701</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>554</v>
+        <v>539</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>575</v>
+        <v>560</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>596</v>
+        <v>581</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -4911,7 +5165,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>610</v>
+        <v>595</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -4919,13 +5173,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>682</v>
+        <v>667</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -4933,13 +5187,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>540</v>
+        <v>525</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>736</v>
+        <v>719</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -4950,37 +5204,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>699</v>
+        <v>684</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>710</v>
+        <v>695</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>555</v>
+        <v>540</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>576</v>
+        <v>561</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>623</v>
+        <v>608</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>599</v>
+        <v>584</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -4999,16 +5253,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>779</v>
+        <v>761</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>780</v>
+        <v>762</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>737</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5019,31 +5273,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>698</v>
+        <v>683</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>717</v>
+        <v>702</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>556</v>
+        <v>541</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>577</v>
+        <v>562</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>624</v>
+        <v>609</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5068,7 +5322,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>738</v>
+        <v>721</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5083,19 +5337,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>558</v>
+        <v>543</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>579</v>
+        <v>564</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>625</v>
+        <v>610</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5119,7 +5373,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>739</v>
+        <v>722</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5134,19 +5388,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>559</v>
+        <v>544</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>580</v>
+        <v>565</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>619</v>
+        <v>604</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5170,7 +5424,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>740</v>
+        <v>723</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5185,19 +5439,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>560</v>
+        <v>545</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>581</v>
+        <v>566</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5218,10 +5472,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>718</v>
+        <v>703</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>722</v>
+        <v>706</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5236,19 +5490,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>561</v>
+        <v>546</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>582</v>
+        <v>567</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>626</v>
+        <v>611</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5269,10 +5523,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>719</v>
+        <v>704</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>723</v>
+        <v>707</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5287,19 +5541,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>562</v>
+        <v>547</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>583</v>
+        <v>568</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5320,10 +5574,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>720</v>
+        <v>774</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>724</v>
+        <v>775</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5338,13 +5592,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>563</v>
+        <v>548</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5367,10 +5621,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>725</v>
+        <v>708</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5385,13 +5639,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>585</v>
+        <v>570</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5414,10 +5668,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>743</v>
+        <v>726</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>744</v>
+        <v>727</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5434,7 +5688,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>586</v>
+        <v>571</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5471,7 +5725,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>741</v>
+        <v>724</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5508,7 +5762,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>587</v>
+        <v>572</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5545,7 +5799,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>584</v>
+        <v>569</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5582,7 +5836,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>742</v>
+        <v>725</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5677,8 +5931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5713,10 +5967,10 @@
         <v>345</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>748</v>
+        <v>731</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>773</v>
+        <v>755</v>
       </c>
       <c r="E2" t="s">
         <v>346</v>
@@ -5734,7 +5988,7 @@
         <v>350</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>774</v>
+        <v>756</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5745,10 +5999,10 @@
         <v>351</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>749</v>
+        <v>732</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>773</v>
+        <v>755</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5759,10 +6013,10 @@
         <v>352</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>773</v>
+        <v>755</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5773,39 +6027,36 @@
         <v>353</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>745</v>
-      </c>
-      <c r="D5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>728</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>746</v>
-      </c>
-      <c r="D6" t="s">
-        <v>772</v>
-      </c>
-      <c r="E6" t="s">
-        <v>356</v>
-      </c>
-      <c r="F6" t="s">
-        <v>357</v>
-      </c>
-      <c r="G6" t="s">
-        <v>358</v>
-      </c>
-      <c r="H6" t="s">
-        <v>360</v>
-      </c>
-      <c r="I6" t="s">
-        <v>359</v>
+        <v>729</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>782</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>776</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>777</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>778</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>779</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5813,22 +6064,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>747</v>
-      </c>
-      <c r="D7" t="s">
-        <v>362</v>
+        <v>730</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>796</v>
       </c>
       <c r="E7" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="F7" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="G7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5836,13 +6087,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>751</v>
+        <v>734</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>785</v>
       </c>
       <c r="E8" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5850,13 +6104,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>752</v>
+        <v>735</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>793</v>
       </c>
       <c r="E9" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5864,19 +6121,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>753</v>
+        <v>736</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>794</v>
       </c>
       <c r="E10" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="F10" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="G10" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5884,13 +6144,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>754</v>
+        <v>737</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>795</v>
       </c>
       <c r="E11" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5898,13 +6161,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>755</v>
-      </c>
-      <c r="D12" t="s">
-        <v>377</v>
+        <v>738</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5912,10 +6175,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>756</v>
+        <v>739</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>783</v>
       </c>
       <c r="E13" t="s">
         <v>134</v>
@@ -5933,10 +6199,10 @@
         <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="K13" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5944,13 +6210,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>757</v>
+        <v>740</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>781</v>
       </c>
       <c r="E14" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5958,13 +6227,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>758</v>
+        <v>741</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>797</v>
       </c>
       <c r="E15" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5972,17 +6244,17 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="3" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G17" t="s">
         <v>344</v>
@@ -5993,16 +6265,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>778</v>
+        <v>760</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -6011,22 +6283,22 @@
         <v>2</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>776</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>392</v>
+        <v>758</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>786</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="G19" t="s">
-        <v>777</v>
+        <v>759</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6034,22 +6306,22 @@
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>762</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>396</v>
+        <v>745</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>787</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="G20" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6057,22 +6329,22 @@
         <v>4</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>763</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>401</v>
+        <v>746</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>788</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="G21" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="98" x14ac:dyDescent="0.3">
@@ -6080,20 +6352,20 @@
         <v>5</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>775</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>405</v>
+        <v>757</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>789</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="8" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.3">
@@ -6101,13 +6373,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -6117,20 +6389,20 @@
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>765</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>410</v>
+        <v>748</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>790</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="8" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.3">
@@ -6138,22 +6410,22 @@
         <v>8</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>766</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>414</v>
+        <v>749</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>791</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6161,18 +6433,18 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>767</v>
-      </c>
-      <c r="D26" s="6"/>
+        <v>750</v>
+      </c>
+      <c r="D26" s="19"/>
       <c r="E26" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="8" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
@@ -6180,20 +6452,20 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>768</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>421</v>
+        <v>751</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>792</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6201,20 +6473,20 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>769</v>
+        <v>752</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="168" x14ac:dyDescent="0.3">
@@ -6222,22 +6494,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>770</v>
+        <v>753</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6245,19 +6517,19 @@
         <v>13</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>771</v>
+        <v>754</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F30" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6265,16 +6537,16 @@
         <v>14</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>760</v>
+        <v>743</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6282,16 +6554,16 @@
         <v>15</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>761</v>
+        <v>744</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -6316,7 +6588,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6324,7 +6596,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20201007 20.48 for gui
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A223CAB-1983-47B4-9FE0-CABD9F2A70C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CA0EB4-D70E-475A-B5F8-210F306DBD79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="804">
   <si>
     <t>矿石</t>
   </si>
@@ -1244,12 +1244,6 @@
   </si>
   <si>
     <t>苹果+水→苹果汁；烈焰粉+苹果汁→苹果糖；金锭+苹果汁→金苹果汁；紫颂花+金苹果汁→金苹果糖；腐化蜘蛛眼+苹果汁→乙烯；烈焰粉+乙烯→聚乙烯片</t>
-  </si>
-  <si>
-    <t>高炉</t>
-  </si>
-  <si>
-    <t>能够烧制铁、铜、锡、青铜（高级窑，但是只产出锭）</t>
   </si>
   <si>
     <t>电力高炉</t>
@@ -2776,6 +2770,51 @@
   </si>
   <si>
     <t>最大电容40000fe，每tick发电16fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>土高炉</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>铁矿石/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>粉碎铁矿石/铁精矿烧制成海绵状铁，在砧上敲打成铁锭，铁锭在土高炉中烧制成灼热的铁锭，灼热的铁锭会伤害玩家，合成灼热的钢锭（未完工）在砧上敲打成钢锭。</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>海绵状铁</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>灼热的铁锭</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>灼热的钢锭（未完工）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>sponge_iron</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot_iron_ingot</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot_steel_ingot</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2875,7 +2914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2925,6 +2964,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3202,7 +3249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O11" sqref="O11"/>
     </sheetView>
@@ -3264,49 +3311,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3320,49 +3367,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3376,49 +3423,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3432,49 +3479,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3488,43 +3535,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3538,37 +3585,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3582,37 +3629,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3626,37 +3673,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="L9" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="M9" s="12" t="s">
         <v>505</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>507</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3670,25 +3717,25 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3702,25 +3749,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3734,25 +3781,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3766,19 +3813,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3792,19 +3839,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3818,19 +3865,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3844,19 +3891,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3870,19 +3917,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3893,22 +3940,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3922,13 +3969,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3942,10 +3989,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3956,7 +4003,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -3997,9 +4044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK19" sqref="AK19"/>
+      <selection pane="topRight" activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4105,109 +4152,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4218,109 +4265,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4331,109 +4378,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4444,109 +4491,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4557,103 +4604,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4664,37 +4711,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4702,19 +4749,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4722,31 +4769,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4757,37 +4804,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4795,19 +4842,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4815,31 +4862,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4850,37 +4897,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4888,19 +4935,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="T9" s="14" t="s">
+        <v>763</v>
+      </c>
+      <c r="U9" s="12" t="s">
         <v>765</v>
-      </c>
-      <c r="U9" s="12" t="s">
-        <v>767</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4908,31 +4955,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4943,37 +4990,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -4981,19 +5028,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -5001,31 +5048,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5036,37 +5083,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -5074,19 +5121,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="T11" s="14" t="s">
+        <v>764</v>
+      </c>
+      <c r="U11" s="13" t="s">
         <v>766</v>
-      </c>
-      <c r="U11" s="13" t="s">
-        <v>768</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -5094,13 +5141,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -5108,13 +5155,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5125,37 +5172,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -5165,7 +5212,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -5173,13 +5220,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -5187,13 +5234,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5204,37 +5251,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -5253,16 +5300,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5273,31 +5320,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5322,7 +5369,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5337,19 +5384,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5373,7 +5420,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5388,19 +5435,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5424,7 +5471,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5439,19 +5486,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5472,10 +5519,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5490,19 +5537,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5523,10 +5570,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5541,19 +5588,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5574,10 +5621,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5592,13 +5639,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5621,10 +5668,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5639,13 +5686,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5668,10 +5715,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5688,7 +5735,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5710,6 +5757,12 @@
       <c r="AA22" s="9"/>
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
+      <c r="AJ22" s="22" t="s">
+        <v>798</v>
+      </c>
+      <c r="AK22" s="23" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -5725,7 +5778,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5747,6 +5800,12 @@
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
+      <c r="AJ23" s="22" t="s">
+        <v>799</v>
+      </c>
+      <c r="AK23" s="23" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -5762,7 +5821,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5784,6 +5843,12 @@
       <c r="AA24" s="9"/>
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
+      <c r="AJ24" s="24" t="s">
+        <v>800</v>
+      </c>
+      <c r="AK24" s="23" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -5799,7 +5864,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5836,7 +5901,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5931,8 +5996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5967,10 +6032,10 @@
         <v>345</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E2" t="s">
         <v>346</v>
@@ -5988,7 +6053,7 @@
         <v>350</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -5999,10 +6064,10 @@
         <v>351</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6013,10 +6078,10 @@
         <v>352</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6027,10 +6092,10 @@
         <v>353</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6041,22 +6106,22 @@
         <v>354</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>774</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>775</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>776</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>777</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>778</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6067,10 +6132,10 @@
         <v>355</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="E7" t="s">
         <v>356</v>
@@ -6090,10 +6155,10 @@
         <v>359</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="E8" t="s">
         <v>360</v>
@@ -6107,10 +6172,10 @@
         <v>361</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E9" t="s">
         <v>362</v>
@@ -6124,10 +6189,10 @@
         <v>363</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E10" t="s">
         <v>364</v>
@@ -6147,10 +6212,10 @@
         <v>367</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E11" t="s">
         <v>368</v>
@@ -6164,10 +6229,10 @@
         <v>369</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6178,10 +6243,10 @@
         <v>370</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E13" t="s">
         <v>134</v>
@@ -6209,14 +6274,14 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="17" t="s">
         <v>373</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E14" t="s">
         <v>374</v>
@@ -6226,14 +6291,14 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="17" t="s">
         <v>375</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E15" t="s">
         <v>376</v>
@@ -6268,10 +6333,10 @@
         <v>381</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>382</v>
@@ -6286,10 +6351,10 @@
         <v>383</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>384</v>
@@ -6298,7 +6363,7 @@
         <v>385</v>
       </c>
       <c r="G19" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6309,10 +6374,10 @@
         <v>386</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>387</v>
@@ -6332,10 +6397,10 @@
         <v>390</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>387</v>
@@ -6355,10 +6420,10 @@
         <v>393</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>387</v>
@@ -6368,18 +6433,18 @@
         <v>394</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>6</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>395</v>
+      <c r="B23" s="21" t="s">
+        <v>796</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>747</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>396</v>
+        <v>745</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="2"/>
@@ -6389,20 +6454,20 @@
         <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="8" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.3">
@@ -6410,22 +6475,22 @@
         <v>8</v>
       </c>
       <c r="B25" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>747</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>789</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>749</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>791</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="G25" s="8" t="s">
         <v>401</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6433,10 +6498,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="6" t="s">
@@ -6444,7 +6509,7 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="8" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
@@ -6452,20 +6517,20 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>384</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6473,20 +6538,20 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>384</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="168" x14ac:dyDescent="0.3">
@@ -6494,22 +6559,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>384</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6517,19 +6582,19 @@
         <v>13</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>384</v>
       </c>
       <c r="F30" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6537,16 +6602,16 @@
         <v>14</v>
       </c>
       <c r="B31" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>741</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>418</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>743</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6554,16 +6619,16 @@
         <v>15</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>421</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>744</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -6588,7 +6653,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6596,7 +6661,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20201008 12.02 for new items
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CA0EB4-D70E-475A-B5F8-210F306DBD79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A40B7E2-5EC6-4472-9335-8B4B5A7E81C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4046,7 +4046,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF13" sqref="AF13"/>
+      <selection pane="topRight" activeCell="AK23" sqref="AK23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
20201115 10.25 for lang and new laser.png/plasma_generator.png/logo
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A40B7E2-5EC6-4472-9335-8B4B5A7E81C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427F9671-B453-414F-BF34-0DF08C19B828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="805">
   <si>
     <t>矿石</t>
   </si>
@@ -2816,6 +2816,10 @@
   <si>
     <t>hot_steel_ingot</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>风箱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2914,7 +2918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2967,11 +2971,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3250,8 +3250,8 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O11" sqref="O11"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3731,6 +3731,10 @@
       <c r="G10" s="12" t="s">
         <v>476</v>
       </c>
+      <c r="N10" s="17" t="s">
+        <v>804</v>
+      </c>
+      <c r="O10" s="17"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
@@ -4044,9 +4048,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK23" sqref="AK23"/>
+      <selection pane="topRight" activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5757,10 +5761,10 @@
       <c r="AA22" s="9"/>
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
-      <c r="AJ22" s="22" t="s">
+      <c r="AJ22" s="14" t="s">
         <v>798</v>
       </c>
-      <c r="AK22" s="23" t="s">
+      <c r="AK22" s="13" t="s">
         <v>801</v>
       </c>
     </row>
@@ -5800,10 +5804,10 @@
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
-      <c r="AJ23" s="22" t="s">
+      <c r="AJ23" s="14" t="s">
         <v>799</v>
       </c>
-      <c r="AK23" s="23" t="s">
+      <c r="AK23" s="13" t="s">
         <v>802</v>
       </c>
     </row>
@@ -5843,10 +5847,10 @@
       <c r="AA24" s="9"/>
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
-      <c r="AJ24" s="24" t="s">
+      <c r="AJ24" s="22" t="s">
         <v>800</v>
       </c>
-      <c r="AK24" s="23" t="s">
+      <c r="AK24" s="13" t="s">
         <v>803</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021.2.13 21.50 for etcher
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\参考\资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427F9671-B453-414F-BF34-0DF08C19B828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2897DF7F-64D8-42B6-BB65-4A795A2D6D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -2393,7 +2393,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>键3次，产出成品，空手右键取下</t>
@@ -2528,7 +2527,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>个模板，可以熔炼青铜合金【锭160mb、杆80mb、</t>
@@ -2549,7 +2547,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>mb、</t>
@@ -2570,7 +2567,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>】</t>
@@ -2607,7 +2603,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>fe</t>
@@ -2623,7 +2618,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>，每</t>
@@ -2644,7 +2638,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>消耗</t>
@@ -2671,7 +2664,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>0000fe，每tick消耗</t>
@@ -2714,7 +2706,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -2746,7 +2737,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>0000fe，每tick消耗</t>
@@ -2826,7 +2816,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2839,20 +2829,17 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2890,6 +2877,12 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4048,7 +4041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AK12" sqref="AK12"/>
     </sheetView>
@@ -6000,8 +5993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6155,7 +6148,7 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="17" t="s">
         <v>359</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -6172,7 +6165,7 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="17" t="s">
         <v>361</v>
       </c>
       <c r="C9" s="12" t="s">

</xml_diff>

<commit_message>
2021.3.8 21.55 for etcher
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2897DF7F-64D8-42B6-BB65-4A795A2D6D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A126A70-848A-4CCC-A502-CD71B7169728}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="806">
   <si>
     <t>矿石</t>
   </si>
@@ -1207,24 +1207,15 @@
     <t>火电厂</t>
   </si>
   <si>
-    <t>电量指示、温度指示、水量指示、启动拉杆、运行警示灯</t>
-  </si>
-  <si>
     <t>锻压机</t>
   </si>
   <si>
-    <t>电量指示、启动拉杆、运行警示灯</t>
-  </si>
-  <si>
     <t>锤头</t>
   </si>
   <si>
     <t>浇注机</t>
   </si>
   <si>
-    <t>电量指示、启动拉杆、运行警示灯、清空拉杆</t>
-  </si>
-  <si>
     <t>浇筑流体块，模具液面</t>
   </si>
   <si>
@@ -1249,16 +1240,10 @@
     <t>电力高炉</t>
   </si>
   <si>
-    <t>电量指示、启动拉杆、运行警示灯、温度指示</t>
-  </si>
-  <si>
     <t>合金配方：铁锭+碳粉→144mb钢；2铁锭+1镍锭→432mb殷钢；3铜锭+1锡锭→576mb青铜；2钢锭+1不锈钢添加剂→432mb不锈钢</t>
   </si>
   <si>
     <t>破碎机</t>
-  </si>
-  <si>
-    <t>电量指示、启动拉杆、运行警示灯、转速表</t>
   </si>
   <si>
     <t>破碎用转轴</t>
@@ -2574,23 +2559,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>每tick发电</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4fe</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>车削加工，选择加工项目：齿轮、杆、辊、螺丝，根据加工项目收取材料）钻削-5，车削-10，铣削-7，磨削-2，刨削-4，镗孔-3，车床最大电容量40000fe，每次加工消耗6400fe</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2611,7 +2579,191 @@
   </si>
   <si>
     <r>
-      <t>可以抽取正下方的液体，若泵正下方为2*2的水源方块，不抽取世界水，直接生成水（最大电容量3200fe</t>
+      <t>最大电容量32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000fe，每tick消耗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4096fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有工作时间相同（便于动画效果实现）正在运行的配方将会把物品渲染在操作台上，然后锤头压下去完成工作</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>浇筑开启后，钢包倾斜，流体块渲染，模具液面提升；随后钢包回归位置，浇筑完成后模具液面消失</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢包液面根据容量确定高度，开始工作后，金属条抽出，移动到轧钢滚轮处，生成一块块金属板</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>四个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>温度提升速度和耗电速度根据线圈材料决定，最高温度根据机械方块决定，高炉温度-产物流体温度≥0时，配方开启运行，运行时间为额定热量/升温速度，运行期间高炉温度不增加，停止运行时，温度每tick-10度（即检测到可运行配方时开启升温）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高转速根据机械方块等级不同，配方实际工作时间=设计工作时间/(10/转速)，转速每10tick+20，不工作时每tick-20；工作时，转轴每秒转一圈</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据投入的籽晶不同，产物不同</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大电容量120000fe，每tick消耗1024fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大电容量40000fe，每tick消耗128fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>最大电容量8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000fe，每tick消耗</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>256fe</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>切断整材，最大电容量40000fe，每tick消耗128fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>土高炉</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>铁矿石/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>粉碎铁矿石/铁精矿烧制成海绵状铁，在砧上敲打成铁锭，铁锭在土高炉中烧制成灼热的铁锭，灼热的铁锭会伤害玩家，合成灼热的钢锭（未完工）在砧上敲打成钢锭。</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>海绵状铁</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>灼热的铁锭</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>灼热的钢锭（未完工）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>sponge_iron</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot_iron_ingot</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot_steel_ingot</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>风箱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>电量指示、运行警示灯</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电量指示、运行警示灯、清空拉杆</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电量指示、温度指示、水量指示、运行警示灯</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电量指示、运行警示灯、温度指示</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电量指示、运行警示灯、转速表</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完工的为红字，完成模型的为黄底，尚未启动制作的是白色</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大电容40000fe，每tick发电200fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>每tick发电16fe</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>可以抽取下方的液体，若泵的检测方块为水源方块，每tick抽取20mb不消耗流体方块；若检测方块为流动水，则每tick抽取10mb，不消耗流体方块；若检测方块为岩浆或流动岩浆，每tick抽取2mb，不消耗流体方块；若检测到其他种类流体源，会立即抽空该流体方块，产出1000mb对应流体；水泵自带2000mb容量（最大电容量3200fe</t>
     </r>
     <r>
       <rPr>
@@ -2640,7 +2792,7 @@
         <rFont val="等线"/>
         <scheme val="minor"/>
       </rPr>
-      <t>消耗</t>
+      <t>消耗50</t>
     </r>
     <r>
       <rPr>
@@ -2651,172 +2803,16 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>10fe</t>
+      <t>fe</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>最大电容量32</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0000fe，每tick消耗</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4096fe</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有工作时间相同（便于动画效果实现）正在运行的配方将会把物品渲染在操作台上，然后锤头压下去完成工作</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>浇筑开启后，钢包倾斜，流体块渲染，模具液面提升；随后钢包回归位置，浇筑完成后模具液面消失</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>钢包液面根据容量确定高度，开始工作后，金属条抽出，移动到轧钢滚轮处，生成一块块金属板</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>四个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>温度提升速度和耗电速度根据线圈材料决定，最高温度根据机械方块决定，高炉温度-产物流体温度≥0时，配方开启运行，运行时间为额定热量/升温速度，运行期间高炉温度不增加，停止运行时，温度每tick-10度（即检测到可运行配方时开启升温）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>最高转速根据机械方块等级不同，配方实际工作时间=设计工作时间/(10/转速)，转速每10tick+20，不工作时每tick-20；工作时，转轴每秒转一圈</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据投入的籽晶不同，产物不同</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大电容量120000fe，每tick消耗1024fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大电容量40000fe，每tick消耗128fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>最大电容量8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0000fe，每tick消耗</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>256fe</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>切断整材，最大电容量40000fe，每tick消耗128fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大电容40000fe，每tick发电16fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>土高炉</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>铁矿石/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>粉碎铁矿石/铁精矿烧制成海绵状铁，在砧上敲打成铁锭，铁锭在土高炉中烧制成灼热的铁锭，灼热的铁锭会伤害玩家，合成灼热的钢锭（未完工）在砧上敲打成钢锭。</t>
-    </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>海绵状铁</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>灼热的铁锭</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>灼热的钢锭（未完工）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>sponge_iron</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>hot_iron_ingot</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>hot_steel_ingot</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>风箱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2884,6 +2880,15 @@
       <name val="等线"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2911,7 +2916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2965,6 +2970,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3304,49 +3315,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3360,49 +3371,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3416,49 +3427,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3472,49 +3483,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3528,43 +3539,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3578,37 +3589,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3622,37 +3633,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3666,37 +3677,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3710,29 +3721,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3746,25 +3757,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3778,25 +3789,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3810,19 +3821,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3836,19 +3847,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3862,19 +3873,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3888,19 +3899,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3914,19 +3925,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3937,22 +3948,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3966,13 +3977,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3986,10 +3997,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4000,7 +4011,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4149,109 +4160,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4262,109 +4273,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4375,109 +4386,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4488,109 +4499,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4601,103 +4612,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4708,37 +4719,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4746,19 +4757,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4766,31 +4777,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4801,37 +4812,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4839,19 +4850,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4859,31 +4870,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4894,37 +4905,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4932,19 +4943,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4952,31 +4963,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4987,37 +4998,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -5025,19 +5036,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -5045,31 +5056,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5080,37 +5091,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -5118,19 +5129,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -5138,13 +5149,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -5152,13 +5163,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5169,37 +5180,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -5209,7 +5220,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -5217,13 +5228,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -5231,13 +5242,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5248,37 +5259,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -5297,16 +5308,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5317,31 +5328,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5366,7 +5377,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5381,19 +5392,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5417,7 +5428,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5432,19 +5443,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5468,7 +5479,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5483,19 +5494,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5516,10 +5527,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5534,19 +5545,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5567,10 +5578,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5585,19 +5596,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5618,10 +5629,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5636,13 +5647,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5665,10 +5676,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5683,13 +5694,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5712,10 +5723,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5732,7 +5743,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5755,10 +5766,10 @@
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
       <c r="AJ22" s="14" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="AK22" s="13" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5775,7 +5786,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5798,10 +5809,10 @@
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AJ23" s="14" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="AK23" s="13" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -5818,7 +5829,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5841,10 +5852,10 @@
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
       <c r="AJ24" s="22" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="AK24" s="13" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.3">
@@ -5861,7 +5872,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5898,7 +5909,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -5991,16 +6002,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" customWidth="1"/>
+    <col min="2" max="2" width="17.08203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.08203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
@@ -6009,623 +6020,628 @@
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>344</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>753</v>
-      </c>
-      <c r="E2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F2" t="s">
-        <v>347</v>
-      </c>
-      <c r="G2" t="s">
-        <v>348</v>
-      </c>
-      <c r="H2" t="s">
-        <v>349</v>
-      </c>
-      <c r="I2" t="s">
-        <v>350</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>351</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>345</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>753</v>
+        <v>748</v>
+      </c>
+      <c r="E3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H3" t="s">
+        <v>349</v>
+      </c>
+      <c r="I3" t="s">
+        <v>350</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>352</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>351</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>353</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>352</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>726</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>721</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B7" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>727</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>780</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="C7" s="12" t="s">
+        <v>722</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>774</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>775</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>776</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>355</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>728</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>794</v>
-      </c>
-      <c r="E7" t="s">
-        <v>356</v>
-      </c>
-      <c r="F7" t="s">
-        <v>357</v>
-      </c>
-      <c r="G7" t="s">
-        <v>358</v>
+      <c r="E7" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>770</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>771</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>359</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>355</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="E8" t="s">
-        <v>360</v>
+        <v>356</v>
+      </c>
+      <c r="F8" t="s">
+        <v>357</v>
+      </c>
+      <c r="G8" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>361</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>359</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>791</v>
+        <v>776</v>
       </c>
       <c r="E9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>363</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>361</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="E10" t="s">
-        <v>364</v>
-      </c>
-      <c r="F10" t="s">
-        <v>365</v>
-      </c>
-      <c r="G10" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>367</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="E11" t="s">
-        <v>368</v>
+        <v>364</v>
+      </c>
+      <c r="F11" t="s">
+        <v>365</v>
+      </c>
+      <c r="G11" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>730</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>786</v>
+      </c>
+      <c r="E12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="70" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>736</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>370</v>
-      </c>
       <c r="C13" s="12" t="s">
-        <v>737</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>781</v>
-      </c>
-      <c r="E13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" t="s">
-        <v>224</v>
-      </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" t="s">
-        <v>371</v>
-      </c>
-      <c r="K13" t="s">
-        <v>372</v>
+        <v>731</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>373</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>370</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="E14" t="s">
-        <v>374</v>
+        <v>134</v>
+      </c>
+      <c r="F14" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>371</v>
+      </c>
+      <c r="K14" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>733</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>804</v>
+      </c>
+      <c r="E15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B16" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>739</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>795</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C16" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>803</v>
+      </c>
+      <c r="E16" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="12"/>
-    </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="3" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="138" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="19" spans="1:7" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>740</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>383</v>
-      </c>
       <c r="C19" s="12" t="s">
-        <v>756</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>784</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="G19" t="s">
-        <v>757</v>
-      </c>
+        <v>735</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>799</v>
+      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>3</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>386</v>
+        <v>2</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>382</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>743</v>
+        <v>751</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>785</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>387</v>
+        <v>777</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="G20" t="s">
-        <v>389</v>
+        <v>752</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>738</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>778</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>798</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="G21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B22" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>739</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>779</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>798</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="G22" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="98" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>744</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>786</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="C23" s="12" t="s">
+        <v>750</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>780</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>798</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="G21" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="42" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>6</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>788</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>789</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>7</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="98" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>5</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="C25" s="12" t="s">
+        <v>741</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>781</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>755</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>787</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="8" t="s">
+    </row>
+    <row r="26" spans="1:7" ht="196" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>8</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="42" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>6</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>796</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>745</v>
-      </c>
-      <c r="D23" s="19" t="s">
+      <c r="C26" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>782</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>801</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>743</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="s">
         <v>797</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="84" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>7</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>746</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>788</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="8" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="196" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>8</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>747</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>789</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>9</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>748</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="70" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>749</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>790</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>384</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="70" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>750</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>384</v>
+        <v>744</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>783</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>797</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>11</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>797</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>12</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>746</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>797</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>13</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="168" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>12</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="C31" s="12" t="s">
+        <v>747</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>751</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E31" s="19" t="s">
+        <v>797</v>
+      </c>
+      <c r="F31" t="s">
         <v>410</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="F29" s="2" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>14</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>411</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="C32" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>13</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>752</v>
-      </c>
-      <c r="D30" s="6" t="s">
+    </row>
+    <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>15</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="C33" s="12" t="s">
+        <v>737</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>14</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="E33" s="4" t="s">
         <v>416</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>741</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="28" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>15</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>419</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>742</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -6650,7 +6666,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6658,7 +6674,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.3.21 20.00 for models
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A126A70-848A-4CCC-A502-CD71B7169728}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95963450-6C98-4E0D-B9D7-FE5C2FC9DFA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1126,9 +1126,6 @@
     <t>车床</t>
   </si>
   <si>
-    <t>切割机</t>
-  </si>
-  <si>
     <t>块→8板</t>
   </si>
   <si>
@@ -1148,9 +1145,6 @@
   </si>
   <si>
     <t>提炼渣→金属粉</t>
-  </si>
-  <si>
-    <t>离心机</t>
   </si>
   <si>
     <t>炉渣→随机金属粉</t>
@@ -2805,6 +2799,14 @@
       </rPr>
       <t>fe</t>
     </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>离心机</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>切割机</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2916,7 +2918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2975,6 +2977,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3315,49 +3320,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3371,49 +3376,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3427,49 +3432,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3483,49 +3488,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3539,43 +3544,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3589,37 +3594,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3633,37 +3638,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3677,37 +3682,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L9" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="M9" s="12" t="s">
         <v>498</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>500</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3721,29 +3726,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="O10" s="17"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3757,25 +3762,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3789,25 +3794,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3821,19 +3826,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3847,19 +3852,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3873,19 +3878,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3899,19 +3904,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3925,19 +3930,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3948,22 +3953,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3977,13 +3982,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -3997,10 +4002,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4011,7 +4016,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4160,109 +4165,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4273,109 +4278,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4386,109 +4391,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4499,109 +4504,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4612,103 +4617,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4719,37 +4724,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4757,19 +4762,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4777,31 +4782,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4812,37 +4817,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4850,19 +4855,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4870,31 +4875,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4905,37 +4910,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4943,19 +4948,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="T9" s="14" t="s">
+        <v>756</v>
+      </c>
+      <c r="U9" s="12" t="s">
         <v>758</v>
-      </c>
-      <c r="U9" s="12" t="s">
-        <v>760</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4963,31 +4968,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -4998,37 +5003,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -5036,19 +5041,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -5056,31 +5061,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5091,37 +5096,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -5129,19 +5134,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="T11" s="14" t="s">
+        <v>757</v>
+      </c>
+      <c r="U11" s="13" t="s">
         <v>759</v>
-      </c>
-      <c r="U11" s="13" t="s">
-        <v>761</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -5149,13 +5154,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -5163,13 +5168,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5180,37 +5185,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -5220,7 +5225,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -5228,13 +5233,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -5242,13 +5247,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5259,37 +5264,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -5308,16 +5313,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5328,31 +5333,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5377,7 +5382,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5392,19 +5397,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5428,7 +5433,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5443,19 +5448,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5479,7 +5484,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5494,19 +5499,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5527,10 +5532,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5545,19 +5550,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5578,10 +5583,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5596,19 +5601,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5629,10 +5634,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5647,13 +5652,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5676,10 +5681,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5694,13 +5699,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5723,10 +5728,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5743,7 +5748,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5766,10 +5771,10 @@
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
       <c r="AJ22" s="14" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="AK22" s="13" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5786,7 +5791,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5809,10 +5814,10 @@
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AJ23" s="14" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="AK23" s="13" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -5829,7 +5834,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5852,10 +5857,10 @@
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
       <c r="AJ24" s="22" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="AK24" s="13" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.3">
@@ -5872,7 +5877,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5909,7 +5914,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -6005,7 +6010,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6022,7 +6027,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6045,10 +6050,10 @@
         <v>345</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6066,7 +6071,7 @@
         <v>350</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6077,10 +6082,10 @@
         <v>351</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6091,10 +6096,10 @@
         <v>352</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6105,10 +6110,10 @@
         <v>353</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6119,45 +6124,45 @@
         <v>354</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>767</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>768</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>769</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>770</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>771</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="23" t="s">
+        <v>805</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>721</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>785</v>
+      </c>
+      <c r="E8" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>723</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>787</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>356</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>357</v>
-      </c>
-      <c r="G8" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6165,87 +6170,87 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>725</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>774</v>
+      </c>
+      <c r="E9" t="s">
         <v>359</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>727</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>776</v>
-      </c>
-      <c r="E9" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>726</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>782</v>
+      </c>
+      <c r="E10" t="s">
         <v>361</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>728</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>784</v>
-      </c>
-      <c r="E10" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="25" t="s">
+        <v>804</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>727</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>783</v>
+      </c>
+      <c r="E11" t="s">
+        <v>362</v>
+      </c>
+      <c r="F11" t="s">
         <v>363</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>785</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>364</v>
-      </c>
-      <c r="F11" t="s">
-        <v>365</v>
-      </c>
-      <c r="G11" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>367</v>
+      <c r="B12" s="16" t="s">
+        <v>365</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="E12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>369</v>
+      <c r="B13" s="23" t="s">
+        <v>367</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6253,13 +6258,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6277,10 +6282,10 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6288,16 +6293,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E15" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6305,16 +6310,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E16" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6322,17 +6327,17 @@
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>378</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="G18" t="s">
         <v>344</v>
@@ -6343,16 +6348,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -6361,22 +6366,22 @@
         <v>2</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G20" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6384,22 +6389,22 @@
         <v>3</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>776</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="G21" t="s">
         <v>384</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>738</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>778</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>798</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="G21" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6407,22 +6412,22 @@
         <v>4</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>737</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>777</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="G22" t="s">
         <v>387</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>739</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>779</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>798</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="G22" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="98" x14ac:dyDescent="0.3">
@@ -6430,20 +6435,20 @@
         <v>5</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="42" x14ac:dyDescent="0.3">
@@ -6451,13 +6456,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
@@ -6467,20 +6472,20 @@
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="196" x14ac:dyDescent="0.3">
@@ -6488,22 +6493,22 @@
         <v>8</v>
       </c>
       <c r="B26" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>780</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>799</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>394</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>742</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>782</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>801</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6511,18 +6516,18 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="70" x14ac:dyDescent="0.3">
@@ -6530,20 +6535,20 @@
         <v>10</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28" x14ac:dyDescent="0.3">
@@ -6551,20 +6556,20 @@
         <v>11</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="8" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="168" x14ac:dyDescent="0.3">
@@ -6572,22 +6577,22 @@
         <v>12</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>744</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>795</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>746</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="G30" s="8" t="s">
         <v>405</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>797</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -6595,19 +6600,19 @@
         <v>13</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>795</v>
+      </c>
+      <c r="F31" t="s">
         <v>408</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>747</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>797</v>
-      </c>
-      <c r="F31" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6615,16 +6620,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>734</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>736</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6632,16 +6637,16 @@
         <v>15</v>
       </c>
       <c r="B33" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>735</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>414</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>737</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -6666,7 +6671,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6674,7 +6679,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.3.25 22.00 for many things
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95963450-6C98-4E0D-B9D7-FE5C2FC9DFA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE9161-B644-4188-B04C-D2C87FCD09CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="990" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="809">
   <si>
     <t>矿石</t>
   </si>
@@ -1201,24 +1201,15 @@
     <t>火电厂</t>
   </si>
   <si>
-    <t>锻压机</t>
-  </si>
-  <si>
     <t>锤头</t>
   </si>
   <si>
-    <t>浇注机</t>
-  </si>
-  <si>
     <t>浇筑流体块，模具液面</t>
   </si>
   <si>
     <t>块1440mb；锭160mb；圆形铸件1440mb</t>
   </si>
   <si>
-    <t>连铸轧钢厂</t>
-  </si>
-  <si>
     <t>钢包液面，金属条，轧钢滚轮，金属板</t>
   </si>
   <si>
@@ -1237,18 +1228,12 @@
     <t>合金配方：铁锭+碳粉→144mb钢；2铁锭+1镍锭→432mb殷钢；3铜锭+1锡锭→576mb青铜；2钢锭+1不锈钢添加剂→432mb不锈钢</t>
   </si>
   <si>
-    <t>破碎机</t>
-  </si>
-  <si>
     <t>破碎用转轴</t>
   </si>
   <si>
     <t>原矿→2粉碎矿石；锭→粉；齿轮→4粉；齿轮坯→4粉；圆形铸件→9粉；块→9粉；管道→3粉；机械方块→对应板材粉末；石头→圆石；圆石→砂砾；砂砾→沙子；石英→硅粉；骨头→6骨粉；红石矿石→12红石粉+石粉；青金石矿石→8青金石+石粉；石英矿石→4石英+石粉；钻石矿石→4钻石+石粉；煤矿石→4煤粉+石粉</t>
   </si>
   <si>
-    <t>电磁选矿机</t>
-  </si>
-  <si>
     <t>粉碎矿石→精矿+石粉+概率金属粉</t>
   </si>
   <si>
@@ -1261,9 +1246,6 @@
     <t>数控机床</t>
   </si>
   <si>
-    <t>两条生产线可以同时开工，生产不同的物品</t>
-  </si>
-  <si>
     <t>齿轮坯→齿轮;锭→2杆；杆→2螺丝；轴→辊</t>
   </si>
   <si>
@@ -1288,16 +1270,7 @@
     <t>液面</t>
   </si>
   <si>
-    <t>球型储罐</t>
-  </si>
-  <si>
     <t>存储256000mb同类型流体/气体</t>
-  </si>
-  <si>
-    <t>容量指示</t>
-  </si>
-  <si>
-    <t>大型飞轮储能装置</t>
   </si>
   <si>
     <t>最大存储能量依据机械方块计算，最大输出能力根据线圈计算；最小储能容量100kFE，最大储能容量100mFE</t>
@@ -2629,10 +2602,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>最高转速根据机械方块等级不同，配方实际工作时间=设计工作时间/(10/转速)，转速每10tick+20，不工作时每tick-20；工作时，转轴每秒转一圈</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>根据投入的籽晶不同，产物不同</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2725,22 +2694,6 @@
   </si>
   <si>
     <t>电量指示、运行警示灯</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>电量指示、运行警示灯、清空拉杆</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>电量指示、温度指示、水量指示、运行警示灯</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>电量指示、运行警示灯、温度指示</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>电量指示、运行警示灯、转速表</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -2809,12 +2762,80 @@
     <t>切割机</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>同时承接土高炉的任务以及熔化金属部件的任务</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>破碎机（无gui，第二产物从背后的输出口输出</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电磁选矿机（无gui，石粉从背后的输出口输出</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>球型储罐（无gui</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>大型飞轮储能装置</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>连铸轧钢厂</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>浇注机</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>锻压机</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>高效率制作零件</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>金属管</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高转速根据机械方块等级不同，配方实际工作时间=设计工作时间/(10/转速)，转速每10tick+传动模块等级*5，不工作时每tick-20；工作时，转轴每秒转一圈</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>转速表</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度指示</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>清空拉杆</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行警示灯</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度指示、水量指示</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>容量指示</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2891,8 +2912,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2905,8 +2933,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2914,11 +2948,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2955,9 +3004,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2972,14 +3018,35 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3259,8 +3326,8 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M13" sqref="M13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N5" sqref="N5:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3320,49 +3387,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3376,49 +3443,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3432,49 +3499,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3488,49 +3555,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3544,43 +3611,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3594,37 +3661,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3638,37 +3705,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3682,37 +3749,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>761</v>
+        <v>752</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3726,29 +3793,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>794</v>
-      </c>
-      <c r="O10" s="17"/>
+        <v>460</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>784</v>
+      </c>
+      <c r="O10" s="16"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3762,25 +3829,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>763</v>
+        <v>754</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3794,25 +3861,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>764</v>
+        <v>755</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3826,19 +3893,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3852,19 +3919,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3878,19 +3945,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3904,19 +3971,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3930,19 +3997,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -3953,22 +4020,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -3982,13 +4049,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -4002,10 +4069,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4016,7 +4083,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4057,7 +4124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AK12" sqref="AK12"/>
     </sheetView>
@@ -4165,109 +4232,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>676</v>
+        <v>667</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4278,109 +4345,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>701</v>
+        <v>692</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4391,109 +4458,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>683</v>
+        <v>674</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>702</v>
+        <v>693</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4504,109 +4571,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>684</v>
+        <v>675</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4617,103 +4684,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>667</v>
+        <v>658</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>685</v>
+        <v>676</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>704</v>
+        <v>695</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4724,37 +4791,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>687</v>
+        <v>678</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4762,19 +4829,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4782,31 +4849,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>705</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4817,37 +4884,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>688</v>
+        <v>679</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4855,19 +4922,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4875,31 +4942,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4910,37 +4977,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -4948,19 +5015,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>756</v>
+        <v>747</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -4968,31 +5035,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5003,37 +5070,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>690</v>
+        <v>681</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -5041,19 +5108,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -5061,31 +5128,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>708</v>
+        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5096,37 +5163,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>691</v>
+        <v>682</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -5134,19 +5201,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>757</v>
+        <v>748</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>759</v>
+        <v>750</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -5154,13 +5221,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -5168,13 +5235,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5185,37 +5252,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>692</v>
+        <v>683</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -5225,7 +5292,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -5233,13 +5300,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -5247,13 +5314,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5264,37 +5331,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -5313,16 +5380,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>752</v>
+        <v>743</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>753</v>
+        <v>744</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5333,31 +5400,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>693</v>
+        <v>684</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5382,7 +5449,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5397,19 +5464,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5433,7 +5500,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5448,19 +5515,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5484,7 +5551,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5499,19 +5566,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5532,10 +5599,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
-        <v>694</v>
+        <v>685</v>
       </c>
       <c r="AK17" s="12" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5550,19 +5617,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5583,10 +5650,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="AK18" s="12" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5601,19 +5668,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5634,10 +5701,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>766</v>
+        <v>757</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5652,13 +5719,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5681,10 +5748,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
-        <v>696</v>
+        <v>687</v>
       </c>
       <c r="AK20" s="12" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5699,13 +5766,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5728,10 +5795,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5748,7 +5815,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5771,10 +5838,10 @@
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
       <c r="AJ22" s="14" t="s">
-        <v>788</v>
+        <v>778</v>
       </c>
       <c r="AK22" s="13" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5791,7 +5858,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5814,10 +5881,10 @@
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AJ23" s="14" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
       <c r="AK23" s="13" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -5834,7 +5901,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5856,11 +5923,11 @@
       <c r="AA24" s="9"/>
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
-      <c r="AJ24" s="22" t="s">
-        <v>790</v>
+      <c r="AJ24" s="21" t="s">
+        <v>780</v>
       </c>
       <c r="AK24" s="13" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.3">
@@ -5877,7 +5944,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5914,7 +5981,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -6007,10 +6074,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6025,13 +6092,13 @@
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="21" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="20" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>342</v>
       </c>
       <c r="C2" s="3"/>
@@ -6042,18 +6109,18 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>345</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>746</v>
+        <v>737</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6071,89 +6138,89 @@
         <v>350</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>351</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>352</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>353</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>354</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>720</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>772</v>
+        <v>711</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>763</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>767</v>
+        <v>758</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>768</v>
+        <v>759</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>805</v>
+      <c r="B8" s="24" t="s">
+        <v>791</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>785</v>
+        <v>775</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6165,52 +6232,52 @@
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="25" t="s">
         <v>358</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>774</v>
+        <v>765</v>
       </c>
       <c r="E9" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="24" t="s">
         <v>360</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>726</v>
+        <v>717</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>782</v>
+        <v>772</v>
       </c>
       <c r="E10" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>804</v>
+      <c r="B11" s="26" t="s">
+        <v>790</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
       <c r="E11" t="s">
         <v>362</v>
@@ -6222,49 +6289,49 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="25" t="s">
         <v>365</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
       <c r="E12" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="24" t="s">
         <v>367</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>720</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="27" t="s">
         <v>368</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>730</v>
+        <v>721</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>773</v>
+        <v>764</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6287,46 +6354,49 @@
       <c r="K14" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="11" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>371</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="E15" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
         <v>373</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>801</v>
+        <v>787</v>
       </c>
       <c r="E16" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="12"/>
     </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
+    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="22" t="s">
         <v>375</v>
       </c>
       <c r="C18" s="12"/>
@@ -6343,310 +6413,305 @@
         <v>344</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="23" t="s">
         <v>379</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>751</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>797</v>
+        <v>742</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>807</v>
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="30" t="s">
+        <v>799</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>740</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>766</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>806</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>749</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>775</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>795</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>381</v>
-      </c>
       <c r="G20" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="28" t="s">
+        <v>798</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>727</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>767</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>806</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="G21" t="s">
         <v>382</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>736</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>776</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>796</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="G21" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>385</v>
+      <c r="B22" s="26" t="s">
+        <v>797</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>737</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>777</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>796</v>
+        <v>728</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>768</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>806</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G22" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="98" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>388</v>
+      <c r="B23" s="23" t="s">
+        <v>385</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>748</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>778</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>796</v>
+        <v>739</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>769</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>805</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="8" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="42" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>6</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>786</v>
+      <c r="B24" s="24" t="s">
+        <v>776</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>738</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>787</v>
+        <v>729</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>777</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="84" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>390</v>
+      <c r="B25" s="27" t="s">
+        <v>387</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>739</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>779</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>798</v>
+        <v>730</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>770</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>804</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="8" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="196" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>392</v>
+      <c r="B26" s="31" t="s">
+        <v>793</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>740</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>780</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>799</v>
+        <v>731</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>802</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>803</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>395</v>
+      <c r="B27" s="29" t="s">
+        <v>794</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>741</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="s">
-        <v>795</v>
-      </c>
+        <v>732</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="70" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="70" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>397</v>
+      <c r="B28" s="27" t="s">
+        <v>392</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>742</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>781</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>795</v>
-      </c>
+        <v>733</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>771</v>
+      </c>
+      <c r="E28" s="18"/>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>399</v>
+      <c r="B29" s="27" t="s">
+        <v>394</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>743</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>795</v>
-      </c>
+        <v>734</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>800</v>
+      </c>
+      <c r="E29" s="18"/>
       <c r="F29" s="2"/>
       <c r="G29" s="8" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="168" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="168" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>402</v>
+      <c r="B30" s="27" t="s">
+        <v>396</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>744</v>
+        <v>735</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>795</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="E30" s="18"/>
       <c r="F30" s="2" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>13</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>406</v>
+      <c r="B31" s="27" t="s">
+        <v>400</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>795</v>
+        <v>401</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>785</v>
       </c>
       <c r="F31" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>14</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>409</v>
+      <c r="B32" s="24" t="s">
+        <v>795</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>411</v>
+        <v>403</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>15</v>
       </c>
-      <c r="B33" s="16" t="s">
-        <v>412</v>
+      <c r="B33" s="26" t="s">
+        <v>796</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -6671,7 +6736,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6679,7 +6744,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.3.27 17.26 for 企划
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE9161-B644-4188-B04C-D2C87FCD09CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EA7418-868D-44B1-859E-D8D7878B3C35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="990" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="815">
   <si>
     <t>矿石</t>
   </si>
@@ -1204,15 +1204,9 @@
     <t>锤头</t>
   </si>
   <si>
-    <t>浇筑流体块，模具液面</t>
-  </si>
-  <si>
     <t>块1440mb；锭160mb；圆形铸件1440mb</t>
   </si>
   <si>
-    <t>钢包液面，金属条，轧钢滚轮，金属板</t>
-  </si>
-  <si>
     <t>板150mb；杆68mb；线68mb；管600mb；</t>
   </si>
   <si>
@@ -1271,9 +1265,6 @@
   </si>
   <si>
     <t>存储256000mb同类型流体/气体</t>
-  </si>
-  <si>
-    <t>最大存储能量依据机械方块计算，最大输出能力根据线圈计算；最小储能容量100kFE，最大储能容量100mFE</t>
   </si>
   <si>
     <t>转速表</t>
@@ -2575,18 +2566,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>浇筑开启后，钢包倾斜，流体块渲染，模具液面提升；随后钢包回归位置，浇筑完成后模具液面消失</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>钢包液面根据容量确定高度，开始工作后，金属条抽出，移动到轧钢滚轮处，生成一块块金属板</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>四个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>温度提升速度和耗电速度根据线圈材料决定，最高温度根据机械方块决定，高炉温度-产物流体温度≥0时，配方开启运行，运行时间为额定热量/升温速度，运行期间高炉温度不增加，停止运行时，温度每tick-10度（即检测到可运行配方时开启升温）</t>
     </r>
@@ -2763,10 +2742,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>同时承接土高炉的任务以及熔化金属部件的任务</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>破碎机（无gui，第二产物从背后的输出口输出</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2815,19 +2790,71 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>清空拉杆</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>运行警示灯</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>温度指示、水量指示</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>容量指示</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢制飞轮（用于制作便携式飞轮电池和放置在大型飞轮蓄电器内）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>碳素飞轮</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>超材料飞轮</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>便携式飞轮电池（蓄电量为单个碳素飞轮的存储量）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flying_wheel_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flying_wheel_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flying_wheel_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>flywheel_battery</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大输出能力根据线圈计算；储能容量根据内部的飞轮数量和等级决定;每片钢飞轮70k，碳素飞轮120k，超材料飞轮450k</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>同时承接熔化金属部件的任务</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>四个按钮（依次为线、杆、板、管）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>共有四个按钮，对应四种生产类型，按下会让按钮移动1/16个方块，其他按钮恢复原位，刚建造的时候默认板材</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢包、浇筑流体块</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>浇筑开启后，钢包倾斜，流体块渲染；随后流体块结束渲染，钢包回归位置</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>六个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2967,7 +2994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3037,15 +3064,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3387,49 +3427,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3443,49 +3483,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3499,49 +3539,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3555,49 +3595,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3611,43 +3651,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3661,37 +3701,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3705,37 +3745,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3749,37 +3789,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3793,29 +3833,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="O10" s="16"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3829,25 +3869,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3861,25 +3901,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3893,19 +3933,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3919,19 +3959,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -3945,19 +3985,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -3971,19 +4011,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -3997,19 +4037,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -4020,22 +4060,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -4049,13 +4089,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -4069,10 +4109,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4083,7 +4123,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4125,8 +4165,8 @@
   <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK12" sqref="AK12"/>
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4232,109 +4272,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="12" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="Z2" s="9" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="AB2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="AF2" s="9" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="AH2" s="9" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="AJ2" s="9" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4345,109 +4385,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="X3" s="9" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="Z3" s="9" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="AD3" s="9" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="12" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="AF3" s="9" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="12" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="AH3" s="9" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="AJ3" s="9" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="12" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4458,109 +4498,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="V4" s="9" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="X4" s="9" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="Z4" s="9" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="AB4" s="9" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="12" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="AD4" s="9" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="12" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="12" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="AJ4" s="9" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="12" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4571,109 +4611,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="V5" s="9" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="X5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="12" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="Z5" s="9" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="12" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="AB5" s="9" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AD5" s="9" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4684,103 +4724,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="12" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="12" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="12" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="AD6" s="9" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="12" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="AF6" s="9" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="AJ6" s="9" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4791,37 +4831,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="L7" s="9" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -4829,19 +4869,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
@@ -4849,31 +4889,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="12" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="Z7" s="9" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="12" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="12" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="AJ7" s="9" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="12" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4884,37 +4924,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -4922,19 +4962,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="12"/>
@@ -4942,31 +4982,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="12" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="Z8" s="9" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="AB8" s="9" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="12" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="AJ8" s="9" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="12" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -4977,37 +5017,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="L9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -5015,19 +5055,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="T9" s="14" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
@@ -5035,31 +5075,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="Z9" s="9" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="12" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="12" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="AF9" s="9" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="AJ9" s="9" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="12" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5070,37 +5110,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -5108,19 +5148,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
@@ -5128,31 +5168,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="12" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="Z10" s="9" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="12" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="AB10" s="9" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="12" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="AF10" s="9" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="12" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="AJ10" s="9" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="12" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5163,37 +5203,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="L11" s="9" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -5201,19 +5241,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="T11" s="14" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="U11" s="13" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
@@ -5221,13 +5261,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="12" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="Z11" s="9" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="12" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
@@ -5235,13 +5275,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="12" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="AJ11" s="9" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="12" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5252,37 +5292,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="L12" s="9" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -5292,7 +5332,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
@@ -5300,13 +5340,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="12" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="Z12" s="9" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="12" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -5314,13 +5354,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="AJ12" s="9" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="12" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5331,37 +5371,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="L13" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
@@ -5380,16 +5420,16 @@
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
       <c r="AF13" s="10" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="AG13" s="12" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="AJ13" s="9" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="12" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5400,31 +5440,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -5449,7 +5489,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="12" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5464,19 +5504,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -5500,7 +5540,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="12" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5515,19 +5555,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
@@ -5551,7 +5591,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="12" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5566,19 +5606,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -5599,10 +5639,10 @@
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
       <c r="AJ17" s="14" t="s">
+        <v>682</v>
+      </c>
+      <c r="AK17" s="12" t="s">
         <v>685</v>
-      </c>
-      <c r="AK17" s="12" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5617,19 +5657,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -5650,10 +5690,10 @@
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AJ18" s="14" t="s">
+        <v>683</v>
+      </c>
+      <c r="AK18" s="12" t="s">
         <v>686</v>
-      </c>
-      <c r="AK18" s="12" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5668,19 +5708,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -5701,10 +5741,10 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
       <c r="AJ19" s="14" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="AK19" s="12" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5719,13 +5759,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -5748,10 +5788,10 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AJ20" s="14" t="s">
+        <v>684</v>
+      </c>
+      <c r="AK20" s="12" t="s">
         <v>687</v>
-      </c>
-      <c r="AK20" s="12" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5766,13 +5806,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -5795,10 +5835,10 @@
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
       <c r="AJ21" s="14" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="AK21" s="12" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5815,7 +5855,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -5838,10 +5878,10 @@
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
       <c r="AJ22" s="14" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="AK22" s="13" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5858,7 +5898,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -5881,10 +5921,10 @@
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AJ23" s="14" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="AK23" s="13" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -5901,7 +5941,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -5924,13 +5964,13 @@
       <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
       <c r="AJ24" s="21" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="AK24" s="13" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5944,7 +5984,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -5966,6 +6006,12 @@
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
       <c r="AC25" s="9"/>
+      <c r="AJ25" s="32" t="s">
+        <v>800</v>
+      </c>
+      <c r="AK25" s="13" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -5981,7 +6027,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
@@ -6003,6 +6049,12 @@
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
+      <c r="AJ26" s="31" t="s">
+        <v>801</v>
+      </c>
+      <c r="AK26" s="13" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B27" s="9"/>
@@ -6033,8 +6085,14 @@
       <c r="AA27" s="9"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="9"/>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="31" t="s">
+        <v>802</v>
+      </c>
+      <c r="AK27" s="13" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -6063,6 +6121,12 @@
       <c r="AA28" s="9"/>
       <c r="AB28" s="9"/>
       <c r="AC28" s="9"/>
+      <c r="AJ28" s="33" t="s">
+        <v>803</v>
+      </c>
+      <c r="AK28" s="13" t="s">
+        <v>807</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -6076,8 +6140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6094,7 +6158,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="20" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6117,10 +6181,10 @@
         <v>345</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6138,7 +6202,7 @@
         <v>350</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6149,10 +6213,10 @@
         <v>351</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6163,10 +6227,10 @@
         <v>352</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6177,10 +6241,10 @@
         <v>353</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6191,22 +6255,22 @@
         <v>354</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>755</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>756</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>757</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>758</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>759</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>760</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6214,13 +6278,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6240,10 +6304,10 @@
         <v>358</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="E9" t="s">
         <v>359</v>
@@ -6257,10 +6321,10 @@
         <v>360</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="E10" t="s">
         <v>361</v>
@@ -6271,13 +6335,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="E11" t="s">
         <v>362</v>
@@ -6297,10 +6361,10 @@
         <v>365</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="E12" t="s">
         <v>366</v>
@@ -6314,10 +6378,10 @@
         <v>367</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6328,10 +6392,10 @@
         <v>368</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6355,7 +6419,7 @@
         <v>370</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6366,10 +6430,10 @@
         <v>371</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="E15" t="s">
         <v>372</v>
@@ -6383,10 +6447,10 @@
         <v>373</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="E16" t="s">
         <v>374</v>
@@ -6421,13 +6485,13 @@
         <v>379</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -6435,69 +6499,65 @@
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="30" t="s">
-        <v>799</v>
+      <c r="B20" s="29" t="s">
+        <v>792</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>766</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>806</v>
-      </c>
+        <v>763</v>
+      </c>
+      <c r="E20" s="18"/>
       <c r="F20" s="7" t="s">
         <v>380</v>
       </c>
       <c r="G20" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>798</v>
+      <c r="B21" s="26" t="s">
+        <v>791</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>767</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>806</v>
-      </c>
-      <c r="F21" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="35" t="s">
+        <v>812</v>
+      </c>
+      <c r="G21" t="s">
         <v>381</v>
-      </c>
-      <c r="G21" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>797</v>
+      <c r="B22" s="36" t="s">
+        <v>790</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>768</v>
+        <v>811</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>806</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>383</v>
+        <v>799</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>810</v>
       </c>
       <c r="G22" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
@@ -6505,20 +6565,18 @@
         <v>5</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>769</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>805</v>
-      </c>
-      <c r="F23" s="2"/>
+        <v>814</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="8" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -6526,13 +6584,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
@@ -6542,63 +6600,63 @@
         <v>7</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>792</v>
+        <v>386</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="31" t="s">
-        <v>793</v>
+      <c r="B26" s="30" t="s">
+        <v>786</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>803</v>
+        <v>796</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="29" t="s">
-        <v>794</v>
+      <c r="B27" s="28" t="s">
+        <v>787</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
       <c r="F27" s="2"/>
       <c r="G27" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="70" x14ac:dyDescent="0.3">
@@ -6606,18 +6664,18 @@
         <v>10</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="2"/>
       <c r="G28" s="8" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6625,18 +6683,18 @@
         <v>11</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="2"/>
       <c r="G29" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="168" x14ac:dyDescent="0.3">
@@ -6644,20 +6702,20 @@
         <v>12</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6665,19 +6723,19 @@
         <v>13</v>
       </c>
       <c r="B31" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>733</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>779</v>
+      </c>
+      <c r="F31" t="s">
         <v>400</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>736</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>785</v>
-      </c>
-      <c r="F31" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6685,16 +6743,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6702,16 +6760,16 @@
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>726</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>404</v>
+        <v>723</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>808</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -6736,7 +6794,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6744,7 +6802,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.3.27 21.33 for 企划
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EA7418-868D-44B1-859E-D8D7878B3C35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94872E1-6D0F-4982-A512-27AF57B98600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="990" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2746,10 +2746,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>电磁选矿机（无gui，石粉从背后的输出口输出</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>球型储罐（无gui</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2855,6 +2851,10 @@
   </si>
   <si>
     <t>六个输入口可以支持流体、物品、气体等；输出口输出产物（优先输出流体，其次气体，再次物品）</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电磁选矿机（无gui</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2994,7 +2994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3062,9 +3062,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4164,8 +4161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AK29" sqref="AK29"/>
     </sheetView>
   </sheetViews>
@@ -6006,11 +6003,11 @@
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
       <c r="AC25" s="9"/>
-      <c r="AJ25" s="32" t="s">
-        <v>800</v>
+      <c r="AJ25" s="31" t="s">
+        <v>799</v>
       </c>
       <c r="AK25" s="13" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6049,11 +6046,11 @@
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
-      <c r="AJ26" s="31" t="s">
-        <v>801</v>
+      <c r="AJ26" s="30" t="s">
+        <v>800</v>
       </c>
       <c r="AK26" s="13" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6085,11 +6082,11 @@
       <c r="AA27" s="9"/>
       <c r="AB27" s="9"/>
       <c r="AC27" s="9"/>
-      <c r="AJ27" s="31" t="s">
-        <v>802</v>
+      <c r="AJ27" s="30" t="s">
+        <v>801</v>
       </c>
       <c r="AK27" s="13" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6121,11 +6118,11 @@
       <c r="AA28" s="9"/>
       <c r="AB28" s="9"/>
       <c r="AC28" s="9"/>
-      <c r="AJ28" s="33" t="s">
-        <v>803</v>
+      <c r="AJ28" s="32" t="s">
+        <v>802</v>
       </c>
       <c r="AK28" s="13" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
   </sheetData>
@@ -6140,8 +6137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6419,7 +6416,7 @@
         <v>370</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6491,7 +6488,7 @@
         <v>739</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -6499,8 +6496,8 @@
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>792</v>
+      <c r="B20" s="28" t="s">
+        <v>791</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>737</v>
@@ -6521,17 +6518,17 @@
         <v>3</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>724</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E21" s="18"/>
-      <c r="F21" s="35" t="s">
-        <v>812</v>
+      <c r="F21" s="34" t="s">
+        <v>811</v>
       </c>
       <c r="G21" t="s">
         <v>381</v>
@@ -6541,20 +6538,20 @@
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>790</v>
+      <c r="B22" s="35" t="s">
+        <v>789</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>725</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>799</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>810</v>
+        <v>798</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>809</v>
       </c>
       <c r="G22" t="s">
         <v>382</v>
@@ -6564,17 +6561,17 @@
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="25" t="s">
         <v>383</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>736</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E23" s="18"/>
-      <c r="F23" s="34"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="8" t="s">
         <v>384</v>
       </c>
@@ -6609,31 +6606,31 @@
         <v>764</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="8" t="s">
         <v>386</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>786</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>728</v>
       </c>
       <c r="D26" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="E26" s="18" t="s">
         <v>795</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>796</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>387</v>
@@ -6642,12 +6639,12 @@
         <v>388</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>787</v>
+      <c r="B27" s="35" t="s">
+        <v>814</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>729</v>
@@ -6689,7 +6686,7 @@
         <v>731</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E29" s="18"/>
       <c r="F29" s="2"/>
@@ -6701,7 +6698,7 @@
       <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="25" t="s">
         <v>394</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -6743,7 +6740,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>722</v>
@@ -6752,7 +6749,7 @@
         <v>401</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6760,13 +6757,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>723</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>402</v>

</xml_diff>

<commit_message>
2021.3.28 10.51 for config
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF4603-EF63-4B72-9FBC-990E5DAC859B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C3EDF8-F4F8-425A-970D-251DFC6BF303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="990" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1135,9 +1135,6 @@
     <t>单晶硅→8晶圆</t>
   </si>
   <si>
-    <t>激光蚀刻机</t>
-  </si>
-  <si>
     <t>晶圆→蚀刻晶圆</t>
   </si>
   <si>
@@ -1154,9 +1151,6 @@
   </si>
   <si>
     <t>特殊炉渣→提炼渣+炉渣</t>
-  </si>
-  <si>
-    <t>金属雾化器</t>
   </si>
   <si>
     <t>熔融金属144mb→金属粉</t>
@@ -2895,12 +2889,20 @@
     <t>球形储罐容量（256000</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>激光蚀刻机（无gui</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>金属雾化器</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2984,8 +2986,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2995,12 +3005,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3083,9 +3087,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3119,6 +3120,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3459,49 +3463,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3515,49 +3519,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3571,49 +3575,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3627,49 +3631,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3683,43 +3687,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3733,37 +3737,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3777,37 +3781,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3821,37 +3825,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L9" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>483</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>485</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3865,29 +3869,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3901,25 +3905,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3933,25 +3937,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3965,19 +3969,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -3991,19 +3995,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -4017,19 +4021,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -4043,19 +4047,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -4069,19 +4073,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -4092,22 +4096,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -4121,13 +4125,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -4141,10 +4145,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4155,7 +4159,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4304,109 +4308,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="11" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="AF2" s="8" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="AH2" s="8" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="AJ2" s="8" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4417,109 +4421,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="X3" s="8" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="AD3" s="8" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="AF3" s="8" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AH3" s="8" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="11" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="AJ3" s="8" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4530,109 +4534,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="AB4" s="8" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="AD4" s="8" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="AF4" s="8" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="11" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="AJ4" s="8" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4643,109 +4647,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="V5" s="8" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="X5" s="8" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="Z5" s="8" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="AB5" s="8" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="AD5" s="8" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="AF5" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="11" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="AJ5" s="8" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4756,103 +4760,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="Z6" s="8" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="AB6" s="8" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="AD6" s="8" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AF6" s="8" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AJ6" s="8" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4863,37 +4867,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -4901,19 +4905,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -4921,31 +4925,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="Z7" s="8" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="AB7" s="8" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="AJ7" s="8" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4956,37 +4960,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -4994,19 +4998,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="T8" s="8" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="11"/>
@@ -5014,31 +5018,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="Z8" s="8" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="AB8" s="8" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="AF8" s="8" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="AJ8" s="8" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5049,37 +5053,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -5087,19 +5091,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="T9" s="13" t="s">
+        <v>740</v>
+      </c>
+      <c r="U9" s="11" t="s">
         <v>742</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>744</v>
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
@@ -5107,31 +5111,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="AB9" s="8" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="AF9" s="8" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="AJ9" s="8" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5142,37 +5146,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -5180,19 +5184,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="T10" s="8" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
@@ -5200,31 +5204,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="Z10" s="8" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="AB10" s="8" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="AF10" s="8" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="AJ10" s="8" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="11" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5235,37 +5239,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -5273,19 +5277,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="T11" s="13" t="s">
+        <v>741</v>
+      </c>
+      <c r="U11" s="12" t="s">
         <v>743</v>
-      </c>
-      <c r="U11" s="12" t="s">
-        <v>745</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
@@ -5293,13 +5297,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="Z11" s="8" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="11" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
@@ -5307,13 +5311,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="AJ11" s="8" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5324,37 +5328,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -5364,7 +5368,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
@@ -5372,13 +5376,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="Z12" s="8" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
@@ -5386,13 +5390,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AJ12" s="8" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5403,37 +5407,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -5452,16 +5456,16 @@
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AF13" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="AG13" s="11" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="AJ13" s="8" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="11" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5472,31 +5476,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -5521,7 +5525,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="11" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5536,19 +5540,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -5572,7 +5576,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="11" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5587,19 +5591,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -5623,7 +5627,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5638,19 +5642,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -5671,10 +5675,10 @@
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
       <c r="AJ17" s="13" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="AK17" s="11" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5689,19 +5693,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -5722,10 +5726,10 @@
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
       <c r="AJ18" s="13" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="AK18" s="11" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5740,19 +5744,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -5773,10 +5777,10 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AJ19" s="13" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="AK19" s="11" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5791,13 +5795,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -5820,10 +5824,10 @@
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
       <c r="AJ20" s="13" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AK20" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5838,13 +5842,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -5867,10 +5871,10 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AJ21" s="13" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="AK21" s="11" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5887,7 +5891,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -5910,10 +5914,10 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AJ22" s="13" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="AK22" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5930,7 +5934,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -5953,10 +5957,10 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AJ23" s="13" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="AK23" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -5973,7 +5977,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -5996,10 +6000,10 @@
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
       <c r="AJ24" s="20" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="AK24" s="12" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6016,7 +6020,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -6038,11 +6042,11 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AJ25" s="30" t="s">
-        <v>797</v>
+      <c r="AJ25" s="29" t="s">
+        <v>795</v>
       </c>
       <c r="AK25" s="12" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6059,7 +6063,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -6081,11 +6085,11 @@
       <c r="AA26" s="8"/>
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
-      <c r="AJ26" s="29" t="s">
-        <v>798</v>
+      <c r="AJ26" s="28" t="s">
+        <v>796</v>
       </c>
       <c r="AK26" s="12" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6117,11 +6121,11 @@
       <c r="AA27" s="8"/>
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
-      <c r="AJ27" s="29" t="s">
-        <v>799</v>
+      <c r="AJ27" s="28" t="s">
+        <v>797</v>
       </c>
       <c r="AK27" s="12" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6153,11 +6157,11 @@
       <c r="AA28" s="8"/>
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
-      <c r="AJ28" s="31" t="s">
-        <v>800</v>
+      <c r="AJ28" s="30" t="s">
+        <v>798</v>
       </c>
       <c r="AK28" s="12" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -6172,8 +6176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6190,7 +6194,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6209,14 +6213,14 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>345</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6234,89 +6238,89 @@
         <v>350</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>351</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>352</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>353</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>354</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>751</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>753</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>754</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>755</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>783</v>
+      <c r="B8" s="22" t="s">
+        <v>781</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6332,102 +6336,102 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
+        <v>822</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>710</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="E9" t="s">
         <v>358</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>712</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>760</v>
-      </c>
-      <c r="E9" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="E10" t="s">
         <v>360</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>713</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>764</v>
-      </c>
-      <c r="E10" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>782</v>
+      <c r="B11" s="24" t="s">
+        <v>780</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E11" t="s">
+        <v>361</v>
+      </c>
+      <c r="F11" t="s">
         <v>362</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>363</v>
-      </c>
-      <c r="G11" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>365</v>
+      <c r="B12" s="34" t="s">
+        <v>823</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E12" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>367</v>
+      <c r="B13" s="34" t="s">
+        <v>365</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>368</v>
+      <c r="B14" s="34" t="s">
+        <v>366</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6445,47 +6449,47 @@
         <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K14" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>371</v>
+      <c r="B15" s="22" t="s">
+        <v>369</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>373</v>
+      <c r="B16" s="22" t="s">
+        <v>371</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
@@ -6493,17 +6497,17 @@
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>378</v>
       </c>
       <c r="G18" t="s">
         <v>344</v>
@@ -6513,17 +6517,17 @@
       <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>379</v>
+      <c r="B19" s="23" t="s">
+        <v>377</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -6531,98 +6535,98 @@
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>789</v>
+      <c r="B20" s="26" t="s">
+        <v>787</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G20" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>788</v>
+      <c r="B21" s="24" t="s">
+        <v>786</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="33" t="s">
-        <v>809</v>
+      <c r="F21" s="32" t="s">
+        <v>807</v>
       </c>
       <c r="G21" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="34" t="s">
-        <v>787</v>
+      <c r="B22" s="33" t="s">
+        <v>785</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>796</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>807</v>
+        <v>794</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>805</v>
       </c>
       <c r="G22" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>383</v>
+      <c r="B23" s="23" t="s">
+        <v>381</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="32"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>6</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>768</v>
+      <c r="B24" s="22" t="s">
+        <v>766</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="2"/>
@@ -6631,177 +6635,177 @@
       <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>385</v>
+      <c r="B25" s="23" t="s">
+        <v>383</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>784</v>
+      <c r="B26" s="27" t="s">
+        <v>782</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>812</v>
+      <c r="B27" s="33" t="s">
+        <v>810</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="2"/>
       <c r="G27" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="70" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>390</v>
+      <c r="B28" s="23" t="s">
+        <v>388</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="2"/>
       <c r="G28" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>392</v>
+      <c r="B29" s="23" t="s">
+        <v>390</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="2"/>
       <c r="G29" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="168" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>394</v>
+      <c r="B30" s="23" t="s">
+        <v>392</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>13</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>729</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="F31" t="s">
         <v>398</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>731</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>777</v>
-      </c>
-      <c r="F31" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>14</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>785</v>
+      <c r="B32" s="22" t="s">
+        <v>783</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>15</v>
       </c>
-      <c r="B33" s="25" t="s">
-        <v>786</v>
+      <c r="B33" s="24" t="s">
+        <v>784</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -6826,7 +6830,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6834,76 +6838,76 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>820</v>
+      <c r="B6" s="28" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>815</v>
+      <c r="B7" s="28" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>822</v>
+      <c r="B8" s="28" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>816</v>
+      <c r="B9" s="28" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>817</v>
+      <c r="B10" s="28" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>818</v>
+      <c r="B11" s="28" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>819</v>
+      <c r="B12" s="28" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>823</v>
+      <c r="B13" s="28" t="s">
+        <v>821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.4.5 20.19 for gui
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35061D44-4F66-4AE2-9E81-3FF7968644E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CC1BD6-7B0D-457A-B2E7-2EE773BC66EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1205,9 +1205,6 @@
     <t>电力高炉</t>
   </si>
   <si>
-    <t>合金配方：铁锭+碳粉→144mb钢；2铁锭+1镍锭→432mb殷钢；3铜锭+1锡锭→576mb青铜；2钢锭+1不锈钢添加剂→432mb不锈钢</t>
-  </si>
-  <si>
     <t>破碎用转轴</t>
   </si>
   <si>
@@ -1233,9 +1230,6 @@
   </si>
   <si>
     <t>工作时渲染火花</t>
-  </si>
-  <si>
-    <t>8铁粉+1碳粉→8钢锭；2铁粉+1镍粉→3殷钢锭；4碳粉+4钨粉+1钴粉→5钨钢锭；3铜粉+1锡粉→4青铜锭；4钢粉+3镍粉+2铬粉→5镍铬合金锭；2钢粉+1不锈钢添加剂→3不锈钢锭；6钢粉+1镍粉+1铬粉+1锰粉→9不锈钢锭；3钨钢粉+5钢粉+1高速钢添加剂→9高速钢锭</t>
   </si>
   <si>
     <t>熔化机</t>
@@ -2869,10 +2863,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>电动泵</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>焊接室</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2934,6 +2924,18 @@
   </si>
   <si>
     <t>冶炼炉灯光</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>8铁粉+1碳粉→8钢锭；2铁粉+1镍粉→3殷钢锭；4碳粉+4钨粉+1钴粉→5钨钢锭；3铜粉+1锡粉→4青铜锭；4钢粉+3镍粉+2铬粉→5镍铬合金锭；2钢粉+1不锈钢添加剂→2不锈钢锭；6钢粉+1镍粉+1铬粉+1锰粉→9不锈钢锭；3钨钢粉+5钢粉+1高速钢添加剂→9高速钢锭</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>合金配方：铁锭+碳粉→144mb钢；2铁锭+1镍锭→432mb殷钢；3铜锭+1锡锭→576mb青铜；2钢锭+1不锈钢添加剂→288mb不锈钢</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电动泵（无gui</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -2941,7 +2943,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3025,6 +3027,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3067,7 +3077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3151,6 +3161,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3491,49 +3504,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3547,49 +3560,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3603,49 +3616,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3659,49 +3672,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3715,43 +3728,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3765,37 +3778,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3809,37 +3822,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3853,37 +3866,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L9" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>477</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>479</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3897,29 +3910,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3933,25 +3946,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3965,25 +3978,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -3997,19 +4010,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -4023,19 +4036,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -4049,19 +4062,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -4075,19 +4088,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -4101,19 +4114,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -4124,22 +4137,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -4153,13 +4166,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -4173,10 +4186,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4187,7 +4200,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4336,109 +4349,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="11" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AF2" s="8" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="AH2" s="8" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="AJ2" s="8" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4449,109 +4462,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="X3" s="8" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AD3" s="8" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AF3" s="8" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="11" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="AH3" s="8" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="AJ3" s="8" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="11" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4562,109 +4575,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="AB4" s="8" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AD4" s="8" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AF4" s="8" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="AJ4" s="8" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4675,109 +4688,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="V5" s="8" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="X5" s="8" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="Z5" s="8" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="AB5" s="8" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="AD5" s="8" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="AF5" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="AJ5" s="8" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4788,103 +4801,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="Z6" s="8" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="AB6" s="8" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="AD6" s="8" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AF6" s="8" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="AJ6" s="8" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="11" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4895,37 +4908,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -4933,19 +4946,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -4953,31 +4966,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="Z7" s="8" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="AB7" s="8" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="11" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="AJ7" s="8" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -4988,37 +5001,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -5026,19 +5039,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="T8" s="8" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="11"/>
@@ -5046,31 +5059,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="Z8" s="8" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="AB8" s="8" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="AF8" s="8" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="AJ8" s="8" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="11" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5081,37 +5094,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -5119,19 +5132,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="T9" s="13" t="s">
+        <v>728</v>
+      </c>
+      <c r="U9" s="11" t="s">
         <v>730</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>732</v>
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
@@ -5139,31 +5152,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="AB9" s="8" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AF9" s="8" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AJ9" s="8" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="11" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5174,37 +5187,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -5212,19 +5225,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="T10" s="8" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
@@ -5232,31 +5245,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="Z10" s="8" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="AB10" s="8" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="11" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="AF10" s="8" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="AJ10" s="8" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5267,37 +5280,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -5305,19 +5318,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="T11" s="13" t="s">
+        <v>729</v>
+      </c>
+      <c r="U11" s="12" t="s">
         <v>731</v>
-      </c>
-      <c r="U11" s="12" t="s">
-        <v>733</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
@@ -5325,13 +5338,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="Z11" s="8" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="11" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
@@ -5339,13 +5352,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="AJ11" s="8" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="11" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5356,37 +5369,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -5396,7 +5409,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
@@ -5404,13 +5417,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="Z12" s="8" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
@@ -5418,13 +5431,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AJ12" s="8" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="11" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5435,37 +5448,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -5484,16 +5497,16 @@
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AF13" s="9" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="AG13" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="AJ13" s="8" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5504,31 +5517,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -5553,7 +5566,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="11" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5568,19 +5581,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -5604,7 +5617,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5619,19 +5632,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -5655,7 +5668,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5670,19 +5683,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -5703,10 +5716,10 @@
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
       <c r="AJ17" s="13" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="AK17" s="11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5721,19 +5734,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -5754,10 +5767,10 @@
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
       <c r="AJ18" s="13" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="AK18" s="11" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5772,19 +5785,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -5805,10 +5818,10 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AJ19" s="13" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="AK19" s="11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5823,13 +5836,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -5852,10 +5865,10 @@
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
       <c r="AJ20" s="13" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="AK20" s="11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5870,13 +5883,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -5899,10 +5912,10 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AJ21" s="13" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="AK21" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5919,7 +5932,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -5942,10 +5955,10 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AJ22" s="13" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="AK22" s="12" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5962,7 +5975,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -5985,10 +5998,10 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AJ23" s="13" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="AK23" s="12" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6005,7 +6018,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -6028,10 +6041,10 @@
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
       <c r="AJ24" s="20" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="AK24" s="12" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6048,7 +6061,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -6071,10 +6084,10 @@
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
       <c r="AJ25" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AK25" s="12" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6091,7 +6104,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -6114,10 +6127,10 @@
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
       <c r="AJ26" s="27" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="AK26" s="12" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6150,10 +6163,10 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AJ27" s="27" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="AK27" s="12" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6186,10 +6199,10 @@
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AJ28" s="29" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="AK28" s="12" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>
@@ -6204,8 +6217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6222,7 +6235,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6245,10 +6258,10 @@
         <v>345</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6266,7 +6279,7 @@
         <v>350</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6277,10 +6290,10 @@
         <v>351</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6291,10 +6304,10 @@
         <v>352</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6305,10 +6318,10 @@
         <v>353</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6319,22 +6332,22 @@
         <v>354</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>741</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>742</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>743</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6342,13 +6355,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6357,7 +6370,7 @@
         <v>356</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6365,13 +6378,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E9" t="s">
         <v>357</v>
@@ -6385,10 +6398,10 @@
         <v>358</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E10" t="s">
         <v>359</v>
@@ -6398,14 +6411,14 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>770</v>
+      <c r="B11" s="34" t="s">
+        <v>768</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E11" t="s">
         <v>360</v>
@@ -6422,13 +6435,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E12" t="s">
         <v>363</v>
@@ -6438,14 +6451,14 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>814</v>
+      <c r="B13" s="34" t="s">
+        <v>830</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6453,13 +6466,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6483,7 +6496,7 @@
         <v>365</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6494,10 +6507,10 @@
         <v>366</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E15" t="s">
         <v>367</v>
@@ -6511,10 +6524,10 @@
         <v>368</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E16" t="s">
         <v>369</v>
@@ -6549,16 +6562,16 @@
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F19" s="31" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6566,20 +6579,20 @@
         <v>2</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="6" t="s">
         <v>375</v>
       </c>
       <c r="G20" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -6587,17 +6600,17 @@
         <v>3</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="31" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G21" t="s">
         <v>376</v>
@@ -6608,19 +6621,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="G22" t="s">
         <v>377</v>
@@ -6634,14 +6647,14 @@
         <v>378</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="30" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>379</v>
@@ -6652,17 +6665,17 @@
         <v>6</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="30" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -6673,22 +6686,22 @@
         <v>380</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>381</v>
+        <v>823</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>829</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
@@ -6696,22 +6709,22 @@
         <v>8</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>382</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6719,18 +6732,18 @@
         <v>9</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="30" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="70" x14ac:dyDescent="0.3">
@@ -6738,20 +6751,20 @@
         <v>10</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="30" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6759,20 +6772,20 @@
         <v>11</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="30" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="168" x14ac:dyDescent="0.3">
@@ -6780,20 +6793,20 @@
         <v>12</v>
       </c>
       <c r="B30" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>716</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>389</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>718</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>390</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="30" t="s">
-        <v>830</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>391</v>
+        <v>827</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6801,19 +6814,19 @@
         <v>13</v>
       </c>
       <c r="B31" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>717</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>763</v>
+      </c>
+      <c r="F31" t="s">
         <v>392</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>765</v>
-      </c>
-      <c r="F31" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6821,16 +6834,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6838,16 +6851,16 @@
         <v>15</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -6873,7 +6886,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6881,7 +6894,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
   </sheetData>
@@ -6907,7 +6920,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6915,7 +6928,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6923,7 +6936,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6931,7 +6944,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -6939,7 +6952,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6947,7 +6960,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6955,7 +6968,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -6963,7 +6976,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6971,7 +6984,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.4.10 19.11 for flying wheel
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CC1BD6-7B0D-457A-B2E7-2EE773BC66EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B80D3D-BC8B-4C6B-B28C-455E7C90D656}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2289,6 +2289,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>键3次，产出成品，空手右键取下</t>
@@ -2423,6 +2424,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>个模板，可以熔炼青铜合金【锭160mb、杆80mb、</t>
@@ -2443,6 +2445,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>mb、</t>
@@ -2463,6 +2466,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>】</t>
@@ -2482,6 +2486,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>fe</t>
@@ -2497,6 +2502,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>0000fe，每tick消耗</t>
@@ -2527,6 +2533,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t/>
@@ -2554,6 +2561,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>0000fe，每tick消耗</t>
@@ -2649,6 +2657,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>，每</t>
@@ -2669,6 +2678,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>消耗50</t>
@@ -2943,7 +2953,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2956,17 +2966,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3004,12 +3017,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -3128,7 +3135,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3140,7 +3147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3159,10 +3166,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6217,8 +6224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:G11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6434,7 +6441,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="34" t="s">
         <v>811</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -6465,7 +6472,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="34" t="s">
         <v>812</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -6833,7 +6840,7 @@
       <c r="A32" s="2">
         <v>14</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="34" t="s">
         <v>771</v>
       </c>
       <c r="C32" s="11" t="s">

</xml_diff>

<commit_message>
2021.4.11 10.34 for recipe debug and flywheel battery
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B80D3D-BC8B-4C6B-B28C-455E7C90D656}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC7929-80FE-4043-A3B4-4897342D6C70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -4248,9 +4248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA12" sqref="AA12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AK28" sqref="AK28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6224,8 +6224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
2021.7.25 21.01 for thermal_power_plant and forging_press
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC7929-80FE-4043-A3B4-4897342D6C70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A81B2-05BC-4E7E-B1C5-179001173B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -3084,7 +3084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3145,9 +3145,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4248,7 +4245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AK28" sqref="AK28"/>
     </sheetView>
@@ -6090,7 +6087,7 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AJ25" s="28" t="s">
+      <c r="AJ25" s="27" t="s">
         <v>783</v>
       </c>
       <c r="AK25" s="12" t="s">
@@ -6133,7 +6130,7 @@
       <c r="AA26" s="8"/>
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
-      <c r="AJ26" s="27" t="s">
+      <c r="AJ26" s="26" t="s">
         <v>784</v>
       </c>
       <c r="AK26" s="12" t="s">
@@ -6169,7 +6166,7 @@
       <c r="AA27" s="8"/>
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
-      <c r="AJ27" s="27" t="s">
+      <c r="AJ27" s="26" t="s">
         <v>785</v>
       </c>
       <c r="AK27" s="12" t="s">
@@ -6205,7 +6202,7 @@
       <c r="AA28" s="8"/>
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
-      <c r="AJ28" s="29" t="s">
+      <c r="AJ28" s="28" t="s">
         <v>786</v>
       </c>
       <c r="AK28" s="12" t="s">
@@ -6224,8 +6221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6418,7 +6415,7 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>768</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -6441,7 +6438,7 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>811</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -6458,7 +6455,7 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>830</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -6472,7 +6469,7 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>812</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -6565,7 +6562,7 @@
       <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="33" t="s">
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -6577,7 +6574,7 @@
       <c r="E19" s="17" t="s">
         <v>781</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="30" t="s">
         <v>821</v>
       </c>
     </row>
@@ -6585,7 +6582,7 @@
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="33" t="s">
         <v>775</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -6616,7 +6613,7 @@
         <v>796</v>
       </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="30" t="s">
         <v>795</v>
       </c>
       <c r="G21" t="s">
@@ -6627,7 +6624,7 @@
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>773</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -6639,7 +6636,7 @@
       <c r="E22" s="17" t="s">
         <v>782</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="30" t="s">
         <v>793</v>
       </c>
       <c r="G22" t="s">
@@ -6660,7 +6657,7 @@
         <v>797</v>
       </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="29" t="s">
         <v>820</v>
       </c>
       <c r="G23" s="7" t="s">
@@ -6681,7 +6678,7 @@
         <v>755</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="29" t="s">
         <v>822</v>
       </c>
     </row>
@@ -6701,7 +6698,7 @@
       <c r="E25" s="17" t="s">
         <v>780</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="29" t="s">
         <v>823</v>
       </c>
       <c r="G25" s="16" t="s">
@@ -6715,7 +6712,7 @@
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="32" t="s">
         <v>770</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -6738,7 +6735,7 @@
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="31" t="s">
         <v>798</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -6746,7 +6743,7 @@
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="29" t="s">
         <v>824</v>
       </c>
       <c r="G27" s="7" t="s">
@@ -6767,7 +6764,7 @@
         <v>749</v>
       </c>
       <c r="E28" s="17"/>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="29" t="s">
         <v>825</v>
       </c>
       <c r="G28" s="7" t="s">
@@ -6788,7 +6785,7 @@
         <v>776</v>
       </c>
       <c r="E29" s="17"/>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="29" t="s">
         <v>826</v>
       </c>
       <c r="G29" s="7" t="s">
@@ -6809,7 +6806,7 @@
         <v>389</v>
       </c>
       <c r="E30" s="17"/>
-      <c r="F30" s="30" t="s">
+      <c r="F30" s="29" t="s">
         <v>827</v>
       </c>
       <c r="G30" s="16" t="s">
@@ -6840,7 +6837,7 @@
       <c r="A32" s="2">
         <v>14</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="33" t="s">
         <v>771</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -6934,7 +6931,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>806</v>
       </c>
     </row>
@@ -6942,7 +6939,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>801</v>
       </c>
     </row>
@@ -6950,7 +6947,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>808</v>
       </c>
     </row>
@@ -6958,7 +6955,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>802</v>
       </c>
     </row>
@@ -6966,7 +6963,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>803</v>
       </c>
     </row>
@@ -6974,7 +6971,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>804</v>
       </c>
     </row>
@@ -6982,7 +6979,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>805</v>
       </c>
     </row>
@@ -6990,7 +6987,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>809</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021.7.25 21.39 for 企划
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A81B2-05BC-4E7E-B1C5-179001173B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC0C73E-6C88-4745-A6BB-F01438B5C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -2637,10 +2637,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>已完工的为红字，完成模型的为黄底，尚未启动制作的是白色</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>最大电容40000fe，每tick发电200fe</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2948,12 +2944,16 @@
     <t>电动泵（无gui</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>尚未启动制作的是白色，完成模型的为黄底，完成gui的为红字，完成配方填写的为黄底加粗红字，已完工的为蓝底黑字</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3019,15 +3019,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="等线"/>
       <family val="3"/>
@@ -3043,7 +3034,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3053,6 +3044,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3084,7 +3081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3135,22 +3132,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3160,14 +3145,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4245,9 +4248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK28" sqref="AK28"/>
+      <selection pane="topRight" activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4377,7 +4380,7 @@
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
@@ -4425,7 +4428,7 @@
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
@@ -4455,7 +4458,7 @@
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4538,7 +4541,7 @@
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
@@ -4681,7 +4684,7 @@
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4982,7 +4985,7 @@
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
@@ -6087,11 +6090,11 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AJ25" s="27" t="s">
-        <v>783</v>
+      <c r="AJ25" s="35" t="s">
+        <v>782</v>
       </c>
       <c r="AK25" s="12" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6130,11 +6133,11 @@
       <c r="AA26" s="8"/>
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
-      <c r="AJ26" s="26" t="s">
-        <v>784</v>
+      <c r="AJ26" s="20" t="s">
+        <v>783</v>
       </c>
       <c r="AK26" s="12" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6166,11 +6169,11 @@
       <c r="AA27" s="8"/>
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
-      <c r="AJ27" s="26" t="s">
-        <v>785</v>
+      <c r="AJ27" s="20" t="s">
+        <v>784</v>
       </c>
       <c r="AK27" s="12" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6202,11 +6205,11 @@
       <c r="AA28" s="8"/>
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
-      <c r="AJ28" s="28" t="s">
-        <v>786</v>
+      <c r="AJ28" s="24" t="s">
+        <v>785</v>
       </c>
       <c r="AK28" s="12" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -6221,8 +6224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6239,7 +6242,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>764</v>
+        <v>830</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6258,7 +6261,7 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>345</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -6290,7 +6293,7 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="28" t="s">
         <v>351</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -6304,7 +6307,7 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="28" t="s">
         <v>352</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -6318,7 +6321,7 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="28" t="s">
         <v>353</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -6332,7 +6335,7 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="28" t="s">
         <v>354</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -6358,8 +6361,8 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>769</v>
+      <c r="B8" s="28" t="s">
+        <v>768</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>694</v>
@@ -6374,15 +6377,15 @@
         <v>356</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>810</v>
+      <c r="B9" s="28" t="s">
+        <v>809</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>698</v>
@@ -6398,7 +6401,7 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="28" t="s">
         <v>358</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -6415,8 +6418,8 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>768</v>
+      <c r="B11" s="27" t="s">
+        <v>767</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>700</v>
@@ -6438,8 +6441,8 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="33" t="s">
-        <v>811</v>
+      <c r="B12" s="27" t="s">
+        <v>810</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>701</v>
@@ -6455,22 +6458,22 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>830</v>
+      <c r="B13" s="29" t="s">
+        <v>829</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>702</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="33" t="s">
-        <v>812</v>
+      <c r="B14" s="27" t="s">
+        <v>811</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>703</v>
@@ -6500,21 +6503,21 @@
         <v>365</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="28" t="s">
         <v>366</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>704</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E15" t="s">
         <v>367</v>
@@ -6524,14 +6527,14 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="28" t="s">
         <v>368</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>705</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E16" t="s">
         <v>369</v>
@@ -6562,28 +6565,28 @@
       <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="29" t="s">
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>723</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>781</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>821</v>
+        <v>780</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>775</v>
+      <c r="B20" s="29" t="s">
+        <v>774</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>721</v>
@@ -6603,18 +6606,18 @@
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>774</v>
+      <c r="B21" s="30" t="s">
+        <v>773</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>708</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="30" t="s">
-        <v>795</v>
+      <c r="F21" s="26" t="s">
+        <v>794</v>
       </c>
       <c r="G21" t="s">
         <v>376</v>
@@ -6625,19 +6628,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>709</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>782</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>793</v>
+        <v>781</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>792</v>
       </c>
       <c r="G22" t="s">
         <v>377</v>
@@ -6647,18 +6650,18 @@
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="32" t="s">
         <v>378</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>720</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="29" t="s">
-        <v>820</v>
+      <c r="F23" s="25" t="s">
+        <v>819</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>379</v>
@@ -6668,7 +6671,7 @@
       <c r="A24" s="2">
         <v>6</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="28" t="s">
         <v>754</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -6678,15 +6681,15 @@
         <v>755</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="29" t="s">
-        <v>822</v>
+      <c r="F24" s="25" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="34" t="s">
         <v>380</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -6696,33 +6699,33 @@
         <v>748</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>780</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>823</v>
+        <v>779</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>822</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>770</v>
+      <c r="B26" s="33" t="s">
+        <v>769</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>712</v>
       </c>
       <c r="D26" s="18" t="s">
+        <v>777</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>778</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>779</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>381</v>
@@ -6736,15 +6739,15 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>713</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="29" t="s">
-        <v>824</v>
+      <c r="F27" s="25" t="s">
+        <v>823</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>383</v>
@@ -6754,7 +6757,7 @@
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="32" t="s">
         <v>384</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -6764,8 +6767,8 @@
         <v>749</v>
       </c>
       <c r="E28" s="17"/>
-      <c r="F28" s="29" t="s">
-        <v>825</v>
+      <c r="F28" s="25" t="s">
+        <v>824</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>385</v>
@@ -6775,18 +6778,18 @@
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="32" t="s">
         <v>386</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>715</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E29" s="17"/>
-      <c r="F29" s="29" t="s">
-        <v>826</v>
+      <c r="F29" s="25" t="s">
+        <v>825</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>387</v>
@@ -6796,7 +6799,7 @@
       <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="32" t="s">
         <v>388</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -6806,18 +6809,18 @@
         <v>389</v>
       </c>
       <c r="E30" s="17"/>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="25" t="s">
+        <v>826</v>
+      </c>
+      <c r="G30" s="16" t="s">
         <v>827</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>13</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="22" t="s">
         <v>390</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -6837,8 +6840,8 @@
       <c r="A32" s="2">
         <v>14</v>
       </c>
-      <c r="B32" s="33" t="s">
-        <v>771</v>
+      <c r="B32" s="29" t="s">
+        <v>770</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>706</v>
@@ -6847,21 +6850,21 @@
         <v>393</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>15</v>
       </c>
-      <c r="B33" s="24" t="s">
-        <v>772</v>
+      <c r="B33" s="30" t="s">
+        <v>771</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>707</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>394</v>
@@ -6898,7 +6901,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
   </sheetData>
@@ -6924,71 +6927,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>806</v>
+      <c r="B2" s="23" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>801</v>
+      <c r="B3" s="23" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>808</v>
+      <c r="B4" s="23" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>802</v>
+      <c r="B5" s="23" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>803</v>
+      <c r="B6" s="23" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>804</v>
+      <c r="B7" s="23" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>805</v>
+      <c r="B8" s="23" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>809</v>
+      <c r="B9" s="23" t="s">
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.7.28 21.39 for many
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC0C73E-6C88-4745-A6BB-F01438B5C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570233E-72D4-476F-A9B2-05C554708616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1202,9 +1202,6 @@
     <t>苹果+水→苹果汁；烈焰粉+苹果汁→苹果糖；金锭+苹果汁→金苹果汁；紫颂花+金苹果汁→金苹果糖；腐化蜘蛛眼+苹果汁→乙烯；烈焰粉+乙烯→聚乙烯片</t>
   </si>
   <si>
-    <t>电力高炉</t>
-  </si>
-  <si>
     <t>破碎用转轴</t>
   </si>
   <si>
@@ -1214,19 +1211,10 @@
     <t>粉碎矿石→精矿+石粉+概率金属粉</t>
   </si>
   <si>
-    <t>单晶炉</t>
-  </si>
-  <si>
     <t>硅锭+64硅粉→1单晶硅；石英+64硅粉→64石英；钻石+64碳粉→2钻石；石墨锭+32碳粉→2石墨锭</t>
   </si>
   <si>
-    <t>数控机床</t>
-  </si>
-  <si>
     <t>齿轮坯→齿轮;锭→2杆；杆→2螺丝；轴→辊</t>
-  </si>
-  <si>
-    <t>真空冶炼炉</t>
   </si>
   <si>
     <t>工作时渲染火花</t>
@@ -2946,6 +2934,22 @@
   </si>
   <si>
     <t>尚未启动制作的是白色，完成模型的为黄底，完成gui的为红字，完成配方填写的为黄底加粗红字，已完工的为蓝底黑字</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>电力高炉</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>单晶炉</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>数控机床</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>真空冶炼炉</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -3081,7 +3085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3160,9 +3164,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3171,6 +3172,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3511,49 +3518,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3567,49 +3574,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3623,49 +3630,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3679,49 +3686,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3735,43 +3742,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3785,37 +3792,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3829,37 +3836,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="L8" t="s">
         <v>63</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="N8" t="s">
         <v>64</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="P8" t="s">
         <v>65</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3873,37 +3880,37 @@
         <v>67</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="P9" t="s">
         <v>71</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3917,29 +3924,29 @@
         <v>73</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D10" t="s">
         <v>74</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F10" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3953,25 +3960,25 @@
         <v>78</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="P11" t="s">
         <v>81</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -3985,25 +3992,25 @@
         <v>83</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D12" t="s">
         <v>84</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="P12" t="s">
         <v>86</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -4017,19 +4024,19 @@
         <v>87</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F13" t="s">
         <v>89</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="R13" t="s">
         <v>94</v>
@@ -4043,19 +4050,19 @@
         <v>91</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D14" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F14" t="s">
         <v>93</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="R14" t="s">
         <v>98</v>
@@ -4069,19 +4076,19 @@
         <v>95</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F15" t="s">
         <v>97</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="R15" t="s">
         <v>102</v>
@@ -4095,19 +4102,19 @@
         <v>99</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D16" t="s">
         <v>100</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F16" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="R16" t="s">
         <v>106</v>
@@ -4121,19 +4128,19 @@
         <v>103</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="R17" t="s">
         <v>109</v>
@@ -4144,22 +4151,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D18" t="s">
         <v>107</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F18" t="s">
         <v>108</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="R18" t="s">
         <v>112</v>
@@ -4173,13 +4180,13 @@
         <v>110</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F19" t="s">
         <v>111</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="R19" t="s">
         <v>116</v>
@@ -4193,10 +4200,10 @@
         <v>113</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4207,7 +4214,7 @@
         <v>115</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="R21" t="s">
         <v>90</v>
@@ -4248,7 +4255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AG25" sqref="AG25"/>
     </sheetView>
@@ -4356,109 +4363,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="V2" s="13" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="11" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="AF2" s="8" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="AH2" s="8" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="AJ2" s="8" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4469,109 +4476,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="X3" s="8" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="AD3" s="8" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="AF3" s="8" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="11" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="AH3" s="8" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="11" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="AJ3" s="8" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="11" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4582,109 +4589,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="AB4" s="8" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="AD4" s="8" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="AF4" s="8" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="11" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="AJ4" s="8" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4695,109 +4702,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="V5" s="8" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="X5" s="8" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="Z5" s="8" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="AB5" s="8" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="AD5" s="8" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="AF5" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="11" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="AJ5" s="8" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="11" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4808,103 +4815,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="Z6" s="8" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AB6" s="8" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="AD6" s="8" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="AF6" s="8" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="AJ6" s="8" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="11" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4915,37 +4922,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -4953,19 +4960,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -4973,31 +4980,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="Z7" s="8" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="AB7" s="8" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="11" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="AJ7" s="8" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -5008,37 +5015,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -5046,19 +5053,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="T8" s="8" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="11"/>
@@ -5066,31 +5073,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="Z8" s="8" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="AB8" s="8" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="AF8" s="8" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="AJ8" s="8" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="11" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5101,37 +5108,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -5139,19 +5146,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
@@ -5159,31 +5166,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="AB9" s="8" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="AF9" s="8" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="AJ9" s="8" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="11" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5194,37 +5201,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -5232,19 +5239,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="T10" s="8" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
@@ -5252,31 +5259,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="Z10" s="8" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="AB10" s="8" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="11" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="AF10" s="8" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="AJ10" s="8" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="11" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5287,37 +5294,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -5325,19 +5332,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
@@ -5345,13 +5352,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="Z11" s="8" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="11" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
@@ -5359,13 +5366,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="AJ11" s="8" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="11" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5376,37 +5383,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -5416,7 +5423,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
@@ -5424,13 +5431,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="Z12" s="8" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
@@ -5438,13 +5445,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="AJ12" s="8" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="11" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5455,37 +5462,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -5504,16 +5511,16 @@
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AF13" s="9" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="AG13" s="11" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="AJ13" s="8" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="11" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5524,31 +5531,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -5573,7 +5580,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="11" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5588,19 +5595,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -5624,7 +5631,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="11" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5639,19 +5646,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -5675,7 +5682,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="11" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5690,19 +5697,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -5723,10 +5730,10 @@
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
       <c r="AJ17" s="13" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="AK17" s="11" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5741,19 +5748,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -5774,10 +5781,10 @@
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
       <c r="AJ18" s="13" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="AK18" s="11" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5792,19 +5799,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -5825,10 +5832,10 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AJ19" s="13" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="AK19" s="11" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5843,13 +5850,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -5872,10 +5879,10 @@
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
       <c r="AJ20" s="13" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="AK20" s="11" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5890,13 +5897,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -5919,10 +5926,10 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AJ21" s="13" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="AK21" s="11" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5939,7 +5946,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -5962,10 +5969,10 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AJ22" s="13" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="AK22" s="12" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5982,7 +5989,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -6005,10 +6012,10 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AJ23" s="13" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="AK23" s="12" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6025,7 +6032,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -6048,10 +6055,10 @@
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
       <c r="AJ24" s="20" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="AK24" s="12" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6068,7 +6075,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -6090,11 +6097,11 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AJ25" s="35" t="s">
+      <c r="AJ25" s="34" t="s">
+        <v>778</v>
+      </c>
+      <c r="AK25" s="12" t="s">
         <v>782</v>
-      </c>
-      <c r="AK25" s="12" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6111,7 +6118,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -6134,10 +6141,10 @@
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
       <c r="AJ26" s="20" t="s">
+        <v>779</v>
+      </c>
+      <c r="AK26" s="12" t="s">
         <v>783</v>
-      </c>
-      <c r="AK26" s="12" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6170,10 +6177,10 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AJ27" s="20" t="s">
+        <v>780</v>
+      </c>
+      <c r="AK27" s="12" t="s">
         <v>784</v>
-      </c>
-      <c r="AK27" s="12" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6206,10 +6213,10 @@
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AJ28" s="24" t="s">
+        <v>781</v>
+      </c>
+      <c r="AK28" s="12" t="s">
         <v>785</v>
-      </c>
-      <c r="AK28" s="12" t="s">
-        <v>789</v>
       </c>
     </row>
   </sheetData>
@@ -6224,8 +6231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6242,7 +6249,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6265,10 +6272,10 @@
         <v>345</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6286,7 +6293,7 @@
         <v>350</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6297,10 +6304,10 @@
         <v>351</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6311,10 +6318,10 @@
         <v>352</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6325,10 +6332,10 @@
         <v>353</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6339,22 +6346,22 @@
         <v>354</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6362,13 +6369,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6377,7 +6384,7 @@
         <v>356</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6385,13 +6392,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="E9" t="s">
         <v>357</v>
@@ -6405,10 +6412,10 @@
         <v>358</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="E10" t="s">
         <v>359</v>
@@ -6419,13 +6426,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E11" t="s">
         <v>360</v>
@@ -6442,13 +6449,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="E12" t="s">
         <v>363</v>
@@ -6459,13 +6466,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6473,13 +6480,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6503,7 +6510,7 @@
         <v>365</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6514,10 +6521,10 @@
         <v>366</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="E15" t="s">
         <v>367</v>
@@ -6531,10 +6538,10 @@
         <v>368</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="E16" t="s">
         <v>369</v>
@@ -6569,16 +6576,16 @@
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6586,38 +6593,38 @@
         <v>2</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="6" t="s">
         <v>375</v>
       </c>
       <c r="G20" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>773</v>
+      <c r="B21" s="35" t="s">
+        <v>769</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="26" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="G21" t="s">
         <v>376</v>
@@ -6628,19 +6635,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="G22" t="s">
         <v>377</v>
@@ -6650,18 +6657,18 @@
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="36" t="s">
         <v>378</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="25" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>379</v>
@@ -6672,66 +6679,66 @@
         <v>6</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="25" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="34" t="s">
-        <v>380</v>
+      <c r="B25" s="33" t="s">
+        <v>827</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="33" t="s">
-        <v>769</v>
+      <c r="B26" s="32" t="s">
+        <v>765</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6739,81 +6746,81 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="25" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="70" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>384</v>
+      <c r="B28" s="30" t="s">
+        <v>828</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="25" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="32" t="s">
-        <v>386</v>
+      <c r="B29" s="30" t="s">
+        <v>829</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="25" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="168" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>388</v>
+      <c r="B30" s="30" t="s">
+        <v>830</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="25" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6821,19 +6828,19 @@
         <v>13</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="F31" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6841,16 +6848,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6858,16 +6865,16 @@
         <v>15</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -6893,7 +6900,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6901,7 +6908,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
     </row>
   </sheetData>
@@ -6927,7 +6934,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6935,7 +6942,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6943,7 +6950,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6951,7 +6958,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -6959,7 +6966,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6967,7 +6974,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6975,7 +6982,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -6983,7 +6990,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6991,7 +6998,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.8.1 20.24 for crystal_growing_furnace
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570233E-72D4-476F-A9B2-05C554708616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276619B6-DDED-4C88-A124-CB36A5C299D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="829">
   <si>
     <t>矿石</t>
   </si>
@@ -2781,10 +2781,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>四个按钮（依次为线、杆、板、管）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>共有四个按钮，对应四种生产类型，按下会让按钮移动1/16个方块，其他按钮恢复原位，刚建造的时候默认板材</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2889,10 +2885,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>反应釜灯光</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>火电灯光（close为不运行的状态，open为运行时的状态，open状态的附属件有亮度</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2909,10 +2901,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>单晶炉灯光</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>机床灯光</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2950,6 +2938,10 @@
   </si>
   <si>
     <t>真空冶炼炉</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>四个按钮（依次为线、杆、板、管）、开关灯光</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -4387,7 +4379,7 @@
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
@@ -4435,7 +4427,7 @@
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
@@ -4465,7 +4457,7 @@
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4548,7 +4540,7 @@
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
@@ -4691,7 +4683,7 @@
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4992,7 +4984,7 @@
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
@@ -6231,8 +6223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6249,7 +6241,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6384,7 +6376,7 @@
         <v>356</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6392,7 +6384,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>694</v>
@@ -6449,7 +6441,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>697</v>
@@ -6466,7 +6458,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>698</v>
@@ -6480,7 +6472,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>699</v>
@@ -6576,7 +6568,7 @@
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>719</v>
@@ -6585,7 +6577,7 @@
         <v>776</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6620,17 +6612,17 @@
         <v>704</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="26" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G21" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>4</v>
       </c>
@@ -6641,13 +6633,13 @@
         <v>705</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>777</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>788</v>
+        <v>828</v>
       </c>
       <c r="G22" t="s">
         <v>377</v>
@@ -6664,12 +6656,10 @@
         <v>716</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="25" t="s">
-        <v>815</v>
-      </c>
+      <c r="F23" s="25"/>
       <c r="G23" s="7" t="s">
         <v>379</v>
       </c>
@@ -6689,7 +6679,7 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="25" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -6697,7 +6687,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>707</v>
@@ -6709,10 +6699,10 @@
         <v>775</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>787</v>
@@ -6746,7 +6736,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>709</v>
@@ -6754,7 +6744,7 @@
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="25" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>382</v>
@@ -6764,8 +6754,8 @@
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="30" t="s">
-        <v>828</v>
+      <c r="B28" s="35" t="s">
+        <v>825</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>710</v>
@@ -6774,9 +6764,7 @@
         <v>745</v>
       </c>
       <c r="E28" s="17"/>
-      <c r="F28" s="25" t="s">
-        <v>820</v>
-      </c>
+      <c r="F28" s="25"/>
       <c r="G28" s="7" t="s">
         <v>383</v>
       </c>
@@ -6786,7 +6774,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>711</v>
@@ -6796,7 +6784,7 @@
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="25" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>384</v>
@@ -6807,7 +6795,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>712</v>
@@ -6817,10 +6805,10 @@
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="25" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6908,7 +6896,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
   </sheetData>
@@ -6934,7 +6922,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6942,7 +6930,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6950,7 +6938,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6958,7 +6946,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -6966,7 +6954,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6974,7 +6962,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6982,7 +6970,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -6990,7 +6978,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6998,7 +6986,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.8.5 20.54 for container
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276619B6-DDED-4C88-A124-CB36A5C299D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C9A7C-2DA3-4293-A2F1-99CA84BB0EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="3000" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="831">
   <si>
     <t>矿石</t>
   </si>
@@ -1475,9 +1475,6 @@
   </si>
   <si>
     <t>pcm</t>
-  </si>
-  <si>
-    <t>tank_block</t>
   </si>
   <si>
     <t>slag_concrete</t>
@@ -2901,10 +2898,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>机床灯光</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>冶炼炉灯光</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2943,6 +2936,22 @@
   <si>
     <t>四个按钮（依次为线、杆、板、管）、开关灯光</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>集装箱</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>container</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>拥有8个格子，每个格子可以存放同类物品4096个</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>tank_block</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3077,7 +3086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3169,6 +3178,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3449,8 +3461,8 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E2" sqref="E2:E19"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3540,7 +3552,7 @@
         <v>14</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
@@ -3552,7 +3564,7 @@
         <v>16</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -3596,7 +3608,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
@@ -3608,7 +3620,7 @@
         <v>25</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -3652,7 +3664,7 @@
         <v>32</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
@@ -3664,7 +3676,7 @@
         <v>34</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -3708,7 +3720,7 @@
         <v>41</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>467</v>
+        <v>830</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -3720,7 +3732,7 @@
         <v>43</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -3758,7 +3770,7 @@
         <v>49</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
@@ -3770,7 +3782,7 @@
         <v>51</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -3802,7 +3814,7 @@
         <v>56</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
@@ -3814,7 +3826,7 @@
         <v>58</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -3858,7 +3870,7 @@
         <v>65</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3887,10 +3899,10 @@
         <v>455</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="N9" t="s">
         <v>70</v>
@@ -3902,7 +3914,7 @@
         <v>71</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3931,14 +3943,14 @@
         <v>444</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3970,7 +3982,7 @@
         <v>81</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -4002,7 +4014,7 @@
         <v>86</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -4355,109 +4367,109 @@
         <v>138</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>140</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>141</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>144</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>145</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>146</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="T2" s="8" t="s">
         <v>199</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="V2" s="13" t="s">
+        <v>721</v>
+      </c>
+      <c r="W2" s="11" t="s">
         <v>722</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>723</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>149</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
       </c>
       <c r="AC2" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AD2" s="8" t="s">
         <v>151</v>
       </c>
       <c r="AE2" s="11" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AF2" s="8" t="s">
         <v>152</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AH2" s="8" t="s">
         <v>153</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AJ2" s="8" t="s">
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4468,109 +4480,109 @@
         <v>155</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>157</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>158</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>159</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>160</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>161</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>162</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>163</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>261</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>218</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="X3" s="8" t="s">
         <v>166</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="AD3" s="8" t="s">
         <v>169</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AF3" s="8" t="s">
         <v>170</v>
       </c>
       <c r="AG3" s="11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AH3" s="8" t="s">
         <v>171</v>
       </c>
       <c r="AI3" s="11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AJ3" s="8" t="s">
         <v>172</v>
       </c>
       <c r="AK3" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -4581,109 +4593,109 @@
         <v>173</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>175</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>176</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>177</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>178</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>179</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>180</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>181</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>147</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>148</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="X4" s="8" t="s">
         <v>183</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>184</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AB4" s="8" t="s">
         <v>185</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AD4" s="8" t="s">
         <v>186</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AF4" s="8" t="s">
         <v>187</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AH4" t="s">
         <v>188</v>
       </c>
       <c r="AI4" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AJ4" s="8" t="s">
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4694,109 +4706,109 @@
         <v>190</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>191</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>192</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>193</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>194</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>196</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>197</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>198</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>247</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="V5" s="8" t="s">
         <v>200</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="X5" s="8" t="s">
         <v>201</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="Z5" s="8" t="s">
         <v>202</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="AB5" s="8" t="s">
         <v>203</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AD5" s="8" t="s">
         <v>204</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="AF5" s="9" t="s">
         <v>205</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AH5" t="s">
         <v>206</v>
       </c>
       <c r="AI5" s="11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AJ5" s="8" t="s">
         <v>207</v>
       </c>
       <c r="AK5" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -4807,103 +4819,103 @@
         <v>208</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>209</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>210</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>211</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>212</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>213</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>214</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>215</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>216</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>164</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>165</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>219</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="Z6" s="8" t="s">
         <v>220</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AB6" s="8" t="s">
         <v>221</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AD6" s="8" t="s">
         <v>222</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AF6" s="8" t="s">
         <v>223</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AJ6" s="8" t="s">
         <v>224</v>
       </c>
       <c r="AK6" s="11" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -4914,37 +4926,37 @@
         <v>225</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>226</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>227</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>228</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>229</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>230</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -4952,19 +4964,19 @@
         <v>231</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>232</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>182</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
@@ -4972,31 +4984,31 @@
         <v>234</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="Z7" s="8" t="s">
         <v>235</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AB7" s="8" t="s">
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
       </c>
       <c r="AG7" s="11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AJ7" s="8" t="s">
         <v>238</v>
       </c>
       <c r="AK7" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -5007,37 +5019,37 @@
         <v>239</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>240</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>241</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>242</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>243</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>244</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
@@ -5045,19 +5057,19 @@
         <v>245</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>246</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="T8" s="8" t="s">
         <v>233</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="11"/>
@@ -5065,31 +5077,31 @@
         <v>248</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="Z8" s="8" t="s">
         <v>249</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AB8" s="8" t="s">
         <v>250</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AF8" s="8" t="s">
         <v>251</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AJ8" s="8" t="s">
         <v>252</v>
       </c>
       <c r="AK8" s="11" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5100,37 +5112,37 @@
         <v>253</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>254</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>255</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>256</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>257</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>258</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
@@ -5138,19 +5150,19 @@
         <v>259</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>260</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
@@ -5158,31 +5170,31 @@
         <v>262</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="Z9" s="8" t="s">
         <v>263</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AB9" s="8" t="s">
         <v>264</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AF9" s="8" t="s">
         <v>265</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AJ9" s="8" t="s">
         <v>266</v>
       </c>
       <c r="AK9" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5193,37 +5205,37 @@
         <v>267</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>268</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>269</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>270</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>271</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>272</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -5231,19 +5243,19 @@
         <v>273</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>274</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="T10" s="8" t="s">
         <v>217</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
@@ -5251,31 +5263,31 @@
         <v>275</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="Z10" s="8" t="s">
         <v>276</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AB10" s="8" t="s">
         <v>277</v>
       </c>
       <c r="AC10" s="11" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AF10" s="8" t="s">
         <v>278</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AJ10" s="8" t="s">
         <v>279</v>
       </c>
       <c r="AK10" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5286,37 +5298,37 @@
         <v>280</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>281</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>282</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>284</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>285</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
@@ -5324,19 +5336,19 @@
         <v>286</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>287</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
@@ -5344,13 +5356,13 @@
         <v>288</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="Z11" s="8" t="s">
         <v>289</v>
       </c>
       <c r="AA11" s="11" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AB11" s="8"/>
       <c r="AC11" s="8"/>
@@ -5358,13 +5370,13 @@
         <v>290</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AJ11" s="8" t="s">
         <v>291</v>
       </c>
       <c r="AK11" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5375,37 +5387,37 @@
         <v>292</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>293</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>294</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>295</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>296</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>297</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
@@ -5415,7 +5427,7 @@
         <v>298</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
@@ -5423,13 +5435,13 @@
         <v>299</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Z12" s="8" t="s">
         <v>300</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
@@ -5437,13 +5449,13 @@
         <v>301</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AJ12" s="8" t="s">
         <v>302</v>
       </c>
       <c r="AK12" s="11" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5454,37 +5466,37 @@
         <v>303</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>304</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>305</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>306</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>308</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -5503,16 +5515,16 @@
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AF13" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="AG13" s="11" t="s">
         <v>720</v>
-      </c>
-      <c r="AG13" s="11" t="s">
-        <v>721</v>
       </c>
       <c r="AJ13" s="8" t="s">
         <v>309</v>
       </c>
       <c r="AK13" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -5523,31 +5535,31 @@
         <v>310</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>311</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>312</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>313</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>314</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -5572,7 +5584,7 @@
         <v>315</v>
       </c>
       <c r="AK14" s="11" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -5587,19 +5599,19 @@
         <v>316</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>317</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>318</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -5623,7 +5635,7 @@
         <v>319</v>
       </c>
       <c r="AK15" s="11" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -5638,19 +5650,19 @@
         <v>320</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>321</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>322</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -5674,7 +5686,7 @@
         <v>323</v>
       </c>
       <c r="AK16" s="11" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -5689,19 +5701,19 @@
         <v>324</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>325</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>326</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -5722,10 +5734,10 @@
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
       <c r="AJ17" s="13" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AK17" s="11" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -5740,19 +5752,19 @@
         <v>327</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>328</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>329</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -5773,10 +5785,10 @@
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
       <c r="AJ18" s="13" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AK18" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -5791,19 +5803,19 @@
         <v>330</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>331</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>332</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -5824,10 +5836,10 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AJ19" s="13" t="s">
+        <v>732</v>
+      </c>
+      <c r="AK19" s="11" t="s">
         <v>733</v>
-      </c>
-      <c r="AK19" s="11" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5842,13 +5854,13 @@
         <v>333</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>334</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -5871,10 +5883,10 @@
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
       <c r="AJ20" s="13" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AK20" s="11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -5889,13 +5901,13 @@
         <v>335</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>336</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -5918,10 +5930,10 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AJ21" s="13" t="s">
+        <v>685</v>
+      </c>
+      <c r="AK21" s="11" t="s">
         <v>686</v>
-      </c>
-      <c r="AK21" s="11" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -5938,7 +5950,7 @@
         <v>337</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -5961,10 +5973,10 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AJ22" s="13" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AK22" s="12" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -5981,7 +5993,7 @@
         <v>338</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -6004,10 +6016,10 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AJ23" s="13" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AK23" s="12" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6024,7 +6036,7 @@
         <v>339</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -6047,10 +6059,10 @@
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
       <c r="AJ24" s="20" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AK24" s="12" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6067,7 +6079,7 @@
         <v>340</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -6090,10 +6102,10 @@
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
       <c r="AJ25" s="34" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AK25" s="12" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6110,7 +6122,7 @@
         <v>341</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -6133,10 +6145,10 @@
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
       <c r="AJ26" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="AK26" s="12" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6169,10 +6181,10 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AJ27" s="20" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="AK27" s="12" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6205,10 +6217,10 @@
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AJ28" s="24" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="AK28" s="12" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -6221,10 +6233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6241,7 +6253,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6264,10 +6276,10 @@
         <v>345</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6285,7 +6297,7 @@
         <v>350</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6296,10 +6308,10 @@
         <v>351</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6310,10 +6322,10 @@
         <v>352</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6324,10 +6336,10 @@
         <v>353</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6338,22 +6350,22 @@
         <v>354</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>734</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>736</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>737</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6361,13 +6373,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6376,7 +6388,7 @@
         <v>356</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6384,13 +6396,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E9" t="s">
         <v>357</v>
@@ -6404,10 +6416,10 @@
         <v>358</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E10" t="s">
         <v>359</v>
@@ -6418,13 +6430,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E11" t="s">
         <v>360</v>
@@ -6441,13 +6453,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E12" t="s">
         <v>363</v>
@@ -6458,13 +6470,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6472,13 +6484,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6502,7 +6514,7 @@
         <v>365</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6513,10 +6525,10 @@
         <v>366</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E15" t="s">
         <v>367</v>
@@ -6530,10 +6542,10 @@
         <v>368</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E16" t="s">
         <v>369</v>
@@ -6568,16 +6580,16 @@
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6585,20 +6597,20 @@
         <v>2</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="6" t="s">
         <v>375</v>
       </c>
       <c r="G20" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -6606,17 +6618,17 @@
         <v>3</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="26" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G21" t="s">
         <v>376</v>
@@ -6627,19 +6639,19 @@
         <v>4</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="G22" t="s">
         <v>377</v>
@@ -6653,10 +6665,10 @@
         <v>378</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="25"/>
@@ -6669,17 +6681,17 @@
         <v>6</v>
       </c>
       <c r="B24" s="28" t="s">
+        <v>749</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>705</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>750</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>706</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>751</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="25" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -6687,25 +6699,25 @@
         <v>7</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
@@ -6713,16 +6725,16 @@
         <v>8</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D26" s="18" t="s">
+        <v>772</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>773</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>774</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>380</v>
@@ -6736,15 +6748,15 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="25" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>382</v>
@@ -6755,13 +6767,13 @@
         <v>10</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="25"/>
@@ -6773,19 +6785,17 @@
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="30" t="s">
-        <v>826</v>
+      <c r="B29" s="35" t="s">
+        <v>824</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E29" s="17"/>
-      <c r="F29" s="25" t="s">
-        <v>818</v>
-      </c>
+      <c r="F29" s="25"/>
       <c r="G29" s="7" t="s">
         <v>384</v>
       </c>
@@ -6795,20 +6805,20 @@
         <v>12</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>385</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="25" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6819,13 +6829,13 @@
         <v>386</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>387</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F31" t="s">
         <v>388</v>
@@ -6836,16 +6846,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>389</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6853,16 +6863,30 @@
         <v>15</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>16</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>827</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>828</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -6896,7 +6920,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -6922,7 +6946,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6930,7 +6954,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6938,7 +6962,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6946,7 +6970,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -6954,7 +6978,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6962,7 +6986,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6970,7 +6994,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -6978,7 +7002,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -6986,7 +7010,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.8.14 22.06 for crusher
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C9A7C-2DA3-4293-A2F1-99CA84BB0EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7079DD3-8729-4D84-89D0-8E2A8D080929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="3000" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3086,7 +3086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3182,6 +3182,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6235,8 +6238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6638,7 +6641,7 @@
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="38" t="s">
         <v>767</v>
       </c>
       <c r="C22" s="11" t="s">

</xml_diff>

<commit_message>
2021.8.22 14.42 for thickener
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7079DD3-8729-4D84-89D0-8E2A8D080929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57577531-C430-413B-BB37-2AE196DD4E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="3000" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2232,10 +2232,6 @@
   </si>
   <si>
     <t>crusher</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>concentrating_machine</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -2794,10 +2790,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>电磁选矿机（无gui</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>熔炉和高炉不可以烧铁矿石、金矿石、铜矿石</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2891,10 +2883,6 @@
   </si>
   <si>
     <t>高炉灯光</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>选矿机灯光</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -2952,6 +2940,17 @@
   <si>
     <t>tank_block</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>浓密机（无gui</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>thickener</t>
+  </si>
+  <si>
+    <t>耙架旋转</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3086,7 +3085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3162,12 +3161,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3184,6 +3177,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3723,7 +3719,7 @@
         <v>41</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -3873,7 +3869,7 @@
         <v>65</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="R8" t="s">
         <v>66</v>
@@ -3917,7 +3913,7 @@
         <v>71</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="R9" t="s">
         <v>114</v>
@@ -3946,14 +3942,14 @@
         <v>444</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="O10" s="15"/>
       <c r="P10" t="s">
         <v>76</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="R10" t="s">
         <v>72</v>
@@ -3985,7 +3981,7 @@
         <v>81</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R11" t="s">
         <v>77</v>
@@ -4017,7 +4013,7 @@
         <v>86</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="R12" t="s">
         <v>82</v>
@@ -4394,7 +4390,7 @@
         <v>142</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>143</v>
@@ -4427,10 +4423,10 @@
         <v>610</v>
       </c>
       <c r="V2" s="13" t="s">
+        <v>720</v>
+      </c>
+      <c r="W2" s="11" t="s">
         <v>721</v>
-      </c>
-      <c r="W2" s="11" t="s">
-        <v>722</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>149</v>
@@ -4442,7 +4438,7 @@
         <v>150</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="AB2" s="8" t="s">
         <v>133</v>
@@ -4472,7 +4468,7 @@
         <v>154</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4555,7 +4551,7 @@
         <v>167</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="AB3" s="8" t="s">
         <v>168</v>
@@ -4698,7 +4694,7 @@
         <v>189</v>
       </c>
       <c r="AK4" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -4999,7 +4995,7 @@
         <v>236</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AF7" s="8" t="s">
         <v>237</v>
@@ -5162,10 +5158,10 @@
         <v>557</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
@@ -5348,10 +5344,10 @@
         <v>559</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
@@ -5518,10 +5514,10 @@
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AF13" s="9" t="s">
+        <v>718</v>
+      </c>
+      <c r="AG13" s="11" t="s">
         <v>719</v>
-      </c>
-      <c r="AG13" s="11" t="s">
-        <v>720</v>
       </c>
       <c r="AJ13" s="8" t="s">
         <v>309</v>
@@ -5839,10 +5835,10 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AJ19" s="13" t="s">
+        <v>731</v>
+      </c>
+      <c r="AK19" s="11" t="s">
         <v>732</v>
-      </c>
-      <c r="AK19" s="11" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -5976,10 +5972,10 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AJ22" s="13" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AK22" s="12" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -6019,10 +6015,10 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AJ23" s="13" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AK23" s="12" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6062,10 +6058,10 @@
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
       <c r="AJ24" s="20" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AK24" s="12" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6104,11 +6100,11 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AJ25" s="34" t="s">
-        <v>777</v>
+      <c r="AJ25" s="32" t="s">
+        <v>776</v>
       </c>
       <c r="AK25" s="12" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6148,10 +6144,10 @@
       <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
       <c r="AJ26" s="20" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="AK26" s="12" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6184,10 +6180,10 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AJ27" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="AK27" s="12" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6220,10 +6216,10 @@
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AJ28" s="24" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="AK28" s="12" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
   </sheetData>
@@ -6238,8 +6234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6256,7 +6252,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6282,7 +6278,7 @@
         <v>690</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E3" t="s">
         <v>346</v>
@@ -6300,7 +6296,7 @@
         <v>350</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6314,7 +6310,7 @@
         <v>691</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6328,7 +6324,7 @@
         <v>692</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6342,7 +6338,7 @@
         <v>687</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6356,19 +6352,19 @@
         <v>688</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E7" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>734</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>735</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>736</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6376,13 +6372,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>689</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E8" t="s">
         <v>355</v>
@@ -6391,7 +6387,7 @@
         <v>356</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6399,13 +6395,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>693</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E9" t="s">
         <v>357</v>
@@ -6422,7 +6418,7 @@
         <v>694</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E10" t="s">
         <v>359</v>
@@ -6433,13 +6429,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>695</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E11" t="s">
         <v>360</v>
@@ -6456,13 +6452,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>696</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E12" t="s">
         <v>363</v>
@@ -6473,13 +6469,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>697</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6487,13 +6483,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>698</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E14" t="s">
         <v>134</v>
@@ -6517,7 +6513,7 @@
         <v>365</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6531,7 +6527,7 @@
         <v>699</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E15" t="s">
         <v>367</v>
@@ -6548,7 +6544,7 @@
         <v>700</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E16" t="s">
         <v>369</v>
@@ -6583,16 +6579,16 @@
         <v>374</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -6600,38 +6596,38 @@
         <v>2</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="6" t="s">
         <v>375</v>
       </c>
       <c r="G20" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="35" t="s">
-        <v>768</v>
+      <c r="B21" s="33" t="s">
+        <v>767</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>703</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="26" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G21" t="s">
         <v>376</v>
@@ -6641,20 +6637,20 @@
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="38" t="s">
-        <v>767</v>
+      <c r="B22" s="36" t="s">
+        <v>766</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>704</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G22" t="s">
         <v>377</v>
@@ -6664,14 +6660,14 @@
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="34" t="s">
         <v>378</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="25"/>
@@ -6684,60 +6680,60 @@
         <v>6</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>705</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="25" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="33" t="s">
-        <v>822</v>
+      <c r="B25" s="31" t="s">
+        <v>819</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>706</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>764</v>
+      <c r="B26" s="37" t="s">
+        <v>763</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>707</v>
       </c>
       <c r="D26" s="18" t="s">
+        <v>771</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>772</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>773</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>380</v>
@@ -6750,16 +6746,16 @@
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="31" t="s">
-        <v>791</v>
+      <c r="B27" s="36" t="s">
+        <v>828</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>708</v>
+        <v>829</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="25" t="s">
-        <v>816</v>
+        <v>830</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>382</v>
@@ -6769,14 +6765,14 @@
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="35" t="s">
-        <v>823</v>
+      <c r="B28" s="33" t="s">
+        <v>820</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="25"/>
@@ -6788,14 +6784,14 @@
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="35" t="s">
-        <v>824</v>
+      <c r="B29" s="33" t="s">
+        <v>821</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="25"/>
@@ -6808,20 +6804,20 @@
         <v>12</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>385</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="25" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
@@ -6832,13 +6828,13 @@
         <v>386</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>387</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F31" t="s">
         <v>388</v>
@@ -6849,7 +6845,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>701</v>
@@ -6858,7 +6854,7 @@
         <v>389</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -6866,13 +6862,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>702</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>390</v>
@@ -6882,14 +6878,14 @@
       <c r="A34" s="2">
         <v>16</v>
       </c>
-      <c r="B34" s="37" t="s">
-        <v>827</v>
+      <c r="B34" s="35" t="s">
+        <v>824</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
   </sheetData>
@@ -6923,7 +6919,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>
@@ -6949,7 +6945,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6957,7 +6953,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6965,7 +6961,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6973,7 +6969,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -6981,7 +6977,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -6989,7 +6985,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6997,7 +6993,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -7005,7 +7001,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7013,7 +7009,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.8.28 21.05 for 真空合金炉
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57577531-C430-413B-BB37-2AE196DD4E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B96A5-BAA1-4C5E-ACA1-C545FBA1A7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="3000" windowWidth="19200" windowHeight="10060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -3085,7 +3085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3156,9 +3156,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6100,7 +6097,7 @@
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AJ25" s="32" t="s">
+      <c r="AJ25" s="31" t="s">
         <v>776</v>
       </c>
       <c r="AK25" s="12" t="s">
@@ -6234,8 +6231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6616,7 +6613,7 @@
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>767</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -6637,7 +6634,7 @@
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>766</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -6660,7 +6657,7 @@
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>378</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -6697,7 +6694,7 @@
       <c r="A25" s="2">
         <v>7</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="30" t="s">
         <v>819</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -6723,7 +6720,7 @@
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>763</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -6746,7 +6743,7 @@
       <c r="A27" s="2">
         <v>9</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="35" t="s">
         <v>828</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -6765,7 +6762,7 @@
       <c r="A28" s="2">
         <v>10</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>820</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -6784,7 +6781,7 @@
       <c r="A29" s="2">
         <v>11</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="32" t="s">
         <v>821</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -6803,7 +6800,7 @@
       <c r="A30" s="2">
         <v>12</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="32" t="s">
         <v>822</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -6861,7 +6858,7 @@
       <c r="A33" s="2">
         <v>15</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="32" t="s">
         <v>765</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -6878,7 +6875,7 @@
       <c r="A34" s="2">
         <v>16</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="34" t="s">
         <v>824</v>
       </c>
       <c r="C34" s="11" t="s">

</xml_diff>

<commit_message>
2021.9.25 13.03 for 修正电力高炉gui的bug
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DF7072-E37D-4D07-8C54-8AF6735F7CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD619E5-2631-4C6E-930A-E6529ABF6B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="881">
   <si>
     <t>矿石</t>
   </si>
@@ -3120,6 +3120,14 @@
   <si>
     <t>钛镍下界合金</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>漏斗可以从机器中的输出格中取出物品；漏斗可以向机器的输入格中输入物品</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>传送带端点在无过滤器时行为和漏斗一致，有过滤器时，可以访问机器的所有库存</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3306,7 +3314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3417,6 +3425,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6683,8 +6694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7455,10 +7466,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07120975-DCD2-44DB-890E-43FB0017A6EE}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7631,7 +7642,15 @@
       <c r="D13" s="13" t="s">
         <v>865</v>
       </c>
+      <c r="F13" s="45" t="s">
+        <v>879</v>
+      </c>
       <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+      <c r="F14" s="45" t="s">
+        <v>880</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
2021.9.27 19.16 for 锻造机合成
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252B85B8-287B-4468-8C07-8B4C3CA124FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AE444D-ED50-4C4C-A604-34A76B4C3941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1698,9 +1698,6 @@
     <t>stick_iron</t>
   </si>
   <si>
-    <t>circle_casting_bronze</t>
-  </si>
-  <si>
     <t>circle_casting_steel</t>
   </si>
   <si>
@@ -1729,57 +1726,9 @@
     <t>circle_casting_tungsten_steel</t>
   </si>
   <si>
-    <t>circle_casting_titanium</t>
-  </si>
-  <si>
-    <t>plate_tin</t>
-  </si>
-  <si>
-    <t>plate_bronze</t>
-  </si>
-  <si>
-    <t>plate_steel</t>
-  </si>
-  <si>
-    <t>plate_invar</t>
-  </si>
-  <si>
-    <t>plate_ss</t>
-  </si>
-  <si>
-    <t>plate_tungsten_steel</t>
-  </si>
-  <si>
     <t>plate_hss</t>
   </si>
   <si>
-    <t>plate_gold</t>
-  </si>
-  <si>
-    <t>plate_silver</t>
-  </si>
-  <si>
-    <t>plate_chromium</t>
-  </si>
-  <si>
-    <t>plate_nickel</t>
-  </si>
-  <si>
-    <t>plate_titanium</t>
-  </si>
-  <si>
-    <t>plate_aluminum</t>
-  </si>
-  <si>
-    <t>plate_ncalloy</t>
-  </si>
-  <si>
-    <t>plate_silicon</t>
-  </si>
-  <si>
-    <t>plate_iron</t>
-  </si>
-  <si>
     <t>plate_pe</t>
   </si>
   <si>
@@ -1858,12 +1807,6 @@
     <t>refined_slag_titanium</t>
   </si>
   <si>
-    <t>axis_bronze</t>
-  </si>
-  <si>
-    <t>axis_invar</t>
-  </si>
-  <si>
     <t>axis_ss</t>
   </si>
   <si>
@@ -1871,15 +1814,6 @@
   </si>
   <si>
     <t>axis_hss</t>
-  </si>
-  <si>
-    <t>axis_steel</t>
-  </si>
-  <si>
-    <t>axis_titanium</t>
-  </si>
-  <si>
-    <t>axis_iron</t>
   </si>
   <si>
     <t>gear_blank_invar</t>
@@ -2217,15 +2151,7 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>铬轴</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>钴轴</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>axis_chromium</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -3145,6 +3071,102 @@
   <si>
     <t>bellow</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>高速钢圆形铸件</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_titanium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_hss</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_bronze</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_bronze</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_steel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_iron</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_invar</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>axis_titanium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_tin</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_bronze</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_steel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_ss</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_nickel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_invar</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_tungsten_steel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_silver</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_chromium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_titanium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_aluminum</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_ncalloy</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_gold</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_iron</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>plate_silicon</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3336,7 +3358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3453,6 +3475,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3921,7 +3946,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N12" sqref="N12"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4005,7 +4030,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>876</v>
+        <v>852</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -4017,13 +4042,13 @@
         <v>15</v>
       </c>
       <c r="O2" s="46" t="s">
-        <v>875</v>
+        <v>851</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>842</v>
+        <v>818</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -4073,13 +4098,13 @@
         <v>24</v>
       </c>
       <c r="O3" s="46" t="s">
-        <v>877</v>
+        <v>853</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>842</v>
+        <v>818</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -4123,19 +4148,19 @@
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>880</v>
+        <v>856</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>879</v>
+        <v>855</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>842</v>
+        <v>818</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -4179,19 +4204,19 @@
         <v>41</v>
       </c>
       <c r="M5" s="46" t="s">
-        <v>751</v>
+        <v>727</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="46" t="s">
-        <v>872</v>
+        <v>848</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>843</v>
+        <v>819</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -4229,7 +4254,7 @@
         <v>49</v>
       </c>
       <c r="M6" s="46" t="s">
-        <v>868</v>
+        <v>844</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
@@ -4241,7 +4266,7 @@
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>844</v>
+        <v>820</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -4285,7 +4310,7 @@
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>845</v>
+        <v>821</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -4314,7 +4339,7 @@
         <v>438</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>874</v>
+        <v>850</v>
       </c>
       <c r="M8" s="46" t="s">
         <v>457</v>
@@ -4329,7 +4354,7 @@
         <v>64</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>687</v>
+        <v>663</v>
       </c>
       <c r="R8" t="s">
         <v>65</v>
@@ -4373,7 +4398,7 @@
         <v>70</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>688</v>
+        <v>664</v>
       </c>
       <c r="R9" t="s">
         <v>113</v>
@@ -4402,16 +4427,16 @@
         <v>439</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>712</v>
+        <v>688</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>881</v>
+        <v>857</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>689</v>
+        <v>665</v>
       </c>
       <c r="R10" t="s">
         <v>71</v>
@@ -4443,7 +4468,7 @@
         <v>80</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>690</v>
+        <v>666</v>
       </c>
       <c r="R11" t="s">
         <v>76</v>
@@ -4475,7 +4500,7 @@
         <v>85</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>691</v>
+        <v>667</v>
       </c>
       <c r="R12" t="s">
         <v>81</v>
@@ -4504,10 +4529,10 @@
         <v>444</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>846</v>
+        <v>822</v>
       </c>
       <c r="Q13" s="46" t="s">
-        <v>847</v>
+        <v>823</v>
       </c>
       <c r="R13" t="s">
         <v>93</v>
@@ -4728,8 +4753,8 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC15" sqref="AC15"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4835,13 +4860,13 @@
         <v>137</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>607</v>
+        <v>585</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>625</v>
+        <v>603</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
@@ -4859,7 +4884,7 @@
         <v>141</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>741</v>
+        <v>717</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>142</v>
@@ -4871,55 +4896,49 @@
         <v>143</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>869</v>
+        <v>845</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>870</v>
+        <v>846</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>527</v>
+        <v>861</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>585</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>681</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>682</v>
+        <v>862</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>873</v>
+        <v>849</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
       </c>
       <c r="AA2" s="46" t="s">
-        <v>744</v>
+        <v>720</v>
       </c>
       <c r="AB2" s="5" t="s">
         <v>132</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>572</v>
+        <v>555</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>150</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>620</v>
+        <v>598</v>
       </c>
       <c r="AF2" s="5" t="s">
         <v>151</v>
@@ -4937,7 +4956,7 @@
         <v>153</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>743</v>
+        <v>719</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4948,13 +4967,13 @@
         <v>154</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>608</v>
+        <v>586</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>155</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>626</v>
+        <v>604</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>156</v>
@@ -4972,7 +4991,7 @@
         <v>158</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>538</v>
+        <v>867</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
@@ -4984,55 +5003,55 @@
         <v>160</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>161</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>559</v>
+        <v>542</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>162</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>260</v>
+        <v>198</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>581</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>217</v>
+        <v>863</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>659</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>568</v>
+        <v>660</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>165</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>606</v>
+        <v>584</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>166</v>
       </c>
       <c r="AA3" s="46" t="s">
-        <v>745</v>
+        <v>721</v>
       </c>
       <c r="AB3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>574</v>
+        <v>557</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>621</v>
+        <v>599</v>
       </c>
       <c r="AF3" s="5" t="s">
         <v>169</v>
@@ -5050,7 +5069,7 @@
         <v>171</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>644</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -5061,13 +5080,13 @@
         <v>172</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>609</v>
+        <v>587</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>627</v>
+        <v>605</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
@@ -5085,7 +5104,7 @@
         <v>176</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>539</v>
+        <v>868</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
@@ -5097,55 +5116,49 @@
         <v>178</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>179</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>567</v>
+        <v>550</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>180</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>146</v>
+        <v>232</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>582</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>569</v>
+        <v>864</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>182</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>604</v>
+        <v>582</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>183</v>
       </c>
       <c r="AA4" s="46" t="s">
-        <v>595</v>
+        <v>573</v>
       </c>
       <c r="AB4" s="5" t="s">
         <v>184</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>575</v>
+        <v>558</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>185</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>622</v>
+        <v>600</v>
       </c>
       <c r="AF4" s="5" t="s">
         <v>186</v>
@@ -5163,7 +5176,7 @@
         <v>188</v>
       </c>
       <c r="AK4" s="8" t="s">
-        <v>739</v>
+        <v>715</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -5174,13 +5187,13 @@
         <v>189</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>610</v>
+        <v>588</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>628</v>
+        <v>606</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>191</v>
@@ -5198,7 +5211,7 @@
         <v>193</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>540</v>
+        <v>869</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>194</v>
@@ -5210,55 +5223,43 @@
         <v>195</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>196</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>560</v>
+        <v>543</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>197</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>583</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>570</v>
+        <v>529</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>200</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>600</v>
+        <v>578</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>201</v>
       </c>
       <c r="AA5" s="46" t="s">
-        <v>591</v>
+        <v>569</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>202</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>576</v>
+        <v>559</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>203</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>623</v>
+        <v>601</v>
       </c>
       <c r="AF5" s="41" t="s">
         <v>204</v>
@@ -5276,7 +5277,7 @@
         <v>206</v>
       </c>
       <c r="AK5" s="46" t="s">
-        <v>645</v>
+        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -5287,13 +5288,13 @@
         <v>207</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>611</v>
+        <v>589</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>629</v>
+        <v>607</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>209</v>
@@ -5311,7 +5312,7 @@
         <v>211</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>542</v>
+        <v>870</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>212</v>
@@ -5323,55 +5324,55 @@
         <v>213</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>214</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>566</v>
+        <v>549</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>215</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>163</v>
+        <v>260</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>584</v>
+        <v>865</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>218</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>597</v>
+        <v>575</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>219</v>
       </c>
       <c r="AA6" s="46" t="s">
-        <v>588</v>
+        <v>566</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>220</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>573</v>
+        <v>556</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>221</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>624</v>
+        <v>602</v>
       </c>
       <c r="AF6" s="5" t="s">
         <v>222</v>
@@ -5383,7 +5384,7 @@
         <v>223</v>
       </c>
       <c r="AK6" s="46" t="s">
-        <v>646</v>
+        <v>624</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -5394,13 +5395,13 @@
         <v>224</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>612</v>
+        <v>590</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>225</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>631</v>
+        <v>609</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>226</v>
@@ -5418,7 +5419,7 @@
         <v>228</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>548</v>
+        <v>871</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>229</v>
@@ -5432,19 +5433,13 @@
         <v>230</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>561</v>
+        <v>544</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>231</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>532</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>580</v>
+        <v>531</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
@@ -5452,19 +5447,19 @@
         <v>233</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>605</v>
+        <v>583</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>234</v>
       </c>
       <c r="AA7" s="46" t="s">
-        <v>596</v>
+        <v>574</v>
       </c>
       <c r="AB7" s="5" t="s">
         <v>235</v>
       </c>
       <c r="AC7" s="46" t="s">
-        <v>740</v>
+        <v>716</v>
       </c>
       <c r="AF7" s="5" t="s">
         <v>236</v>
@@ -5476,7 +5471,7 @@
         <v>237</v>
       </c>
       <c r="AK7" s="8" t="s">
-        <v>647</v>
+        <v>625</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -5487,13 +5482,13 @@
         <v>238</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>613</v>
+        <v>591</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>239</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>632</v>
+        <v>610</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>240</v>
@@ -5511,7 +5506,7 @@
         <v>242</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>541</v>
+        <v>872</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>243</v>
@@ -5525,19 +5520,19 @@
         <v>244</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>562</v>
+        <v>545</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>245</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>587</v>
+        <v>532</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>662</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="8"/>
@@ -5545,19 +5540,19 @@
         <v>247</v>
       </c>
       <c r="Y8" s="8" t="s">
-        <v>603</v>
+        <v>581</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>248</v>
       </c>
       <c r="AA8" s="46" t="s">
-        <v>594</v>
+        <v>572</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>249</v>
       </c>
       <c r="AC8" s="46" t="s">
-        <v>578</v>
+        <v>561</v>
       </c>
       <c r="AF8" s="5" t="s">
         <v>250</v>
@@ -5569,7 +5564,7 @@
         <v>251</v>
       </c>
       <c r="AK8" s="8" t="s">
-        <v>871</v>
+        <v>847</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5580,13 +5575,13 @@
         <v>252</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>614</v>
+        <v>592</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>633</v>
+        <v>611</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>254</v>
@@ -5604,7 +5599,7 @@
         <v>256</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>543</v>
+        <v>873</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>257</v>
@@ -5618,19 +5613,13 @@
         <v>258</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>563</v>
+        <v>546</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>259</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>683</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>685</v>
+        <v>533</v>
       </c>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
@@ -5638,19 +5627,19 @@
         <v>261</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>601</v>
+        <v>579</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>262</v>
       </c>
       <c r="AA9" s="46" t="s">
-        <v>592</v>
+        <v>570</v>
       </c>
       <c r="AB9" s="5" t="s">
         <v>263</v>
       </c>
       <c r="AC9" s="46" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
       <c r="AF9" s="5" t="s">
         <v>264</v>
@@ -5662,7 +5651,7 @@
         <v>265</v>
       </c>
       <c r="AK9" s="8" t="s">
-        <v>648</v>
+        <v>626</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5673,13 +5662,13 @@
         <v>266</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>615</v>
+        <v>593</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>267</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>634</v>
+        <v>612</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>268</v>
@@ -5691,13 +5680,13 @@
         <v>269</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>857</v>
+        <v>833</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>270</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>271</v>
@@ -5711,39 +5700,43 @@
         <v>272</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>564</v>
+        <v>547</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>273</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>586</v>
-      </c>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
+        <v>563</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>552</v>
+      </c>
       <c r="X10" s="5" t="s">
         <v>274</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>598</v>
+        <v>576</v>
       </c>
       <c r="Z10" s="5" t="s">
         <v>275</v>
       </c>
       <c r="AA10" s="46" t="s">
-        <v>589</v>
+        <v>567</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>276</v>
       </c>
       <c r="AC10" s="46" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
       <c r="AF10" s="5" t="s">
         <v>277</v>
@@ -5755,7 +5748,7 @@
         <v>278</v>
       </c>
       <c r="AK10" s="46" t="s">
-        <v>649</v>
+        <v>627</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5766,13 +5759,13 @@
         <v>279</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>616</v>
+        <v>594</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>635</v>
+        <v>613</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>281</v>
@@ -5790,7 +5783,7 @@
         <v>283</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>546</v>
+        <v>874</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>284</v>
@@ -5804,33 +5797,37 @@
         <v>285</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>565</v>
+        <v>548</v>
       </c>
       <c r="R11" s="5" t="s">
         <v>286</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="T11" s="10" t="s">
-        <v>684</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>686</v>
-      </c>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
+        <v>535</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>553</v>
+      </c>
       <c r="X11" s="5" t="s">
         <v>287</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>599</v>
+        <v>577</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>288</v>
       </c>
       <c r="AA11" s="46" t="s">
-        <v>590</v>
+        <v>568</v>
       </c>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
@@ -5844,7 +5841,7 @@
         <v>290</v>
       </c>
       <c r="AK11" s="46" t="s">
-        <v>650</v>
+        <v>628</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5855,13 +5852,13 @@
         <v>291</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>617</v>
+        <v>595</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>292</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>636</v>
+        <v>614</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>293</v>
@@ -5879,7 +5876,7 @@
         <v>295</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>547</v>
+        <v>875</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>296</v>
@@ -5895,7 +5892,13 @@
         <v>297</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>537</v>
+        <v>859</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>866</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -5903,13 +5906,13 @@
         <v>298</v>
       </c>
       <c r="Y12" s="8" t="s">
-        <v>602</v>
+        <v>580</v>
       </c>
       <c r="Z12" s="5" t="s">
         <v>299</v>
       </c>
       <c r="AA12" s="46" t="s">
-        <v>593</v>
+        <v>571</v>
       </c>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
@@ -5923,7 +5926,7 @@
         <v>301</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>651</v>
+        <v>629</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5934,13 +5937,13 @@
         <v>302</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>619</v>
+        <v>597</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>303</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>630</v>
+        <v>608</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>304</v>
@@ -5952,13 +5955,13 @@
         <v>305</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>856</v>
+        <v>832</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>306</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>549</v>
+        <v>876</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>307</v>
@@ -5970,12 +5973,24 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
+      <c r="R13" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>860</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="W13" s="8" t="s">
+        <v>554</v>
+      </c>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="Z13" s="5"/>
@@ -5983,16 +5998,16 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AF13" s="41" t="s">
-        <v>679</v>
+        <v>657</v>
       </c>
       <c r="AG13" s="46" t="s">
-        <v>680</v>
+        <v>658</v>
       </c>
       <c r="AJ13" s="5" t="s">
         <v>308</v>
       </c>
       <c r="AK13" s="8" t="s">
-        <v>652</v>
+        <v>630</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -6003,13 +6018,13 @@
         <v>309</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>618</v>
+        <v>596</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>637</v>
+        <v>615</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>311</v>
@@ -6021,13 +6036,13 @@
         <v>312</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>855</v>
+        <v>831</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>313</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>550</v>
+        <v>877</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6035,10 +6050,10 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="8"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
@@ -6052,7 +6067,7 @@
         <v>314</v>
       </c>
       <c r="AK14" s="8" t="s">
-        <v>653</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -6079,7 +6094,7 @@
         <v>317</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>551</v>
+        <v>878</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -6087,10 +6102,8 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="9"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
@@ -6103,7 +6116,7 @@
         <v>318</v>
       </c>
       <c r="AK15" s="8" t="s">
-        <v>654</v>
+        <v>632</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -6130,7 +6143,7 @@
         <v>321</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>545</v>
+        <v>879</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -6140,8 +6153,6 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
@@ -6154,7 +6165,7 @@
         <v>322</v>
       </c>
       <c r="AK16" s="46" t="s">
-        <v>655</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -6181,7 +6192,7 @@
         <v>325</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>553</v>
+        <v>880</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -6191,8 +6202,6 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
@@ -6202,10 +6211,10 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AJ17" s="10" t="s">
-        <v>638</v>
+        <v>616</v>
       </c>
       <c r="AK17" s="46" t="s">
-        <v>641</v>
+        <v>619</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -6232,7 +6241,7 @@
         <v>328</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>552</v>
+        <v>881</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -6242,8 +6251,6 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
@@ -6253,10 +6260,10 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AJ18" s="10" t="s">
-        <v>639</v>
+        <v>617</v>
       </c>
       <c r="AK18" s="46" t="s">
-        <v>642</v>
+        <v>620</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -6277,13 +6284,13 @@
         <v>330</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>858</v>
+        <v>834</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>331</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -6304,10 +6311,10 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AJ19" s="10" t="s">
-        <v>692</v>
+        <v>668</v>
       </c>
       <c r="AK19" s="46" t="s">
-        <v>693</v>
+        <v>669</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -6351,10 +6358,10 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AJ20" s="10" t="s">
-        <v>640</v>
+        <v>618</v>
       </c>
       <c r="AK20" s="46" t="s">
-        <v>643</v>
+        <v>621</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -6369,7 +6376,7 @@
         <v>334</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>878</v>
+        <v>854</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>335</v>
@@ -6398,10 +6405,10 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AJ21" s="10" t="s">
-        <v>658</v>
+        <v>636</v>
       </c>
       <c r="AK21" s="46" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -6441,10 +6448,10 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AJ22" s="10" t="s">
-        <v>706</v>
+        <v>682</v>
       </c>
       <c r="AK22" s="46" t="s">
-        <v>709</v>
+        <v>685</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -6461,10 +6468,10 @@
         <v>337</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>656</v>
+        <v>634</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>859</v>
+        <v>835</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -6486,10 +6493,10 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AJ23" s="10" t="s">
-        <v>707</v>
+        <v>683</v>
       </c>
       <c r="AK23" s="46" t="s">
-        <v>710</v>
+        <v>686</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6506,7 +6513,7 @@
         <v>338</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>860</v>
+        <v>836</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -6528,10 +6535,10 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AJ24" s="16" t="s">
-        <v>708</v>
+        <v>684</v>
       </c>
       <c r="AK24" s="46" t="s">
-        <v>711</v>
+        <v>687</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6570,10 +6577,10 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AJ25" s="21" t="s">
-        <v>718</v>
+        <v>694</v>
       </c>
       <c r="AK25" s="9" t="s">
-        <v>722</v>
+        <v>698</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6590,10 +6597,10 @@
         <v>340</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>657</v>
+        <v>635</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>861</v>
+        <v>837</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -6615,10 +6622,10 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AJ26" s="16" t="s">
-        <v>719</v>
+        <v>695</v>
       </c>
       <c r="AK26" s="9" t="s">
-        <v>723</v>
+        <v>699</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6629,11 +6636,11 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="42" t="s">
-        <v>862</v>
+        <v>838</v>
       </c>
       <c r="I27" s="42"/>
       <c r="J27" s="42" t="s">
-        <v>863</v>
+        <v>839</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -6655,10 +6662,10 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AJ27" s="16" t="s">
-        <v>720</v>
+        <v>696</v>
       </c>
       <c r="AK27" s="9" t="s">
-        <v>724</v>
+        <v>700</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6669,11 +6676,11 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="42" t="s">
-        <v>864</v>
+        <v>840</v>
       </c>
       <c r="I28" s="42"/>
       <c r="J28" s="42" t="s">
-        <v>865</v>
+        <v>841</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -6695,18 +6702,18 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AJ28" s="40" t="s">
-        <v>721</v>
+        <v>697</v>
       </c>
       <c r="AK28" s="9" t="s">
-        <v>725</v>
+        <v>701</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ29" s="39" t="s">
-        <v>848</v>
+        <v>824</v>
       </c>
       <c r="AK29" s="9" t="s">
-        <v>849</v>
+        <v>825</v>
       </c>
     </row>
   </sheetData>
@@ -6721,8 +6728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6739,7 +6746,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
-        <v>747</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6762,10 +6769,10 @@
         <v>344</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
       <c r="E3" t="s">
         <v>345</v>
@@ -6783,7 +6790,7 @@
         <v>349</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>678</v>
+        <v>656</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6794,10 +6801,10 @@
         <v>350</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6808,10 +6815,10 @@
         <v>351</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>665</v>
+        <v>643</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6822,10 +6829,10 @@
         <v>352</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>698</v>
+        <v>674</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6836,22 +6843,22 @@
         <v>353</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>699</v>
+        <v>675</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>694</v>
+        <v>670</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>695</v>
+        <v>671</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>696</v>
+        <v>672</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>697</v>
+        <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6859,13 +6866,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>716</v>
+        <v>692</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>662</v>
+        <v>640</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>705</v>
+        <v>681</v>
       </c>
       <c r="E8" t="s">
         <v>354</v>
@@ -6874,7 +6881,7 @@
         <v>355</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>742</v>
+        <v>718</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6882,13 +6889,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>736</v>
+        <v>712</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>666</v>
+        <v>644</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>701</v>
+        <v>677</v>
       </c>
       <c r="E9" t="s">
         <v>356</v>
@@ -6902,10 +6909,10 @@
         <v>357</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>667</v>
+        <v>645</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>702</v>
+        <v>678</v>
       </c>
       <c r="E10" t="s">
         <v>358</v>
@@ -6916,13 +6923,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>715</v>
+        <v>691</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>668</v>
+        <v>646</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>703</v>
+        <v>679</v>
       </c>
       <c r="E11" t="s">
         <v>359</v>
@@ -6939,13 +6946,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>737</v>
+        <v>713</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>704</v>
+        <v>680</v>
       </c>
       <c r="E12" t="s">
         <v>362</v>
@@ -6956,13 +6963,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>746</v>
+        <v>722</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>670</v>
+        <v>648</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>853</v>
+        <v>829</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6970,13 +6977,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>738</v>
+        <v>714</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>700</v>
+        <v>676</v>
       </c>
       <c r="E14" t="s">
         <v>133</v>
@@ -7000,7 +7007,7 @@
         <v>364</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>717</v>
+        <v>693</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7011,10 +7018,10 @@
         <v>365</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>672</v>
+        <v>650</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>714</v>
+        <v>690</v>
       </c>
       <c r="E15" t="s">
         <v>366</v>
@@ -7028,10 +7035,10 @@
         <v>367</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>673</v>
+        <v>651</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>713</v>
+        <v>689</v>
       </c>
       <c r="E16" t="s">
         <v>368</v>
@@ -7066,16 +7073,16 @@
         <v>373</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>760</v>
+        <v>736</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>761</v>
+        <v>737</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>762</v>
+        <v>738</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>763</v>
+        <v>739</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -7088,21 +7095,21 @@
       <c r="A20" s="23">
         <v>2</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>764</v>
+      <c r="B20" s="47" t="s">
+        <v>740</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>765</v>
+        <v>741</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>766</v>
+        <v>742</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="27" t="s">
         <v>374</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>767</v>
+        <v>743</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
@@ -7115,17 +7122,17 @@
         <v>3</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>768</v>
+        <v>744</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>769</v>
+        <v>745</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>770</v>
+        <v>746</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="27" t="s">
-        <v>771</v>
+        <v>747</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>375</v>
@@ -7141,32 +7148,32 @@
         <v>4</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>759</v>
+        <v>735</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>676</v>
+        <v>654</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>772</v>
+        <v>748</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>773</v>
+        <v>749</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>774</v>
+        <v>750</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>376</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="22" t="s">
-        <v>775</v>
+        <v>751</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>776</v>
+        <v>752</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="L22" s="28"/>
     </row>
@@ -7178,10 +7185,10 @@
         <v>377</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>778</v>
+        <v>754</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>779</v>
+        <v>755</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="23"/>
@@ -7189,16 +7196,16 @@
         <v>378</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>780</v>
+        <v>756</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>775</v>
+        <v>751</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>776</v>
+        <v>752</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="L23" s="28"/>
     </row>
@@ -7207,17 +7214,17 @@
         <v>6</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>781</v>
+        <v>757</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>782</v>
+        <v>758</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>783</v>
+        <v>759</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="23" t="s">
-        <v>784</v>
+        <v>760</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -7231,34 +7238,34 @@
         <v>7</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>785</v>
+        <v>761</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>786</v>
+        <v>762</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>787</v>
+        <v>763</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>788</v>
+        <v>764</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>789</v>
+        <v>765</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>790</v>
+        <v>766</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>791</v>
+        <v>767</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>753</v>
+        <v>729</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>754</v>
+        <v>730</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>755</v>
+        <v>731</v>
       </c>
       <c r="L25" s="28"/>
     </row>
@@ -7267,13 +7274,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>792</v>
+        <v>768</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>793</v>
+        <v>769</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>758</v>
+        <v>734</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>386</v>
@@ -7285,19 +7292,19 @@
         <v>380</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>756</v>
+        <v>732</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>757</v>
+        <v>733</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>775</v>
+        <v>751</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>794</v>
+        <v>770</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="117" x14ac:dyDescent="0.3">
@@ -7305,27 +7312,27 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>795</v>
+        <v>771</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>752</v>
+        <v>728</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="23" t="s">
-        <v>796</v>
+        <v>772</v>
       </c>
       <c r="G27" s="32" t="s">
         <v>381</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>775</v>
+        <v>751</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>776</v>
+        <v>752</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
@@ -7335,29 +7342,29 @@
         <v>10</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>797</v>
+        <v>773</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>798</v>
+        <v>774</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>799</v>
+        <v>775</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="23" t="s">
-        <v>800</v>
+        <v>776</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>382</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>775</v>
+        <v>751</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>776</v>
+        <v>752</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
@@ -7367,29 +7374,29 @@
         <v>11</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>801</v>
+        <v>777</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>802</v>
+        <v>778</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>803</v>
+        <v>779</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="23" t="s">
-        <v>804</v>
+        <v>780</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>383</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>775</v>
+        <v>751</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>776</v>
+        <v>752</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>777</v>
+        <v>753</v>
       </c>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
@@ -7399,23 +7406,23 @@
         <v>12</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>805</v>
+        <v>781</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>806</v>
+        <v>782</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>384</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="23" t="s">
-        <v>807</v>
+        <v>783</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>854</v>
+        <v>830</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>811</v>
+        <v>787</v>
       </c>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
@@ -7427,16 +7434,16 @@
         <v>13</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>808</v>
+        <v>784</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>674</v>
+        <v>652</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>385</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>773</v>
+        <v>749</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -7451,13 +7458,13 @@
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>809</v>
+        <v>785</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>810</v>
+        <v>786</v>
       </c>
       <c r="E32" s="34" t="s">
         <v>386</v>
@@ -7475,13 +7482,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>748</v>
+        <v>724</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>749</v>
+        <v>725</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>750</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>
@@ -7515,36 +7522,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>812</v>
+        <v>788</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>813</v>
+        <v>789</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>815</v>
+        <v>791</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>817</v>
+        <v>793</v>
       </c>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>814</v>
+        <v>790</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>816</v>
+        <v>792</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>818</v>
+        <v>794</v>
       </c>
       <c r="G3" s="37">
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>823</v>
+        <v>799</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
@@ -7552,131 +7559,131 @@
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>824</v>
+        <v>800</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D5" s="38" t="s">
-        <v>835</v>
+        <v>811</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>821</v>
+        <v>797</v>
       </c>
       <c r="G5" s="37">
         <v>3</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>825</v>
+        <v>801</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
       <c r="D6" s="38" t="s">
-        <v>836</v>
+        <v>812</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>840</v>
+        <v>816</v>
       </c>
       <c r="G6" s="37">
         <v>4</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>828</v>
+        <v>804</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
-        <v>838</v>
+        <v>814</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>819</v>
+        <v>795</v>
       </c>
       <c r="G7" s="37">
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>826</v>
+        <v>802</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
-        <v>837</v>
+        <v>813</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>820</v>
+        <v>796</v>
       </c>
       <c r="G8" s="37">
         <v>6</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>827</v>
+        <v>803</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="D9" s="38" t="s">
-        <v>839</v>
+        <v>815</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>841</v>
+        <v>817</v>
       </c>
       <c r="G9" s="37">
         <v>7</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>829</v>
+        <v>805</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D10" s="13" t="s">
-        <v>851</v>
+        <v>827</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>832</v>
+        <v>808</v>
       </c>
       <c r="G10" s="37">
         <v>8</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>830</v>
+        <v>806</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="F11" s="13" t="s">
-        <v>822</v>
+        <v>798</v>
       </c>
       <c r="G11" s="37">
         <v>9</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>831</v>
+        <v>807</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D12" s="13" t="s">
-        <v>850</v>
+        <v>826</v>
       </c>
       <c r="G12" s="37">
         <v>10</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>834</v>
+        <v>810</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
-        <v>852</v>
+        <v>828</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>866</v>
+        <v>842</v>
       </c>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="F14" s="44" t="s">
-        <v>867</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -7711,7 +7718,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>726</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -7737,7 +7744,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>727</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7745,7 +7752,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>733</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7753,7 +7760,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>728</v>
+        <v>704</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7761,7 +7768,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>734</v>
+        <v>710</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7769,7 +7776,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>729</v>
+        <v>705</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -7777,7 +7784,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>730</v>
+        <v>706</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7785,7 +7792,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>731</v>
+        <v>707</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -7793,7 +7800,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>732</v>
+        <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7801,7 +7808,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>735</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.9.28 13.21 for 浇注机合成及bug修复
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AE444D-ED50-4C4C-A604-34A76B4C3941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F04A584-27A0-4C4B-A3E5-FA9A97C90FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -65,10 +65,37 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>hqyzsy</author>
     <author>胡清源</author>
   </authors>
   <commentList>
-    <comment ref="AG13" authorId="0" shapeId="0" xr:uid="{E6B9CEB0-A8B1-4AB6-8F78-859BBD03C147}">
+    <comment ref="R11" authorId="0" shapeId="0" xr:uid="{23AE657E-3C83-418D-8383-7C74A6A01A55}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>hqyzsy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+钨钢锭焊接成钨钢块，然后通过锻压机变成钨钢圆形铸件</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG13" authorId="1" shapeId="0" xr:uid="{E6B9CEB0-A8B1-4AB6-8F78-859BBD03C147}">
       <text>
         <r>
           <rPr>
@@ -1318,57 +1345,6 @@
     <t>orenolanite_nether</t>
   </si>
   <si>
-    <t>blockcopper</t>
-  </si>
-  <si>
-    <t>blocktin</t>
-  </si>
-  <si>
-    <t>blockbronze</t>
-  </si>
-  <si>
-    <t>blocksteel</t>
-  </si>
-  <si>
-    <t>blockss</t>
-  </si>
-  <si>
-    <t>blocktungsten</t>
-  </si>
-  <si>
-    <t>blocknickel</t>
-  </si>
-  <si>
-    <t>blocktungsten_steel</t>
-  </si>
-  <si>
-    <t>blockinvar</t>
-  </si>
-  <si>
-    <t>blockhss</t>
-  </si>
-  <si>
-    <t>blocksilver</t>
-  </si>
-  <si>
-    <t>blockchromium</t>
-  </si>
-  <si>
-    <t>blockvanadium</t>
-  </si>
-  <si>
-    <t>blockcobalt</t>
-  </si>
-  <si>
-    <t>blocktitanium</t>
-  </si>
-  <si>
-    <t>blockaluminum</t>
-  </si>
-  <si>
-    <t>blockncalloy</t>
-  </si>
-  <si>
     <t>coilnickel</t>
   </si>
   <si>
@@ -1403,9 +1379,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>blockmanganese</t>
-  </si>
-  <si>
     <t>molten_copper_discarded</t>
   </si>
   <si>
@@ -1551,60 +1524,12 @@
     <t>apple_jam_bun</t>
   </si>
   <si>
-    <t>ingot_copper</t>
-  </si>
-  <si>
     <t>ingot_tin</t>
   </si>
   <si>
-    <t>ingot_bronze</t>
-  </si>
-  <si>
-    <t>ingot_steel</t>
-  </si>
-  <si>
-    <t>ingot_invar</t>
-  </si>
-  <si>
-    <t>ingot_ss</t>
-  </si>
-  <si>
-    <t>ingot_tungsten</t>
-  </si>
-  <si>
     <t>ingot_tungsten_steel</t>
   </si>
   <si>
-    <t>ingot_hss</t>
-  </si>
-  <si>
-    <t>ingot_silver</t>
-  </si>
-  <si>
-    <t>ingot_manganese</t>
-  </si>
-  <si>
-    <t>ingot_chromium</t>
-  </si>
-  <si>
-    <t>ingot_nickel</t>
-  </si>
-  <si>
-    <t>ingot_vanadium</t>
-  </si>
-  <si>
-    <t>ingot_cobalt</t>
-  </si>
-  <si>
-    <t>ingot_titanium</t>
-  </si>
-  <si>
-    <t>ingot_aluminum</t>
-  </si>
-  <si>
-    <t>ingot_ncalloy</t>
-  </si>
-  <si>
     <t>ingot_silicon</t>
   </si>
   <si>
@@ -1698,29 +1623,8 @@
     <t>stick_iron</t>
   </si>
   <si>
-    <t>circle_casting_steel</t>
-  </si>
-  <si>
-    <t>circle_casting_iron</t>
-  </si>
-  <si>
-    <t>circle_casting_silver</t>
-  </si>
-  <si>
-    <t>circle_casting_invar</t>
-  </si>
-  <si>
     <t>circle_casting_gold</t>
     <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>circle_casting_aluminum</t>
-  </si>
-  <si>
-    <t>circle_casting_nickel</t>
-  </si>
-  <si>
-    <t>circle_casting_ss</t>
   </si>
   <si>
     <t>circle_casting_tungsten_steel</t>
@@ -3166,6 +3070,170 @@
   </si>
   <si>
     <t>plate_silicon</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_copper</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_bronze</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_steel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_ss</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_tungsten</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_nickel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_invar</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_hss</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_silver</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_manganese</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_chromium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_vanadium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_cobalt</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_titanium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_aluminum</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingot_ncalloy</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockcopper</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocktin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockbronze</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocksteel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockss</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocktungsten</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocknickel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockinvar</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockhss</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocksilver</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockchromium</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockvanadium</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockcobalt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocktitanium</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockaluminum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockncalloy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockmanganese</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>blocktungsten_steel</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_steel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_iron</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_silver</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_invar</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_aluminum</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_nickel</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>circle_casting_ss</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -3945,8 +4013,8 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4012,43 +4080,43 @@
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>404</v>
+        <v>857</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>852</v>
+        <v>811</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="46" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="46" t="s">
-        <v>851</v>
+        <v>810</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>818</v>
+        <v>777</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -4062,49 +4130,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>405</v>
+        <v>858</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="46" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="46" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="46" t="s">
-        <v>853</v>
+        <v>812</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>818</v>
+        <v>777</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -4118,49 +4186,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>406</v>
+        <v>859</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="45" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="46" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>856</v>
+        <v>815</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>855</v>
+        <v>814</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>818</v>
+        <v>777</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -4180,43 +4248,43 @@
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>407</v>
+        <v>860</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="46" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="46" t="s">
-        <v>727</v>
+        <v>686</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="46" t="s">
-        <v>848</v>
+        <v>807</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>819</v>
+        <v>778</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -4236,37 +4304,37 @@
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>408</v>
+        <v>861</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="46" t="s">
-        <v>844</v>
+        <v>803</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="46" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>820</v>
+        <v>779</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -4286,31 +4354,31 @@
         <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>409</v>
+        <v>862</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="46" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="46" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>821</v>
+        <v>780</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -4330,31 +4398,31 @@
         <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>410</v>
+        <v>863</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>850</v>
+        <v>809</v>
       </c>
       <c r="M8" s="46" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="N8" t="s">
         <v>63</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>663</v>
+        <v>622</v>
       </c>
       <c r="R8" t="s">
         <v>65</v>
@@ -4374,31 +4442,31 @@
         <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>411</v>
+        <v>874</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
       </c>
       <c r="G9" s="45" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="N9" t="s">
         <v>69</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="P9" t="s">
         <v>70</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>664</v>
+        <v>623</v>
       </c>
       <c r="R9" t="s">
         <v>113</v>
@@ -4418,25 +4486,25 @@
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>412</v>
+        <v>864</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
       </c>
       <c r="G10" s="45" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>688</v>
+        <v>647</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>857</v>
+        <v>816</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>665</v>
+        <v>624</v>
       </c>
       <c r="R10" t="s">
         <v>71</v>
@@ -4456,19 +4524,19 @@
         <v>78</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>413</v>
+        <v>865</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
       </c>
       <c r="G11" s="45" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="P11" t="s">
         <v>80</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>666</v>
+        <v>625</v>
       </c>
       <c r="R11" t="s">
         <v>76</v>
@@ -4488,19 +4556,19 @@
         <v>83</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>414</v>
+        <v>866</v>
       </c>
       <c r="F12" t="s">
         <v>84</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>667</v>
+        <v>626</v>
       </c>
       <c r="R12" t="s">
         <v>81</v>
@@ -4520,19 +4588,19 @@
         <v>87</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>415</v>
+        <v>867</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
       <c r="G13" s="45" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>822</v>
+        <v>781</v>
       </c>
       <c r="Q13" s="46" t="s">
-        <v>823</v>
+        <v>782</v>
       </c>
       <c r="R13" t="s">
         <v>93</v>
@@ -4552,13 +4620,13 @@
         <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>416</v>
+        <v>868</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="R14" t="s">
         <v>97</v>
@@ -4578,13 +4646,13 @@
         <v>95</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>417</v>
+        <v>869</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
       </c>
       <c r="G15" s="45" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="R15" t="s">
         <v>101</v>
@@ -4604,13 +4672,13 @@
         <v>99</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>418</v>
+        <v>870</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
       </c>
       <c r="G16" s="45" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="R16" t="s">
         <v>105</v>
@@ -4630,13 +4698,13 @@
         <v>103</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>419</v>
+        <v>871</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
       </c>
       <c r="G17" s="45" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="R17" t="s">
         <v>108</v>
@@ -4656,13 +4724,13 @@
         <v>106</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>420</v>
+        <v>872</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="R18" t="s">
         <v>111</v>
@@ -4676,13 +4744,13 @@
         <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>431</v>
+        <v>873</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
       </c>
       <c r="G19" s="45" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="R19" t="s">
         <v>115</v>
@@ -4696,10 +4764,10 @@
         <v>112</v>
       </c>
       <c r="G20" s="45" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4710,7 +4778,7 @@
         <v>114</v>
       </c>
       <c r="G21" s="45" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="R21" t="s">
         <v>89</v>
@@ -4752,9 +4820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4860,103 +4928,103 @@
         <v>137</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>585</v>
+        <v>544</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>603</v>
+        <v>562</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>478</v>
+        <v>841</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>140</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>497</v>
+        <v>463</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>141</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>717</v>
+        <v>676</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>142</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>515</v>
+        <v>481</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>845</v>
+        <v>804</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>846</v>
+        <v>805</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>861</v>
+      <c r="S2" s="46" t="s">
+        <v>820</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>181</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>862</v>
+        <v>821</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>849</v>
+        <v>808</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
       </c>
       <c r="AA2" s="46" t="s">
-        <v>720</v>
+        <v>679</v>
       </c>
       <c r="AB2" s="5" t="s">
         <v>132</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>555</v>
+        <v>514</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>150</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>598</v>
+        <v>557</v>
       </c>
       <c r="AF2" s="5" t="s">
         <v>151</v>
       </c>
       <c r="AG2" s="46" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="AH2" s="5" t="s">
         <v>152</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>153</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>719</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -4967,109 +5035,109 @@
         <v>154</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>586</v>
+        <v>545</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>155</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>604</v>
+        <v>563</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>156</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>157</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>498</v>
+        <v>464</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>158</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>867</v>
+        <v>826</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>516</v>
+        <v>482</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>160</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>541</v>
+        <v>500</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>161</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>542</v>
+        <v>501</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="S3" s="8" t="s">
-        <v>527</v>
+      <c r="S3" s="46" t="s">
+        <v>875</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>198</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>863</v>
+        <v>822</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>659</v>
+        <v>618</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>660</v>
+        <v>619</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>165</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>584</v>
+        <v>543</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>166</v>
       </c>
       <c r="AA3" s="46" t="s">
-        <v>721</v>
+        <v>680</v>
       </c>
       <c r="AB3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>557</v>
+        <v>516</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>599</v>
+        <v>558</v>
       </c>
       <c r="AF3" s="5" t="s">
         <v>169</v>
       </c>
       <c r="AG3" s="46" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="AH3" s="5" t="s">
         <v>170</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="AJ3" s="5" t="s">
         <v>171</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>622</v>
+        <v>581</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -5080,103 +5148,103 @@
         <v>172</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>587</v>
+        <v>546</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>605</v>
+        <v>564</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>480</v>
+        <v>842</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>175</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>499</v>
+        <v>465</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>176</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>868</v>
+        <v>827</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>517</v>
+        <v>483</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>178</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>538</v>
+        <v>497</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>179</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>550</v>
+        <v>509</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="S4" s="8" t="s">
-        <v>528</v>
+      <c r="S4" s="46" t="s">
+        <v>876</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>232</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>864</v>
+        <v>823</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>182</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>582</v>
+        <v>541</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>183</v>
       </c>
       <c r="AA4" s="46" t="s">
-        <v>573</v>
+        <v>532</v>
       </c>
       <c r="AB4" s="5" t="s">
         <v>184</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>558</v>
+        <v>517</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>185</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>600</v>
+        <v>559</v>
       </c>
       <c r="AF4" s="5" t="s">
         <v>186</v>
       </c>
       <c r="AG4" s="46" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="AH4" t="s">
         <v>187</v>
       </c>
       <c r="AI4" s="8" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="AJ4" s="5" t="s">
         <v>188</v>
       </c>
       <c r="AK4" s="8" t="s">
-        <v>715</v>
+        <v>674</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -5187,97 +5255,97 @@
         <v>189</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>588</v>
+        <v>547</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>606</v>
+        <v>565</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>191</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>481</v>
+        <v>843</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>500</v>
+        <v>466</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>193</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>869</v>
+        <v>828</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>194</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>518</v>
+        <v>484</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>195</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>539</v>
+        <v>498</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>196</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>543</v>
+        <v>502</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>529</v>
+      <c r="S5" s="46" t="s">
+        <v>877</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>200</v>
       </c>
       <c r="Y5" s="8" t="s">
-        <v>578</v>
+        <v>537</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>201</v>
       </c>
       <c r="AA5" s="46" t="s">
-        <v>569</v>
+        <v>528</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>202</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>559</v>
+        <v>518</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>203</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>601</v>
+        <v>560</v>
       </c>
       <c r="AF5" s="41" t="s">
         <v>204</v>
       </c>
       <c r="AG5" s="8" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="AH5" t="s">
         <v>205</v>
       </c>
       <c r="AI5" s="8" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="AJ5" s="5" t="s">
         <v>206</v>
       </c>
       <c r="AK5" s="46" t="s">
-        <v>623</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -5288,103 +5356,103 @@
         <v>207</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>589</v>
+        <v>548</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>607</v>
+        <v>566</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>209</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>483</v>
+        <v>844</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>210</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>502</v>
+        <v>468</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>211</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>870</v>
+        <v>829</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>212</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>520</v>
+        <v>486</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>213</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>540</v>
+        <v>499</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>214</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>549</v>
+        <v>508</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="S6" s="8" t="s">
-        <v>530</v>
+      <c r="S6" s="46" t="s">
+        <v>878</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>260</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>865</v>
+        <v>824</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>217</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>551</v>
+        <v>510</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>218</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>575</v>
+        <v>534</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>219</v>
       </c>
       <c r="AA6" s="46" t="s">
-        <v>566</v>
+        <v>525</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>220</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>556</v>
+        <v>515</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>221</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>602</v>
+        <v>561</v>
       </c>
       <c r="AF6" s="5" t="s">
         <v>222</v>
       </c>
       <c r="AG6" s="46" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="AJ6" s="5" t="s">
         <v>223</v>
       </c>
       <c r="AK6" s="46" t="s">
-        <v>624</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -5395,37 +5463,37 @@
         <v>224</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>590</v>
+        <v>549</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>225</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>609</v>
+        <v>568</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>226</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>484</v>
+        <v>845</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>227</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>503</v>
+        <v>469</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>228</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>871</v>
+        <v>830</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>229</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>519</v>
+        <v>485</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -5433,13 +5501,13 @@
         <v>230</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>544</v>
+        <v>503</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="S7" s="9" t="s">
-        <v>531</v>
+      <c r="S7" s="46" t="s">
+        <v>493</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
@@ -5447,31 +5515,31 @@
         <v>233</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>583</v>
+        <v>542</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>234</v>
       </c>
       <c r="AA7" s="46" t="s">
-        <v>574</v>
+        <v>533</v>
       </c>
       <c r="AB7" s="5" t="s">
         <v>235</v>
       </c>
       <c r="AC7" s="46" t="s">
-        <v>716</v>
+        <v>675</v>
       </c>
       <c r="AF7" s="5" t="s">
         <v>236</v>
       </c>
       <c r="AG7" s="46" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="AJ7" s="5" t="s">
         <v>237</v>
       </c>
       <c r="AK7" s="8" t="s">
-        <v>625</v>
+        <v>584</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -5482,37 +5550,37 @@
         <v>238</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>591</v>
+        <v>550</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>239</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>610</v>
+        <v>569</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>240</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>490</v>
+        <v>846</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>241</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>507</v>
+        <v>473</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>242</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>872</v>
+        <v>831</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>243</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>521</v>
+        <v>487</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -5520,19 +5588,19 @@
         <v>244</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>545</v>
+        <v>504</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="S8" s="8" t="s">
-        <v>532</v>
+      <c r="S8" s="46" t="s">
+        <v>879</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>661</v>
+        <v>620</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>662</v>
+        <v>621</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="8"/>
@@ -5540,31 +5608,31 @@
         <v>247</v>
       </c>
       <c r="Y8" s="8" t="s">
-        <v>581</v>
+        <v>540</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>248</v>
       </c>
       <c r="AA8" s="46" t="s">
-        <v>572</v>
+        <v>531</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>249</v>
       </c>
       <c r="AC8" s="46" t="s">
-        <v>561</v>
+        <v>520</v>
       </c>
       <c r="AF8" s="5" t="s">
         <v>250</v>
       </c>
       <c r="AG8" s="46" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="AJ8" s="5" t="s">
         <v>251</v>
       </c>
       <c r="AK8" s="8" t="s">
-        <v>847</v>
+        <v>806</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5575,37 +5643,37 @@
         <v>252</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>592</v>
+        <v>551</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>611</v>
+        <v>570</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>254</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>482</v>
+        <v>847</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>255</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>256</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>873</v>
+        <v>832</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>257</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>522</v>
+        <v>488</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -5613,13 +5681,13 @@
         <v>258</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>546</v>
+        <v>505</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="S9" s="8" t="s">
-        <v>533</v>
+      <c r="S9" s="46" t="s">
+        <v>880</v>
       </c>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
@@ -5627,31 +5695,31 @@
         <v>261</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>579</v>
+        <v>538</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>262</v>
       </c>
       <c r="AA9" s="46" t="s">
-        <v>570</v>
+        <v>529</v>
       </c>
       <c r="AB9" s="5" t="s">
         <v>263</v>
       </c>
       <c r="AC9" s="46" t="s">
-        <v>562</v>
+        <v>521</v>
       </c>
       <c r="AF9" s="5" t="s">
         <v>264</v>
       </c>
       <c r="AG9" s="46" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="AJ9" s="5" t="s">
         <v>265</v>
       </c>
       <c r="AK9" s="8" t="s">
-        <v>626</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5662,37 +5730,37 @@
         <v>266</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>593</v>
+        <v>552</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>267</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>612</v>
+        <v>571</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>269</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>833</v>
+        <v>792</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>270</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>536</v>
+        <v>495</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>271</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>524</v>
+        <v>490</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -5700,55 +5768,55 @@
         <v>272</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>547</v>
+        <v>506</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="S10" s="8" t="s">
-        <v>534</v>
+      <c r="S10" s="46" t="s">
+        <v>881</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>146</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>563</v>
+        <v>522</v>
       </c>
       <c r="V10" s="5" t="s">
         <v>147</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>552</v>
+        <v>511</v>
       </c>
       <c r="X10" s="5" t="s">
         <v>274</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>576</v>
+        <v>535</v>
       </c>
       <c r="Z10" s="5" t="s">
         <v>275</v>
       </c>
       <c r="AA10" s="46" t="s">
-        <v>567</v>
+        <v>526</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>276</v>
       </c>
       <c r="AC10" s="46" t="s">
-        <v>560</v>
+        <v>519</v>
       </c>
       <c r="AF10" s="5" t="s">
         <v>277</v>
       </c>
       <c r="AG10" s="46" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="AJ10" s="5" t="s">
         <v>278</v>
       </c>
       <c r="AK10" s="46" t="s">
-        <v>627</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5759,37 +5827,37 @@
         <v>279</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>594</v>
+        <v>553</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>613</v>
+        <v>572</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>281</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>486</v>
+        <v>848</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>282</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>504</v>
+        <v>470</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>283</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>874</v>
+        <v>833</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>284</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>525</v>
+        <v>491</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -5797,37 +5865,37 @@
         <v>285</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>548</v>
+        <v>507</v>
       </c>
       <c r="R11" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="S11" s="8" t="s">
-        <v>535</v>
+      <c r="S11" s="46" t="s">
+        <v>494</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>246</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>564</v>
+        <v>523</v>
       </c>
       <c r="V11" s="5" t="s">
         <v>199</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>553</v>
+        <v>512</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>287</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>577</v>
+        <v>536</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>288</v>
       </c>
       <c r="AA11" s="46" t="s">
-        <v>568</v>
+        <v>527</v>
       </c>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
@@ -5835,13 +5903,13 @@
         <v>289</v>
       </c>
       <c r="AG11" s="46" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="AJ11" s="5" t="s">
         <v>290</v>
       </c>
       <c r="AK11" s="46" t="s">
-        <v>628</v>
+        <v>587</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5852,37 +5920,37 @@
         <v>291</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>595</v>
+        <v>554</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>292</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>614</v>
+        <v>573</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>293</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>487</v>
+        <v>849</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>294</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>506</v>
+        <v>472</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>295</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>875</v>
+        <v>834</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>296</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>523</v>
+        <v>489</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -5891,14 +5959,14 @@
       <c r="R12" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="S12" s="8" t="s">
-        <v>859</v>
+      <c r="S12" s="46" t="s">
+        <v>818</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>216</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>866</v>
+        <v>825</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -5906,13 +5974,13 @@
         <v>298</v>
       </c>
       <c r="Y12" s="8" t="s">
-        <v>580</v>
+        <v>539</v>
       </c>
       <c r="Z12" s="5" t="s">
         <v>299</v>
       </c>
       <c r="AA12" s="46" t="s">
-        <v>571</v>
+        <v>530</v>
       </c>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
@@ -5920,13 +5988,13 @@
         <v>300</v>
       </c>
       <c r="AG12" s="8" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="AJ12" s="5" t="s">
         <v>301</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>629</v>
+        <v>588</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -5937,59 +6005,59 @@
         <v>302</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>597</v>
+        <v>556</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>303</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>608</v>
+        <v>567</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>304</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>488</v>
+        <v>850</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>305</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>832</v>
+        <v>791</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>306</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>876</v>
+        <v>835</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>307</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>526</v>
+        <v>492</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="10" t="s">
-        <v>858</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>860</v>
+        <v>817</v>
+      </c>
+      <c r="S13" s="46" t="s">
+        <v>819</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>163</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>565</v>
+        <v>524</v>
       </c>
       <c r="V13" s="5" t="s">
         <v>164</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>554</v>
+        <v>513</v>
       </c>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -5998,16 +6066,16 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AF13" s="41" t="s">
-        <v>657</v>
+        <v>616</v>
       </c>
       <c r="AG13" s="46" t="s">
-        <v>658</v>
+        <v>617</v>
       </c>
       <c r="AJ13" s="5" t="s">
         <v>308</v>
       </c>
       <c r="AK13" s="8" t="s">
-        <v>630</v>
+        <v>589</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -6018,31 +6086,31 @@
         <v>309</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>596</v>
+        <v>555</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>615</v>
+        <v>574</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>311</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>489</v>
+        <v>851</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>312</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>831</v>
+        <v>790</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>313</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>877</v>
+        <v>836</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6067,7 +6135,7 @@
         <v>314</v>
       </c>
       <c r="AK14" s="8" t="s">
-        <v>631</v>
+        <v>590</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -6082,19 +6150,19 @@
         <v>315</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>491</v>
+        <v>852</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>316</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>508</v>
+        <v>474</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>317</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>878</v>
+        <v>837</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -6116,7 +6184,7 @@
         <v>318</v>
       </c>
       <c r="AK15" s="8" t="s">
-        <v>632</v>
+        <v>591</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -6131,19 +6199,19 @@
         <v>319</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>492</v>
+        <v>853</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>320</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>509</v>
+        <v>475</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>321</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>879</v>
+        <v>838</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -6165,7 +6233,7 @@
         <v>322</v>
       </c>
       <c r="AK16" s="46" t="s">
-        <v>633</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -6180,19 +6248,19 @@
         <v>323</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>493</v>
+        <v>854</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>324</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>510</v>
+        <v>476</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>325</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>880</v>
+        <v>839</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -6211,10 +6279,10 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AJ17" s="10" t="s">
-        <v>616</v>
+        <v>575</v>
       </c>
       <c r="AK17" s="46" t="s">
-        <v>619</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -6229,19 +6297,19 @@
         <v>326</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>494</v>
+        <v>855</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>327</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>511</v>
+        <v>477</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>328</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>881</v>
+        <v>840</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -6260,10 +6328,10 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AJ18" s="10" t="s">
-        <v>617</v>
+        <v>576</v>
       </c>
       <c r="AK18" s="46" t="s">
-        <v>620</v>
+        <v>579</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -6278,19 +6346,19 @@
         <v>329</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>495</v>
+        <v>856</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>330</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>834</v>
+        <v>793</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>331</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>537</v>
+        <v>496</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -6311,10 +6379,10 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AJ19" s="10" t="s">
-        <v>668</v>
+        <v>627</v>
       </c>
       <c r="AK19" s="46" t="s">
-        <v>669</v>
+        <v>628</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -6329,13 +6397,13 @@
         <v>332</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>496</v>
+        <v>462</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>333</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>505</v>
+        <v>471</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -6358,10 +6426,10 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AJ20" s="10" t="s">
-        <v>618</v>
+        <v>577</v>
       </c>
       <c r="AK20" s="46" t="s">
-        <v>621</v>
+        <v>580</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -6376,13 +6444,13 @@
         <v>334</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>854</v>
+        <v>813</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>335</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>513</v>
+        <v>479</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -6405,10 +6473,10 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AJ21" s="10" t="s">
-        <v>636</v>
+        <v>595</v>
       </c>
       <c r="AK21" s="46" t="s">
-        <v>637</v>
+        <v>596</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -6425,7 +6493,7 @@
         <v>336</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>514</v>
+        <v>480</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -6448,10 +6516,10 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AJ22" s="10" t="s">
-        <v>682</v>
+        <v>641</v>
       </c>
       <c r="AK22" s="46" t="s">
-        <v>685</v>
+        <v>644</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -6468,10 +6536,10 @@
         <v>337</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>634</v>
+        <v>593</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>835</v>
+        <v>794</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -6493,10 +6561,10 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AJ23" s="10" t="s">
-        <v>683</v>
+        <v>642</v>
       </c>
       <c r="AK23" s="46" t="s">
-        <v>686</v>
+        <v>645</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6513,7 +6581,7 @@
         <v>338</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>836</v>
+        <v>795</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -6535,10 +6603,10 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AJ24" s="16" t="s">
-        <v>684</v>
+        <v>643</v>
       </c>
       <c r="AK24" s="46" t="s">
-        <v>687</v>
+        <v>646</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6555,7 +6623,7 @@
         <v>339</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>512</v>
+        <v>478</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -6577,10 +6645,10 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AJ25" s="21" t="s">
-        <v>694</v>
+        <v>653</v>
       </c>
       <c r="AK25" s="9" t="s">
-        <v>698</v>
+        <v>657</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6597,10 +6665,10 @@
         <v>340</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>635</v>
+        <v>594</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>837</v>
+        <v>796</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -6622,10 +6690,10 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AJ26" s="16" t="s">
-        <v>695</v>
+        <v>654</v>
       </c>
       <c r="AK26" s="9" t="s">
-        <v>699</v>
+        <v>658</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6636,11 +6704,11 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="42" t="s">
-        <v>838</v>
+        <v>797</v>
       </c>
       <c r="I27" s="42"/>
       <c r="J27" s="42" t="s">
-        <v>839</v>
+        <v>798</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -6662,10 +6730,10 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AJ27" s="16" t="s">
-        <v>696</v>
+        <v>655</v>
       </c>
       <c r="AK27" s="9" t="s">
-        <v>700</v>
+        <v>659</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6676,11 +6744,11 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="42" t="s">
-        <v>840</v>
+        <v>799</v>
       </c>
       <c r="I28" s="42"/>
       <c r="J28" s="42" t="s">
-        <v>841</v>
+        <v>800</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -6702,18 +6770,18 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AJ28" s="40" t="s">
-        <v>697</v>
+        <v>656</v>
       </c>
       <c r="AK28" s="9" t="s">
-        <v>701</v>
+        <v>660</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ29" s="39" t="s">
-        <v>824</v>
+        <v>783</v>
       </c>
       <c r="AK29" s="9" t="s">
-        <v>825</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -6728,8 +6796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6746,7 +6814,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
-        <v>723</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6769,10 +6837,10 @@
         <v>344</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>641</v>
+        <v>600</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>655</v>
+        <v>614</v>
       </c>
       <c r="E3" t="s">
         <v>345</v>
@@ -6790,7 +6858,7 @@
         <v>349</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>656</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6801,10 +6869,10 @@
         <v>350</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>642</v>
+        <v>601</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>655</v>
+        <v>614</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6815,10 +6883,10 @@
         <v>351</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>643</v>
+        <v>602</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>655</v>
+        <v>614</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6829,10 +6897,10 @@
         <v>352</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>638</v>
+        <v>597</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>674</v>
+        <v>633</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6843,22 +6911,22 @@
         <v>353</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>639</v>
+        <v>598</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>675</v>
+        <v>634</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>670</v>
+        <v>629</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>671</v>
+        <v>630</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>672</v>
+        <v>631</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>673</v>
+        <v>632</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6866,13 +6934,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>692</v>
+        <v>651</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>640</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>681</v>
       </c>
       <c r="E8" t="s">
         <v>354</v>
@@ -6881,7 +6949,7 @@
         <v>355</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>718</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6889,13 +6957,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>712</v>
+        <v>671</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>644</v>
+        <v>603</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>677</v>
+        <v>636</v>
       </c>
       <c r="E9" t="s">
         <v>356</v>
@@ -6909,10 +6977,10 @@
         <v>357</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>645</v>
+        <v>604</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>678</v>
+        <v>637</v>
       </c>
       <c r="E10" t="s">
         <v>358</v>
@@ -6923,13 +6991,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>691</v>
+        <v>650</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>646</v>
+        <v>605</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>679</v>
+        <v>638</v>
       </c>
       <c r="E11" t="s">
         <v>359</v>
@@ -6946,13 +7014,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="43" t="s">
-        <v>713</v>
+        <v>672</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>647</v>
+        <v>606</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>680</v>
+        <v>639</v>
       </c>
       <c r="E12" t="s">
         <v>362</v>
@@ -6963,13 +7031,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>722</v>
+        <v>681</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>648</v>
+        <v>607</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>829</v>
+        <v>788</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6977,13 +7045,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="43" t="s">
-        <v>714</v>
+        <v>673</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>649</v>
+        <v>608</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>676</v>
+        <v>635</v>
       </c>
       <c r="E14" t="s">
         <v>133</v>
@@ -7007,7 +7075,7 @@
         <v>364</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>693</v>
+        <v>652</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7018,10 +7086,10 @@
         <v>365</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>650</v>
+        <v>609</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>690</v>
+        <v>649</v>
       </c>
       <c r="E15" t="s">
         <v>366</v>
@@ -7035,10 +7103,10 @@
         <v>367</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>651</v>
+        <v>610</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>689</v>
+        <v>648</v>
       </c>
       <c r="E16" t="s">
         <v>368</v>
@@ -7073,16 +7141,16 @@
         <v>373</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>736</v>
+        <v>695</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>737</v>
+        <v>696</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>738</v>
+        <v>697</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>739</v>
+        <v>698</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -7096,20 +7164,20 @@
         <v>2</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>740</v>
+        <v>699</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>741</v>
+        <v>700</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>742</v>
+        <v>701</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="27" t="s">
         <v>374</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>743</v>
+        <v>702</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
@@ -7121,18 +7189,18 @@
       <c r="A21" s="23">
         <v>3</v>
       </c>
-      <c r="B21" s="29" t="s">
-        <v>744</v>
+      <c r="B21" s="47" t="s">
+        <v>703</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>745</v>
+        <v>704</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>746</v>
+        <v>705</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="27" t="s">
-        <v>747</v>
+        <v>706</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>375</v>
@@ -7148,32 +7216,32 @@
         <v>4</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>735</v>
+        <v>694</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>654</v>
+        <v>613</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>748</v>
+        <v>707</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>749</v>
+        <v>708</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>750</v>
+        <v>709</v>
       </c>
       <c r="G22" s="30" t="s">
         <v>376</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="22" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>752</v>
+        <v>711</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
       <c r="L22" s="28"/>
     </row>
@@ -7185,10 +7253,10 @@
         <v>377</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>754</v>
+        <v>713</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>755</v>
+        <v>714</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="23"/>
@@ -7196,16 +7264,16 @@
         <v>378</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>756</v>
+        <v>715</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>752</v>
+        <v>711</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
       <c r="L23" s="28"/>
     </row>
@@ -7214,17 +7282,17 @@
         <v>6</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>757</v>
+        <v>716</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>758</v>
+        <v>717</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>759</v>
+        <v>718</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="23" t="s">
-        <v>760</v>
+        <v>719</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -7238,34 +7306,34 @@
         <v>7</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>761</v>
+        <v>720</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>762</v>
+        <v>721</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>763</v>
+        <v>722</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>764</v>
+        <v>723</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>765</v>
+        <v>724</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>766</v>
+        <v>725</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>767</v>
+        <v>726</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>729</v>
+        <v>688</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>730</v>
+        <v>689</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>731</v>
+        <v>690</v>
       </c>
       <c r="L25" s="28"/>
     </row>
@@ -7274,13 +7342,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>768</v>
+        <v>727</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>769</v>
+        <v>728</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>734</v>
+        <v>693</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>386</v>
@@ -7292,19 +7360,19 @@
         <v>380</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>732</v>
+        <v>691</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>733</v>
+        <v>692</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>770</v>
+        <v>729</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="117" x14ac:dyDescent="0.3">
@@ -7312,27 +7380,27 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>771</v>
+        <v>730</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>728</v>
+        <v>687</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="23" t="s">
-        <v>772</v>
+        <v>731</v>
       </c>
       <c r="G27" s="32" t="s">
         <v>381</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>752</v>
+        <v>711</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
@@ -7342,29 +7410,29 @@
         <v>10</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>773</v>
+        <v>732</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>774</v>
+        <v>733</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>775</v>
+        <v>734</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="23" t="s">
-        <v>776</v>
+        <v>735</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>382</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>752</v>
+        <v>711</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
@@ -7374,29 +7442,29 @@
         <v>11</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>777</v>
+        <v>736</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>778</v>
+        <v>737</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>779</v>
+        <v>738</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="23" t="s">
-        <v>780</v>
+        <v>739</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>383</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>751</v>
+        <v>710</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>752</v>
+        <v>711</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>753</v>
+        <v>712</v>
       </c>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
@@ -7406,23 +7474,23 @@
         <v>12</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>781</v>
+        <v>740</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>782</v>
+        <v>741</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>384</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="23" t="s">
-        <v>783</v>
+        <v>742</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>830</v>
+        <v>789</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>787</v>
+        <v>746</v>
       </c>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
@@ -7434,16 +7502,16 @@
         <v>13</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>784</v>
+        <v>743</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>652</v>
+        <v>611</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>385</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>749</v>
+        <v>708</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -7458,13 +7526,13 @@
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>785</v>
+        <v>744</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>653</v>
+        <v>612</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>786</v>
+        <v>745</v>
       </c>
       <c r="E32" s="34" t="s">
         <v>386</v>
@@ -7482,13 +7550,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>724</v>
+        <v>683</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>725</v>
+        <v>684</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>726</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -7522,36 +7590,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>788</v>
+        <v>747</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>789</v>
+        <v>748</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>791</v>
+        <v>750</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>793</v>
+        <v>752</v>
       </c>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>790</v>
+        <v>749</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>792</v>
+        <v>751</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>794</v>
+        <v>753</v>
       </c>
       <c r="G3" s="37">
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>799</v>
+        <v>758</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
@@ -7559,131 +7627,131 @@
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>800</v>
+        <v>759</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D5" s="38" t="s">
-        <v>811</v>
+        <v>770</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>797</v>
+        <v>756</v>
       </c>
       <c r="G5" s="37">
         <v>3</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>801</v>
+        <v>760</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
       <c r="D6" s="38" t="s">
-        <v>812</v>
+        <v>771</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>816</v>
+        <v>775</v>
       </c>
       <c r="G6" s="37">
         <v>4</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>804</v>
+        <v>763</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>809</v>
+        <v>768</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
-        <v>814</v>
+        <v>773</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>795</v>
+        <v>754</v>
       </c>
       <c r="G7" s="37">
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>802</v>
+        <v>761</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
-        <v>813</v>
+        <v>772</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>796</v>
+        <v>755</v>
       </c>
       <c r="G8" s="37">
         <v>6</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>803</v>
+        <v>762</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="D9" s="38" t="s">
-        <v>815</v>
+        <v>774</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>817</v>
+        <v>776</v>
       </c>
       <c r="G9" s="37">
         <v>7</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>805</v>
+        <v>764</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D10" s="13" t="s">
-        <v>827</v>
+        <v>786</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>808</v>
+        <v>767</v>
       </c>
       <c r="G10" s="37">
         <v>8</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>806</v>
+        <v>765</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="F11" s="13" t="s">
-        <v>798</v>
+        <v>757</v>
       </c>
       <c r="G11" s="37">
         <v>9</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>807</v>
+        <v>766</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D12" s="13" t="s">
-        <v>826</v>
+        <v>785</v>
       </c>
       <c r="G12" s="37">
         <v>10</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>810</v>
+        <v>769</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
-        <v>828</v>
+        <v>787</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>842</v>
+        <v>801</v>
       </c>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="F14" s="44" t="s">
-        <v>843</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -7718,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>702</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -7744,7 +7812,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>703</v>
+        <v>662</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7752,7 +7820,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>709</v>
+        <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7760,7 +7828,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>704</v>
+        <v>663</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7768,7 +7836,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>710</v>
+        <v>669</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7776,7 +7844,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>705</v>
+        <v>664</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -7784,7 +7852,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>706</v>
+        <v>665</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7792,7 +7860,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>707</v>
+        <v>666</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -7800,7 +7868,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>708</v>
+        <v>667</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7808,7 +7876,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>711</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2021.9.28 21.47 for 更多合成及bug修复
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F04A584-27A0-4C4B-A3E5-FA9A97C90FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FFBB9C-D132-48DD-BED3-7DA3D32170ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1256,9 +1256,6 @@
     <t>块1440mb；锭160mb；圆形铸件1440mb</t>
   </si>
   <si>
-    <t>板150mb；杆68mb；线68mb；管600mb；</t>
-  </si>
-  <si>
     <t>反应釜</t>
   </si>
   <si>
@@ -1518,9 +1515,6 @@
     <t>golden_apple_jam_bun</t>
   </si>
   <si>
-    <t>apple_drops</t>
-  </si>
-  <si>
     <t>apple_jam_bun</t>
   </si>
   <si>
@@ -1642,9 +1636,6 @@
     <t>screw_ss</t>
   </si>
   <si>
-    <t>screw_titanium</t>
-  </si>
-  <si>
     <t>screw_iron</t>
   </si>
   <si>
@@ -1690,18 +1681,9 @@
     <t>slag</t>
   </si>
   <si>
-    <t>slag_manganese</t>
-  </si>
-  <si>
-    <t>slag_vanadium</t>
-  </si>
-  <si>
     <t>slag_cobalt</t>
   </si>
   <si>
-    <t>slag_titanium</t>
-  </si>
-  <si>
     <t>refined_slag_manganese</t>
   </si>
   <si>
@@ -1783,36 +1765,15 @@
     <t>crushed_tin</t>
   </si>
   <si>
-    <t>crushed_ilmenite</t>
-  </si>
-  <si>
     <t>crushed_silver</t>
   </si>
   <si>
-    <t>crushed_pyrolusite</t>
-  </si>
-  <si>
     <t>crushed_gold</t>
   </si>
   <si>
-    <t>crushed_chromite</t>
-  </si>
-  <si>
-    <t>crushed_bauxite</t>
-  </si>
-  <si>
-    <t>crushed_ferromanganese</t>
-  </si>
-  <si>
     <t>crushed_nickel</t>
   </si>
   <si>
-    <t>crushed_nolanite</t>
-  </si>
-  <si>
-    <t>crushed_tunstite</t>
-  </si>
-  <si>
     <t>crushed_iron</t>
   </si>
   <si>
@@ -1835,15 +1796,9 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>ore_copper_concentrate</t>
-  </si>
-  <si>
     <t>ore_tin_concentrate</t>
   </si>
   <si>
-    <t>ore_ilmenite_concentrate</t>
-  </si>
-  <si>
     <t>ore_silver_concentrate</t>
   </si>
   <si>
@@ -1871,9 +1826,6 @@
     <t>ore_nolanite_concentrate</t>
   </si>
   <si>
-    <t>ore_tunstite_concentrate</t>
-  </si>
-  <si>
     <t>锭模具</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -1932,9 +1884,6 @@
   </si>
   <si>
     <t>hss_additive</t>
-  </si>
-  <si>
-    <t>ss_additive</t>
   </si>
   <si>
     <t>青铜剑刃</t>
@@ -3234,6 +3183,74 @@
   </si>
   <si>
     <t>circle_casting_ss</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>板150mb；杆75mb；线75mb；管600mb；</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>screw_titanium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>apple_drops</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ore_copper_concentrate</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ore_ilmenite_concentrate</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_chromite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_ilmenite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>slag_titanium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_pyrolusite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_bauxite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_ferromanganese</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>slag_manganese</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_nolanite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>slag_vanadium</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>crushed_tunstite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ore_tunstite_concentrate</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss_additive</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -3426,7 +3443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3517,9 +3534,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3546,6 +3560,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4013,8 +4033,8 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2:Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4074,49 +4094,49 @@
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>857</v>
+        <v>840</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="45" t="s">
-        <v>414</v>
+      <c r="G2" s="44" t="s">
+        <v>413</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="46" t="s">
-        <v>408</v>
+      <c r="I2" s="45" t="s">
+        <v>407</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>811</v>
+        <v>794</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="46" t="s">
-        <v>440</v>
+      <c r="M2" s="45" t="s">
+        <v>439</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="46" t="s">
-        <v>810</v>
+      <c r="O2" s="45" t="s">
+        <v>793</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
@@ -4130,49 +4150,49 @@
         <v>18</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>858</v>
+        <v>841</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>415</v>
+      <c r="G3" s="44" t="s">
+        <v>414</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="46" t="s">
-        <v>409</v>
+      <c r="I3" s="45" t="s">
+        <v>408</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="46" t="s">
-        <v>441</v>
+      <c r="M3" s="45" t="s">
+        <v>440</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="46" t="s">
-        <v>812</v>
+      <c r="O3" s="45" t="s">
+        <v>795</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -4186,49 +4206,49 @@
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>859</v>
+        <v>842</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="45" t="s">
-        <v>416</v>
+      <c r="G4" s="44" t="s">
+        <v>415</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="46" t="s">
-        <v>410</v>
+      <c r="I4" s="45" t="s">
+        <v>409</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>815</v>
+        <v>798</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="46" t="s">
-        <v>814</v>
+      <c r="O4" s="45" t="s">
+        <v>797</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
@@ -4242,49 +4262,49 @@
         <v>36</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>860</v>
+        <v>843</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="45" t="s">
-        <v>417</v>
+      <c r="G5" s="44" t="s">
+        <v>416</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="46" t="s">
-        <v>411</v>
+      <c r="I5" s="45" t="s">
+        <v>410</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="46" t="s">
-        <v>686</v>
+      <c r="M5" s="45" t="s">
+        <v>669</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="46" t="s">
-        <v>807</v>
+      <c r="O5" s="45" t="s">
+        <v>790</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
@@ -4298,43 +4318,43 @@
         <v>45</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>861</v>
+        <v>844</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="45" t="s">
-        <v>418</v>
+      <c r="G6" s="44" t="s">
+        <v>417</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="46" t="s">
-        <v>803</v>
+      <c r="M6" s="45" t="s">
+        <v>786</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="46" t="s">
-        <v>435</v>
+      <c r="O6" s="45" t="s">
+        <v>434</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>779</v>
+        <v>762</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
@@ -4348,37 +4368,37 @@
         <v>53</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>862</v>
+        <v>845</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="45" t="s">
-        <v>419</v>
+      <c r="G7" s="44" t="s">
+        <v>418</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="46" t="s">
-        <v>444</v>
+      <c r="M7" s="45" t="s">
+        <v>443</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="46" t="s">
-        <v>436</v>
+      <c r="O7" s="45" t="s">
+        <v>435</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>780</v>
+        <v>763</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
@@ -4392,37 +4412,37 @@
         <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>863</v>
+        <v>846</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="45" t="s">
-        <v>420</v>
+      <c r="G8" s="44" t="s">
+        <v>419</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>809</v>
-      </c>
-      <c r="M8" s="46" t="s">
-        <v>439</v>
+        <v>792</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>438</v>
       </c>
       <c r="N8" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="46" t="s">
-        <v>437</v>
+      <c r="O8" s="45" t="s">
+        <v>436</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>622</v>
+        <v>605</v>
       </c>
       <c r="R8" t="s">
         <v>65</v>
@@ -4436,37 +4456,37 @@
         <v>66</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D9" t="s">
         <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>874</v>
+        <v>857</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="45" t="s">
-        <v>432</v>
+      <c r="G9" s="44" t="s">
+        <v>431</v>
       </c>
       <c r="L9" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>442</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>443</v>
       </c>
       <c r="N9" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="46" t="s">
-        <v>438</v>
+      <c r="O9" s="45" t="s">
+        <v>437</v>
       </c>
       <c r="P9" t="s">
         <v>70</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>623</v>
+        <v>606</v>
       </c>
       <c r="R9" t="s">
         <v>113</v>
@@ -4480,31 +4500,31 @@
         <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>864</v>
+        <v>847</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
       </c>
-      <c r="G10" s="45" t="s">
-        <v>421</v>
+      <c r="G10" s="44" t="s">
+        <v>420</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>816</v>
+        <v>799</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>624</v>
+        <v>607</v>
       </c>
       <c r="R10" t="s">
         <v>71</v>
@@ -4518,25 +4538,25 @@
         <v>77</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D11" t="s">
         <v>78</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>865</v>
+        <v>848</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="45" t="s">
-        <v>422</v>
+      <c r="G11" s="44" t="s">
+        <v>421</v>
       </c>
       <c r="P11" t="s">
         <v>80</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>625</v>
+        <v>608</v>
       </c>
       <c r="R11" t="s">
         <v>76</v>
@@ -4550,25 +4570,25 @@
         <v>82</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>866</v>
+        <v>849</v>
       </c>
       <c r="F12" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="45" t="s">
-        <v>423</v>
+      <c r="G12" s="44" t="s">
+        <v>422</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>626</v>
+        <v>609</v>
       </c>
       <c r="R12" t="s">
         <v>81</v>
@@ -4582,25 +4602,25 @@
         <v>86</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D13" t="s">
         <v>87</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>867</v>
+        <v>850</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="45" t="s">
-        <v>426</v>
+      <c r="G13" s="44" t="s">
+        <v>425</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>781</v>
-      </c>
-      <c r="Q13" s="46" t="s">
-        <v>782</v>
+        <v>764</v>
+      </c>
+      <c r="Q13" s="45" t="s">
+        <v>765</v>
       </c>
       <c r="R13" t="s">
         <v>93</v>
@@ -4614,19 +4634,19 @@
         <v>90</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D14" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>868</v>
+        <v>851</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="45" t="s">
-        <v>427</v>
+      <c r="G14" s="44" t="s">
+        <v>426</v>
       </c>
       <c r="R14" t="s">
         <v>97</v>
@@ -4640,19 +4660,19 @@
         <v>94</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>869</v>
+        <v>852</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="45" t="s">
-        <v>428</v>
+      <c r="G15" s="44" t="s">
+        <v>427</v>
       </c>
       <c r="R15" t="s">
         <v>101</v>
@@ -4666,19 +4686,19 @@
         <v>98</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D16" t="s">
         <v>99</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>870</v>
+        <v>853</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="45" t="s">
-        <v>429</v>
+      <c r="G16" s="44" t="s">
+        <v>428</v>
       </c>
       <c r="R16" t="s">
         <v>105</v>
@@ -4692,19 +4712,19 @@
         <v>102</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D17" t="s">
         <v>103</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="45" t="s">
-        <v>430</v>
+      <c r="G17" s="44" t="s">
+        <v>429</v>
       </c>
       <c r="R17" t="s">
         <v>108</v>
@@ -4715,22 +4735,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>402</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>403</v>
       </c>
       <c r="D18" t="s">
         <v>106</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="45" t="s">
-        <v>431</v>
+      <c r="G18" s="44" t="s">
+        <v>430</v>
       </c>
       <c r="R18" t="s">
         <v>111</v>
@@ -4744,13 +4764,13 @@
         <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>873</v>
+        <v>856</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="45" t="s">
-        <v>433</v>
+      <c r="G19" s="44" t="s">
+        <v>432</v>
       </c>
       <c r="R19" t="s">
         <v>115</v>
@@ -4763,11 +4783,11 @@
       <c r="F20" t="s">
         <v>112</v>
       </c>
-      <c r="G20" s="45" t="s">
-        <v>424</v>
+      <c r="G20" s="44" t="s">
+        <v>423</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4777,8 +4797,8 @@
       <c r="F21" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="45" t="s">
-        <v>425</v>
+      <c r="G21" s="44" t="s">
+        <v>424</v>
       </c>
       <c r="R21" t="s">
         <v>89</v>
@@ -4820,9 +4840,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4927,104 +4947,104 @@
       <c r="B2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>544</v>
+      <c r="C2" s="9" t="s">
+        <v>538</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>562</v>
+        <v>868</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>841</v>
+      <c r="G2" s="9" t="s">
+        <v>824</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>463</v>
+      <c r="I2" s="9" t="s">
+        <v>461</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>676</v>
+      <c r="K2" s="9" t="s">
+        <v>659</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>481</v>
+      <c r="M2" s="9" t="s">
+        <v>479</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>804</v>
+      <c r="O2" s="9" t="s">
+        <v>787</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>805</v>
+      <c r="Q2" s="9" t="s">
+        <v>788</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="S2" s="46" t="s">
-        <v>820</v>
+      <c r="S2" s="48" t="s">
+        <v>803</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="U2" s="8" t="s">
-        <v>821</v>
+      <c r="U2" s="9" t="s">
+        <v>804</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="Y2" s="8" t="s">
-        <v>808</v>
+      <c r="Y2" s="9" t="s">
+        <v>791</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AA2" s="46" t="s">
-        <v>679</v>
+      <c r="AA2" s="48" t="s">
+        <v>662</v>
       </c>
       <c r="AB2" s="5" t="s">
         <v>132</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>150</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="AF2" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="AG2" s="46" t="s">
-        <v>445</v>
+      <c r="AG2" s="45" t="s">
+        <v>444</v>
       </c>
       <c r="AH2" s="5" t="s">
         <v>152</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>458</v>
+        <v>867</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>153</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>678</v>
+        <v>661</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -5034,110 +5054,110 @@
       <c r="B3" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>545</v>
+      <c r="C3" s="9" t="s">
+        <v>539</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>155</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>460</v>
+      <c r="G3" s="9" t="s">
+        <v>458</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>464</v>
+      <c r="I3" s="9" t="s">
+        <v>462</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>826</v>
+      <c r="K3" s="9" t="s">
+        <v>809</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>482</v>
+      <c r="M3" s="9" t="s">
+        <v>480</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>500</v>
+      <c r="O3" s="9" t="s">
+        <v>497</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>501</v>
+      <c r="Q3" s="9" t="s">
+        <v>498</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="S3" s="46" t="s">
-        <v>875</v>
+      <c r="S3" s="48" t="s">
+        <v>858</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="8" t="s">
-        <v>822</v>
+      <c r="U3" s="9" t="s">
+        <v>805</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>618</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>619</v>
+        <v>601</v>
+      </c>
+      <c r="W3" s="9" t="s">
+        <v>602</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="Y3" s="8" t="s">
-        <v>543</v>
+      <c r="Y3" s="9" t="s">
+        <v>537</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="AA3" s="46" t="s">
-        <v>680</v>
+      <c r="AA3" s="48" t="s">
+        <v>663</v>
       </c>
       <c r="AB3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>516</v>
+        <v>878</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="AF3" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AG3" s="46" t="s">
-        <v>446</v>
+      <c r="AG3" s="45" t="s">
+        <v>445</v>
       </c>
       <c r="AH3" s="5" t="s">
         <v>170</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AJ3" s="5" t="s">
         <v>171</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>581</v>
+        <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -5147,104 +5167,105 @@
       <c r="B4" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>546</v>
+      <c r="C4" s="9" t="s">
+        <v>871</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>564</v>
+        <v>869</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>842</v>
+      <c r="G4" s="9" t="s">
+        <v>825</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>465</v>
+      <c r="I4" s="9" t="s">
+        <v>463</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>827</v>
+      <c r="K4" s="9" t="s">
+        <v>810</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="M4" s="8" t="s">
-        <v>483</v>
+      <c r="M4" s="9" t="s">
+        <v>481</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="O4" s="8" t="s">
-        <v>497</v>
+      <c r="O4" s="9" t="s">
+        <v>495</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="Q4" s="8" t="s">
-        <v>509</v>
+      <c r="Q4" s="9" t="s">
+        <v>506</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="S4" s="46" t="s">
-        <v>876</v>
+      <c r="S4" s="48" t="s">
+        <v>859</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="U4" s="8" t="s">
-        <v>823</v>
-      </c>
+      <c r="U4" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="W4" s="5"/>
       <c r="X4" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="Y4" s="8" t="s">
-        <v>541</v>
+      <c r="Y4" s="9" t="s">
+        <v>535</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="AA4" s="46" t="s">
-        <v>532</v>
+      <c r="AA4" s="48" t="s">
+        <v>526</v>
       </c>
       <c r="AB4" s="5" t="s">
         <v>184</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>185</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="AF4" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="AG4" s="46" t="s">
-        <v>447</v>
+      <c r="AG4" s="45" t="s">
+        <v>446</v>
       </c>
       <c r="AH4" t="s">
         <v>187</v>
       </c>
       <c r="AI4" s="8" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="AJ4" s="5" t="s">
         <v>188</v>
       </c>
       <c r="AK4" s="8" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -5254,98 +5275,100 @@
       <c r="B5" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>547</v>
+      <c r="C5" s="9" t="s">
+        <v>540</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>843</v>
+      <c r="G5" s="9" t="s">
+        <v>826</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>466</v>
+      <c r="I5" s="9" t="s">
+        <v>464</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>828</v>
+      <c r="K5" s="9" t="s">
+        <v>811</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>484</v>
+      <c r="M5" s="9" t="s">
+        <v>482</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>498</v>
+      <c r="O5" s="9" t="s">
+        <v>496</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="Q5" s="8" t="s">
-        <v>502</v>
+      <c r="Q5" s="9" t="s">
+        <v>499</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="S5" s="46" t="s">
-        <v>877</v>
-      </c>
+      <c r="S5" s="48" t="s">
+        <v>860</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="W5" s="5"/>
       <c r="X5" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="Y5" s="8" t="s">
-        <v>537</v>
+      <c r="Y5" s="9" t="s">
+        <v>531</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="AA5" s="46" t="s">
-        <v>528</v>
+      <c r="AA5" s="48" t="s">
+        <v>522</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>202</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>518</v>
+        <v>872</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>203</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>560</v>
-      </c>
-      <c r="AF5" s="41" t="s">
+        <v>547</v>
+      </c>
+      <c r="AF5" s="40" t="s">
         <v>204</v>
       </c>
       <c r="AG5" s="8" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AH5" t="s">
         <v>205</v>
       </c>
       <c r="AI5" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AJ5" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="AK5" s="46" t="s">
-        <v>582</v>
+      <c r="AK5" s="45" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -5355,104 +5378,104 @@
       <c r="B6" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>548</v>
+      <c r="C6" s="9" t="s">
+        <v>873</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>844</v>
+      <c r="G6" s="9" t="s">
+        <v>827</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>468</v>
+      <c r="I6" s="9" t="s">
+        <v>466</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>829</v>
+      <c r="K6" s="9" t="s">
+        <v>812</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>486</v>
+      <c r="M6" s="9" t="s">
+        <v>484</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="O6" s="8" t="s">
-        <v>499</v>
+      <c r="O6" s="9" t="s">
+        <v>866</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="Q6" s="8" t="s">
-        <v>508</v>
+      <c r="Q6" s="9" t="s">
+        <v>505</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="S6" s="46" t="s">
-        <v>878</v>
+      <c r="S6" s="48" t="s">
+        <v>861</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="U6" s="8" t="s">
-        <v>824</v>
+      <c r="U6" s="9" t="s">
+        <v>807</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="W6" s="8" t="s">
-        <v>510</v>
+      <c r="W6" s="9" t="s">
+        <v>507</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="Y6" s="8" t="s">
-        <v>534</v>
+      <c r="Y6" s="9" t="s">
+        <v>528</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="AA6" s="46" t="s">
-        <v>525</v>
+      <c r="AA6" s="48" t="s">
+        <v>519</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>220</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>515</v>
+        <v>876</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>221</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="AF6" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="AG6" s="46" t="s">
-        <v>449</v>
+      <c r="AG6" s="45" t="s">
+        <v>448</v>
       </c>
       <c r="AJ6" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="AK6" s="46" t="s">
-        <v>583</v>
+      <c r="AK6" s="45" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -5462,84 +5485,85 @@
       <c r="B7" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>549</v>
+      <c r="C7" s="9" t="s">
+        <v>541</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>225</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>568</v>
+        <v>553</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>845</v>
+      <c r="G7" s="9" t="s">
+        <v>828</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>469</v>
+      <c r="I7" s="9" t="s">
+        <v>467</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>830</v>
+      <c r="K7" s="9" t="s">
+        <v>813</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>485</v>
+      <c r="M7" s="9" t="s">
+        <v>483</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="Q7" s="8" t="s">
-        <v>503</v>
+      <c r="Q7" s="9" t="s">
+        <v>500</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="S7" s="46" t="s">
-        <v>493</v>
-      </c>
+      <c r="S7" s="48" t="s">
+        <v>491</v>
+      </c>
+      <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="Y7" s="8" t="s">
-        <v>542</v>
+      <c r="Y7" s="9" t="s">
+        <v>536</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="AA7" s="46" t="s">
-        <v>533</v>
+      <c r="AA7" s="48" t="s">
+        <v>527</v>
       </c>
       <c r="AB7" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="AC7" s="46" t="s">
-        <v>675</v>
+      <c r="AC7" s="45" t="s">
+        <v>658</v>
       </c>
       <c r="AF7" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="AG7" s="46" t="s">
-        <v>451</v>
+      <c r="AG7" s="45" t="s">
+        <v>450</v>
       </c>
       <c r="AJ7" s="5" t="s">
         <v>237</v>
       </c>
       <c r="AK7" s="8" t="s">
-        <v>584</v>
+        <v>568</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -5549,90 +5573,90 @@
       <c r="B8" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>550</v>
+      <c r="C8" s="9" t="s">
+        <v>870</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>239</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>569</v>
+        <v>554</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>846</v>
+      <c r="G8" s="9" t="s">
+        <v>829</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>473</v>
+      <c r="I8" s="9" t="s">
+        <v>471</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>831</v>
+      <c r="K8" s="9" t="s">
+        <v>814</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="M8" s="8" t="s">
-        <v>487</v>
+      <c r="M8" s="9" t="s">
+        <v>485</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="Q8" s="8" t="s">
-        <v>504</v>
+      <c r="Q8" s="9" t="s">
+        <v>501</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="S8" s="46" t="s">
-        <v>879</v>
+      <c r="S8" s="48" t="s">
+        <v>862</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
       <c r="U8" s="9" t="s">
-        <v>621</v>
+        <v>604</v>
       </c>
       <c r="V8" s="5"/>
-      <c r="W8" s="8"/>
+      <c r="W8" s="9"/>
       <c r="X8" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="Y8" s="8" t="s">
-        <v>540</v>
+      <c r="Y8" s="9" t="s">
+        <v>534</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="AA8" s="46" t="s">
-        <v>531</v>
+      <c r="AA8" s="48" t="s">
+        <v>525</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="AC8" s="46" t="s">
-        <v>520</v>
+      <c r="AC8" s="45" t="s">
+        <v>514</v>
       </c>
       <c r="AF8" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="AG8" s="46" t="s">
-        <v>450</v>
+      <c r="AG8" s="45" t="s">
+        <v>449</v>
       </c>
       <c r="AJ8" s="5" t="s">
         <v>251</v>
       </c>
       <c r="AK8" s="8" t="s">
-        <v>806</v>
+        <v>789</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -5642,84 +5666,85 @@
       <c r="B9" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>551</v>
+      <c r="C9" s="9" t="s">
+        <v>874</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>570</v>
+        <v>555</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>847</v>
+      <c r="G9" s="9" t="s">
+        <v>830</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>467</v>
+      <c r="I9" s="9" t="s">
+        <v>465</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>832</v>
+      <c r="K9" s="9" t="s">
+        <v>815</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>488</v>
+      <c r="M9" s="9" t="s">
+        <v>486</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="Q9" s="8" t="s">
-        <v>505</v>
+      <c r="Q9" s="9" t="s">
+        <v>502</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="S9" s="46" t="s">
-        <v>880</v>
-      </c>
+      <c r="S9" s="48" t="s">
+        <v>863</v>
+      </c>
+      <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="Y9" s="8" t="s">
-        <v>538</v>
+      <c r="Y9" s="9" t="s">
+        <v>532</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AA9" s="46" t="s">
-        <v>529</v>
+      <c r="AA9" s="48" t="s">
+        <v>523</v>
       </c>
       <c r="AB9" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC9" s="46" t="s">
-        <v>521</v>
+      <c r="AC9" s="45" t="s">
+        <v>515</v>
       </c>
       <c r="AF9" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AG9" s="46" t="s">
-        <v>452</v>
+      <c r="AG9" s="45" t="s">
+        <v>451</v>
       </c>
       <c r="AJ9" s="5" t="s">
         <v>265</v>
       </c>
       <c r="AK9" s="8" t="s">
-        <v>585</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -5729,94 +5754,94 @@
       <c r="B10" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>552</v>
+      <c r="C10" s="9" t="s">
+        <v>875</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>267</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>571</v>
+        <v>556</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>461</v>
+      <c r="G10" s="9" t="s">
+        <v>459</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>792</v>
+      <c r="I10" s="9" t="s">
+        <v>775</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>495</v>
+      <c r="K10" s="9" t="s">
+        <v>493</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="M10" s="8" t="s">
-        <v>490</v>
+      <c r="M10" s="9" t="s">
+        <v>488</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="Q10" s="8" t="s">
-        <v>506</v>
+      <c r="Q10" s="9" t="s">
+        <v>503</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="S10" s="46" t="s">
-        <v>881</v>
+      <c r="S10" s="48" t="s">
+        <v>864</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="U10" s="8" t="s">
-        <v>522</v>
+      <c r="U10" s="9" t="s">
+        <v>516</v>
       </c>
       <c r="V10" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="W10" s="8" t="s">
-        <v>511</v>
+      <c r="W10" s="9" t="s">
+        <v>508</v>
       </c>
       <c r="X10" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="Y10" s="8" t="s">
-        <v>535</v>
+      <c r="Y10" s="9" t="s">
+        <v>529</v>
       </c>
       <c r="Z10" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="AA10" s="46" t="s">
-        <v>526</v>
+      <c r="AA10" s="48" t="s">
+        <v>520</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AC10" s="46" t="s">
-        <v>519</v>
+      <c r="AC10" s="45" t="s">
+        <v>513</v>
       </c>
       <c r="AF10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="AG10" s="46" t="s">
-        <v>454</v>
+      <c r="AG10" s="45" t="s">
+        <v>453</v>
       </c>
       <c r="AJ10" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="AK10" s="46" t="s">
-        <v>586</v>
+      <c r="AK10" s="45" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -5826,90 +5851,90 @@
       <c r="B11" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>553</v>
+      <c r="C11" s="9" t="s">
+        <v>542</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>572</v>
+        <v>557</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>848</v>
+      <c r="G11" s="9" t="s">
+        <v>831</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>470</v>
+      <c r="I11" s="9" t="s">
+        <v>468</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>833</v>
+      <c r="K11" s="9" t="s">
+        <v>816</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>491</v>
+      <c r="M11" s="9" t="s">
+        <v>489</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="Q11" s="8" t="s">
-        <v>507</v>
+      <c r="Q11" s="9" t="s">
+        <v>504</v>
       </c>
       <c r="R11" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="S11" s="46" t="s">
-        <v>494</v>
+      <c r="S11" s="45" t="s">
+        <v>492</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="U11" s="8" t="s">
-        <v>523</v>
+      <c r="U11" s="9" t="s">
+        <v>517</v>
       </c>
       <c r="V11" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="W11" s="8" t="s">
-        <v>512</v>
+      <c r="W11" s="9" t="s">
+        <v>509</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="Y11" s="8" t="s">
-        <v>536</v>
+      <c r="Y11" s="9" t="s">
+        <v>530</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="AA11" s="46" t="s">
-        <v>527</v>
+      <c r="AA11" s="45" t="s">
+        <v>521</v>
       </c>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
       <c r="AF11" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="AG11" s="46" t="s">
-        <v>453</v>
+      <c r="AG11" s="45" t="s">
+        <v>452</v>
       </c>
       <c r="AJ11" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="AK11" s="46" t="s">
-        <v>587</v>
+      <c r="AK11" s="45" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -5919,38 +5944,38 @@
       <c r="B12" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>554</v>
+      <c r="C12" s="9" t="s">
+        <v>877</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>292</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>573</v>
+        <v>558</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>849</v>
+      <c r="G12" s="9" t="s">
+        <v>832</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="I12" s="8" t="s">
-        <v>472</v>
+      <c r="I12" s="9" t="s">
+        <v>470</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>834</v>
+      <c r="K12" s="9" t="s">
+        <v>817</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="M12" s="8" t="s">
-        <v>489</v>
+      <c r="M12" s="9" t="s">
+        <v>487</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -5959,28 +5984,28 @@
       <c r="R12" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="S12" s="46" t="s">
-        <v>818</v>
+      <c r="S12" s="48" t="s">
+        <v>801</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="U12" s="8" t="s">
-        <v>825</v>
+      <c r="U12" s="9" t="s">
+        <v>808</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="Y12" s="8" t="s">
-        <v>539</v>
+      <c r="Y12" s="9" t="s">
+        <v>533</v>
       </c>
       <c r="Z12" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="AA12" s="46" t="s">
-        <v>530</v>
+      <c r="AA12" s="48" t="s">
+        <v>524</v>
       </c>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
@@ -5988,13 +6013,13 @@
         <v>300</v>
       </c>
       <c r="AG12" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AJ12" s="5" t="s">
         <v>301</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>588</v>
+        <v>572</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -6004,60 +6029,60 @@
       <c r="B13" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>556</v>
+      <c r="C13" s="9" t="s">
+        <v>543</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>303</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>567</v>
+        <v>552</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>850</v>
+      <c r="G13" s="9" t="s">
+        <v>833</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>791</v>
+      <c r="I13" s="9" t="s">
+        <v>774</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>835</v>
+      <c r="K13" s="9" t="s">
+        <v>818</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="M13" s="8" t="s">
-        <v>492</v>
+      <c r="M13" s="9" t="s">
+        <v>490</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="10" t="s">
-        <v>817</v>
-      </c>
-      <c r="S13" s="46" t="s">
-        <v>819</v>
+        <v>800</v>
+      </c>
+      <c r="S13" s="48" t="s">
+        <v>802</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="U13" s="8" t="s">
-        <v>524</v>
+      <c r="U13" s="9" t="s">
+        <v>518</v>
       </c>
       <c r="V13" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="W13" s="8" t="s">
-        <v>513</v>
+      <c r="W13" s="9" t="s">
+        <v>510</v>
       </c>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -6065,17 +6090,17 @@
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
-      <c r="AF13" s="41" t="s">
-        <v>616</v>
-      </c>
-      <c r="AG13" s="46" t="s">
-        <v>617</v>
+      <c r="AF13" s="40" t="s">
+        <v>599</v>
+      </c>
+      <c r="AG13" s="45" t="s">
+        <v>600</v>
       </c>
       <c r="AJ13" s="5" t="s">
         <v>308</v>
       </c>
       <c r="AK13" s="8" t="s">
-        <v>589</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -6085,32 +6110,32 @@
       <c r="B14" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>555</v>
+      <c r="C14" s="9" t="s">
+        <v>879</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>574</v>
+        <v>880</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>851</v>
+      <c r="G14" s="9" t="s">
+        <v>834</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>790</v>
+      <c r="I14" s="9" t="s">
+        <v>773</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>836</v>
+      <c r="K14" s="9" t="s">
+        <v>819</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6135,7 +6160,7 @@
         <v>314</v>
       </c>
       <c r="AK14" s="8" t="s">
-        <v>590</v>
+        <v>574</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -6149,20 +6174,20 @@
       <c r="F15" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>852</v>
+      <c r="G15" s="9" t="s">
+        <v>835</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>474</v>
+      <c r="I15" s="9" t="s">
+        <v>472</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="K15" s="8" t="s">
-        <v>837</v>
+      <c r="K15" s="9" t="s">
+        <v>820</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -6184,7 +6209,7 @@
         <v>318</v>
       </c>
       <c r="AK15" s="8" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
@@ -6198,20 +6223,20 @@
       <c r="F16" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>853</v>
+      <c r="G16" s="9" t="s">
+        <v>836</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>475</v>
+      <c r="I16" s="9" t="s">
+        <v>473</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="K16" s="8" t="s">
-        <v>838</v>
+      <c r="K16" s="9" t="s">
+        <v>821</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -6232,8 +6257,8 @@
       <c r="AJ16" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="AK16" s="46" t="s">
-        <v>592</v>
+      <c r="AK16" s="45" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -6247,20 +6272,20 @@
       <c r="F17" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>854</v>
+      <c r="G17" s="9" t="s">
+        <v>837</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>476</v>
+      <c r="I17" s="9" t="s">
+        <v>474</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="K17" s="8" t="s">
-        <v>839</v>
+      <c r="K17" s="9" t="s">
+        <v>822</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -6279,10 +6304,10 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AJ17" s="10" t="s">
-        <v>575</v>
-      </c>
-      <c r="AK17" s="46" t="s">
-        <v>578</v>
+        <v>559</v>
+      </c>
+      <c r="AK17" s="45" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -6296,20 +6321,20 @@
       <c r="F18" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>855</v>
+      <c r="G18" s="9" t="s">
+        <v>838</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>477</v>
+      <c r="I18" s="9" t="s">
+        <v>475</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="K18" s="8" t="s">
-        <v>840</v>
+      <c r="K18" s="9" t="s">
+        <v>823</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -6328,10 +6353,10 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AJ18" s="10" t="s">
-        <v>576</v>
-      </c>
-      <c r="AK18" s="46" t="s">
-        <v>579</v>
+        <v>560</v>
+      </c>
+      <c r="AK18" s="45" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -6345,20 +6370,20 @@
       <c r="F19" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>856</v>
+      <c r="G19" s="9" t="s">
+        <v>839</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>793</v>
+      <c r="I19" s="9" t="s">
+        <v>776</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="K19" s="8" t="s">
-        <v>496</v>
+      <c r="K19" s="9" t="s">
+        <v>494</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -6379,10 +6404,10 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AJ19" s="10" t="s">
-        <v>627</v>
-      </c>
-      <c r="AK19" s="46" t="s">
-        <v>628</v>
+        <v>610</v>
+      </c>
+      <c r="AK19" s="45" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -6396,14 +6421,14 @@
       <c r="F20" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>462</v>
+      <c r="G20" s="9" t="s">
+        <v>460</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>471</v>
+      <c r="I20" s="9" t="s">
+        <v>469</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -6426,10 +6451,10 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AJ20" s="10" t="s">
-        <v>577</v>
-      </c>
-      <c r="AK20" s="46" t="s">
-        <v>580</v>
+        <v>561</v>
+      </c>
+      <c r="AK20" s="45" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -6443,14 +6468,14 @@
       <c r="F21" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>813</v>
+      <c r="G21" s="9" t="s">
+        <v>796</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>479</v>
+      <c r="I21" s="9" t="s">
+        <v>477</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -6473,10 +6498,10 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AJ21" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="AK21" s="46" t="s">
-        <v>596</v>
+        <v>578</v>
+      </c>
+      <c r="AK21" s="45" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -6492,8 +6517,8 @@
       <c r="H22" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>480</v>
+      <c r="I22" s="9" t="s">
+        <v>478</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -6516,10 +6541,10 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AJ22" s="10" t="s">
-        <v>641</v>
-      </c>
-      <c r="AK22" s="46" t="s">
-        <v>644</v>
+        <v>624</v>
+      </c>
+      <c r="AK22" s="45" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.3">
@@ -6532,14 +6557,14 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" t="s">
+      <c r="H23" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>593</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>794</v>
+      <c r="I23" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>777</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -6561,10 +6586,10 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AJ23" s="10" t="s">
-        <v>642</v>
-      </c>
-      <c r="AK23" s="46" t="s">
-        <v>645</v>
+        <v>625</v>
+      </c>
+      <c r="AK23" s="45" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -6577,12 +6602,13 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" t="s">
+      <c r="H24" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>795</v>
-      </c>
+      <c r="I24" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -6603,10 +6629,10 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AJ24" s="16" t="s">
-        <v>643</v>
-      </c>
-      <c r="AK24" s="46" t="s">
-        <v>646</v>
+        <v>626</v>
+      </c>
+      <c r="AK24" s="45" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -6623,7 +6649,7 @@
         <v>339</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -6645,10 +6671,10 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AJ25" s="21" t="s">
-        <v>653</v>
+        <v>636</v>
       </c>
       <c r="AK25" s="9" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.3">
@@ -6665,10 +6691,10 @@
         <v>340</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>594</v>
+        <v>881</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>796</v>
+        <v>779</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -6690,10 +6716,10 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AJ26" s="16" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="AK26" s="9" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -6703,12 +6729,12 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="42" t="s">
-        <v>797</v>
-      </c>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42" t="s">
-        <v>798</v>
+      <c r="H27" s="41" t="s">
+        <v>780</v>
+      </c>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41" t="s">
+        <v>781</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -6730,10 +6756,10 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AJ27" s="16" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
       <c r="AK27" s="9" t="s">
-        <v>659</v>
+        <v>642</v>
       </c>
     </row>
     <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -6743,12 +6769,12 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="42" t="s">
-        <v>799</v>
-      </c>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42" t="s">
-        <v>800</v>
+      <c r="H28" s="41" t="s">
+        <v>782</v>
+      </c>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41" t="s">
+        <v>783</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -6769,19 +6795,19 @@
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
-      <c r="AJ28" s="40" t="s">
-        <v>656</v>
+      <c r="AJ28" s="39" t="s">
+        <v>639</v>
       </c>
       <c r="AK28" s="9" t="s">
-        <v>660</v>
+        <v>643</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="AJ29" s="39" t="s">
-        <v>783</v>
+      <c r="AJ29" s="38" t="s">
+        <v>766</v>
       </c>
       <c r="AK29" s="9" t="s">
-        <v>784</v>
+        <v>767</v>
       </c>
     </row>
   </sheetData>
@@ -6796,8 +6822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -6814,7 +6840,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
-        <v>682</v>
+        <v>665</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6836,11 +6862,11 @@
       <c r="B3" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="C3" s="46" t="s">
-        <v>600</v>
+      <c r="C3" s="45" t="s">
+        <v>583</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>614</v>
+        <v>597</v>
       </c>
       <c r="E3" t="s">
         <v>345</v>
@@ -6858,7 +6884,7 @@
         <v>349</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>615</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6868,11 +6894,11 @@
       <c r="B4" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>601</v>
+      <c r="C4" s="45" t="s">
+        <v>584</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>614</v>
+        <v>597</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6882,11 +6908,11 @@
       <c r="B5" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="C5" s="46" t="s">
-        <v>602</v>
+      <c r="C5" s="45" t="s">
+        <v>585</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>614</v>
+        <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6896,11 +6922,11 @@
       <c r="B6" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="46" t="s">
-        <v>597</v>
+      <c r="C6" s="45" t="s">
+        <v>580</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>633</v>
+        <v>616</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -6911,22 +6937,22 @@
         <v>353</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>598</v>
+        <v>581</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>634</v>
+        <v>617</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>629</v>
+        <v>612</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>630</v>
+        <v>613</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>631</v>
+        <v>614</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>632</v>
+        <v>615</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6934,13 +6960,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>651</v>
+        <v>634</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>599</v>
+        <v>582</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>640</v>
+        <v>623</v>
       </c>
       <c r="E8" t="s">
         <v>354</v>
@@ -6949,7 +6975,7 @@
         <v>355</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>677</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -6957,13 +6983,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>671</v>
+        <v>654</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>603</v>
+        <v>586</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>636</v>
+        <v>619</v>
       </c>
       <c r="E9" t="s">
         <v>356</v>
@@ -6977,10 +7003,10 @@
         <v>357</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>637</v>
+        <v>620</v>
       </c>
       <c r="E10" t="s">
         <v>358</v>
@@ -6990,14 +7016,14 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>650</v>
+      <c r="B11" s="42" t="s">
+        <v>633</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>605</v>
+        <v>588</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="E11" t="s">
         <v>359</v>
@@ -7013,14 +7039,14 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>672</v>
+      <c r="B12" s="42" t="s">
+        <v>655</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>606</v>
+        <v>589</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>639</v>
+        <v>622</v>
       </c>
       <c r="E12" t="s">
         <v>362</v>
@@ -7031,27 +7057,27 @@
         <v>11</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>607</v>
+        <v>590</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="43" t="s">
-        <v>673</v>
+      <c r="B14" s="42" t="s">
+        <v>656</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>635</v>
+        <v>618</v>
       </c>
       <c r="E14" t="s">
         <v>133</v>
@@ -7075,7 +7101,7 @@
         <v>364</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>652</v>
+        <v>635</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7086,10 +7112,10 @@
         <v>365</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>609</v>
+        <v>592</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
       <c r="E15" t="s">
         <v>366</v>
@@ -7103,10 +7129,10 @@
         <v>367</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>610</v>
+        <v>593</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
       <c r="E16" t="s">
         <v>368</v>
@@ -7141,16 +7167,16 @@
         <v>373</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>695</v>
+        <v>678</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>696</v>
+        <v>679</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -7163,21 +7189,21 @@
       <c r="A20" s="23">
         <v>2</v>
       </c>
-      <c r="B20" s="47" t="s">
-        <v>699</v>
+      <c r="B20" s="46" t="s">
+        <v>682</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>700</v>
+        <v>683</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>701</v>
+        <v>684</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="27" t="s">
         <v>374</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
@@ -7189,18 +7215,18 @@
       <c r="A21" s="23">
         <v>3</v>
       </c>
-      <c r="B21" s="47" t="s">
-        <v>703</v>
+      <c r="B21" s="46" t="s">
+        <v>686</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>705</v>
+        <v>688</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="27" t="s">
-        <v>706</v>
+        <v>689</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>375</v>
@@ -7215,33 +7241,33 @@
       <c r="A22" s="23">
         <v>4</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>694</v>
+      <c r="B22" s="47" t="s">
+        <v>677</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>707</v>
+        <v>690</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>709</v>
+        <v>692</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>376</v>
+        <v>865</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="22" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="K22" s="28" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="L22" s="28"/>
     </row>
@@ -7249,31 +7275,31 @@
       <c r="A23" s="23">
         <v>5</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>377</v>
+      <c r="B23" s="46" t="s">
+        <v>376</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>713</v>
+        <v>696</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>714</v>
+        <v>697</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="23"/>
       <c r="G23" s="32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>715</v>
+        <v>698</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="L23" s="28"/>
     </row>
@@ -7282,17 +7308,17 @@
         <v>6</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>716</v>
+        <v>699</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>717</v>
+        <v>700</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>718</v>
+        <v>701</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="23" t="s">
-        <v>719</v>
+        <v>702</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -7305,35 +7331,35 @@
       <c r="A25" s="23">
         <v>7</v>
       </c>
-      <c r="B25" s="29" t="s">
-        <v>720</v>
+      <c r="B25" s="46" t="s">
+        <v>703</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>721</v>
+        <v>704</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>722</v>
+        <v>705</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>723</v>
+        <v>706</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>724</v>
+        <v>707</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>725</v>
+        <v>708</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>726</v>
+        <v>709</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
       <c r="L25" s="28"/>
     </row>
@@ -7342,37 +7368,37 @@
         <v>8</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>727</v>
+        <v>710</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>728</v>
+        <v>711</v>
       </c>
       <c r="D26" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>379</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>674</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>675</v>
+      </c>
+      <c r="J26" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>379</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>380</v>
-      </c>
-      <c r="H26" s="27" t="s">
-        <v>691</v>
-      </c>
-      <c r="I26" s="27" t="s">
-        <v>692</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>710</v>
-      </c>
       <c r="K26" s="22" t="s">
-        <v>729</v>
+        <v>712</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="117" x14ac:dyDescent="0.3">
@@ -7380,27 +7406,27 @@
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>730</v>
+        <v>713</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>687</v>
+        <v>670</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="23" t="s">
-        <v>731</v>
+        <v>714</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
@@ -7409,30 +7435,30 @@
       <c r="A28" s="23">
         <v>10</v>
       </c>
-      <c r="B28" s="29" t="s">
-        <v>732</v>
+      <c r="B28" s="46" t="s">
+        <v>715</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>733</v>
+        <v>716</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>734</v>
+        <v>717</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="23" t="s">
-        <v>735</v>
+        <v>718</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H28" s="22" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
@@ -7442,29 +7468,29 @@
         <v>11</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>736</v>
+        <v>719</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>737</v>
+        <v>720</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>738</v>
+        <v>721</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="23" t="s">
-        <v>739</v>
+        <v>722</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
@@ -7474,23 +7500,23 @@
         <v>12</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>740</v>
+        <v>723</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>741</v>
+        <v>724</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="23" t="s">
-        <v>742</v>
+        <v>725</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>746</v>
+        <v>729</v>
       </c>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
@@ -7502,16 +7528,16 @@
         <v>13</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>743</v>
+        <v>726</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>611</v>
+        <v>594</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -7526,16 +7552,16 @@
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>744</v>
+        <v>727</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>612</v>
+        <v>595</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>745</v>
+        <v>728</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
@@ -7550,13 +7576,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>683</v>
+        <v>666</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>685</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -7576,182 +7602,182 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="37"/>
-    <col min="2" max="2" width="20.08203125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="37"/>
-    <col min="4" max="4" width="34.4140625" style="37" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="37"/>
-    <col min="6" max="6" width="27.25" style="37" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="37"/>
-    <col min="8" max="8" width="29.75" style="37" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="36"/>
+    <col min="2" max="2" width="20.08203125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="36"/>
+    <col min="4" max="4" width="34.4140625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="36"/>
+    <col min="6" max="6" width="27.25" style="36" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="36"/>
+    <col min="8" max="8" width="29.75" style="36" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="36" customWidth="1"/>
     <col min="10" max="10" width="8.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>747</v>
+        <v>730</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>748</v>
+        <v>731</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>749</v>
+        <v>732</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>734</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>736</v>
+      </c>
+      <c r="G3" s="36">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="G4" s="36">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+      <c r="D5" s="37" t="s">
+        <v>753</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>739</v>
+      </c>
+      <c r="G5" s="36">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+      <c r="D6" s="37" t="s">
+        <v>754</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>758</v>
+      </c>
+      <c r="G6" s="36">
+        <v>4</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>746</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>751</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>753</v>
-      </c>
-      <c r="G3" s="37">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
-      <c r="G4" s="37">
-        <v>2</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
-      <c r="D5" s="38" t="s">
-        <v>770</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>756</v>
-      </c>
-      <c r="G5" s="37">
-        <v>3</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
-      <c r="D6" s="38" t="s">
-        <v>771</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>775</v>
-      </c>
-      <c r="G6" s="37">
-        <v>4</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>763</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
-        <v>773</v>
+        <v>756</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>754</v>
-      </c>
-      <c r="G7" s="37">
+        <v>737</v>
+      </c>
+      <c r="G7" s="36">
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>761</v>
+        <v>744</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>755</v>
-      </c>
-      <c r="G8" s="37">
+        <v>738</v>
+      </c>
+      <c r="G8" s="36">
         <v>6</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>762</v>
+        <v>745</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
-      <c r="D9" s="38" t="s">
-        <v>774</v>
+      <c r="D9" s="37" t="s">
+        <v>757</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>776</v>
-      </c>
-      <c r="G9" s="37">
+        <v>759</v>
+      </c>
+      <c r="G9" s="36">
         <v>7</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D10" s="13" t="s">
-        <v>786</v>
+        <v>769</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>767</v>
-      </c>
-      <c r="G10" s="37">
+        <v>750</v>
+      </c>
+      <c r="G10" s="36">
         <v>8</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>765</v>
+        <v>748</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="F11" s="13" t="s">
-        <v>757</v>
-      </c>
-      <c r="G11" s="37">
+        <v>740</v>
+      </c>
+      <c r="G11" s="36">
         <v>9</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D12" s="13" t="s">
-        <v>785</v>
-      </c>
-      <c r="G12" s="37">
+        <v>768</v>
+      </c>
+      <c r="G12" s="36">
         <v>10</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>769</v>
+        <v>752</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
-        <v>787</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>801</v>
+        <v>770</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>784</v>
       </c>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
-      <c r="F14" s="44" t="s">
-        <v>802</v>
+      <c r="F14" s="43" t="s">
+        <v>785</v>
       </c>
     </row>
   </sheetData>
@@ -7778,7 +7804,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7786,7 +7812,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -7812,7 +7838,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -7820,7 +7846,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7828,7 +7854,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7836,7 +7862,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>669</v>
+        <v>652</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7844,7 +7870,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -7852,7 +7878,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>665</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7860,7 +7886,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -7868,7 +7894,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7876,7 +7902,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>670</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another day, another fish
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbydd\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FFBB9C-D132-48DD-BED3-7DA3D32170ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FA7EE8-A5D3-4E23-BEF9-B36C676DB843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1965,7 +1965,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1976,7 +1976,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2059,7 +2059,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2076,7 +2076,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2087,7 +2087,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2097,7 +2097,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2108,7 +2108,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2118,7 +2118,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2129,7 +2129,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2149,7 +2149,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2165,7 +2165,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2175,7 +2175,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2200,7 +2200,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2210,7 +2210,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2510,7 +2510,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2724,18 +2724,6 @@
   </si>
   <si>
     <t>conveyer_belt_1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>pipe_1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>pipe_2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>pipe_3</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -2774,7 +2762,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2784,7 +2772,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2795,7 +2783,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2805,7 +2793,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3253,16 +3241,25 @@
     <t>ss_additive</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>pipe_invar</t>
+  </si>
+  <si>
+    <t>pipe_stainless_steel</t>
+  </si>
+  <si>
+    <t>pipe_tungsten_steel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -3270,27 +3267,27 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3303,7 +3300,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3325,7 +3322,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3333,7 +3330,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3341,7 +3338,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3349,7 +3346,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3358,7 +3355,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4033,31 +4030,31 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q2" sqref="Q2:Q13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N13" sqref="N13:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="24.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.75" customWidth="1"/>
-    <col min="6" max="6" width="12.75" customWidth="1"/>
-    <col min="7" max="7" width="28.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.4140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.58203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08203125" customWidth="1"/>
-    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.08203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="3" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4086,7 +4083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4100,7 +4097,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -4118,7 +4115,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -4130,7 +4127,7 @@
         <v>15</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
@@ -4142,7 +4139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4156,7 +4153,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -4186,7 +4183,7 @@
         <v>24</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
@@ -4198,7 +4195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4212,7 +4209,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -4236,13 +4233,13 @@
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
@@ -4254,7 +4251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4268,7 +4265,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
@@ -4298,19 +4295,19 @@
         <v>42</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>761</v>
+        <v>879</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4324,7 +4321,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -4342,7 +4339,7 @@
         <v>49</v>
       </c>
       <c r="M6" s="45" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
@@ -4354,13 +4351,13 @@
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>762</v>
+        <v>880</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4374,7 +4371,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
@@ -4398,13 +4395,13 @@
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>763</v>
+        <v>881</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4418,7 +4415,7 @@
         <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
@@ -4427,7 +4424,7 @@
         <v>419</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="M8" s="45" t="s">
         <v>438</v>
@@ -4448,7 +4445,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4462,7 +4459,7 @@
         <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
@@ -4492,7 +4489,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4506,7 +4503,7 @@
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
@@ -4518,7 +4515,7 @@
         <v>630</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
@@ -4530,7 +4527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4544,7 +4541,7 @@
         <v>78</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
@@ -4562,7 +4559,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4576,7 +4573,7 @@
         <v>83</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="F12" t="s">
         <v>84</v>
@@ -4594,7 +4591,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4608,7 +4605,7 @@
         <v>87</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
@@ -4617,16 +4614,16 @@
         <v>425</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="Q13" s="45" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="R13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4640,7 +4637,7 @@
         <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -4652,7 +4649,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4666,7 +4663,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -4678,7 +4675,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4692,7 +4689,7 @@
         <v>99</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -4704,7 +4701,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4718,7 +4715,7 @@
         <v>103</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
@@ -4730,7 +4727,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4744,7 +4741,7 @@
         <v>106</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
@@ -4756,7 +4753,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4764,7 +4761,7 @@
         <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
@@ -4776,7 +4773,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4790,7 +4787,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4804,7 +4801,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4812,7 +4809,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4820,7 +4817,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4841,50 +4838,50 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G21" sqref="G21"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP20" sqref="AP20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="22.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" customWidth="1"/>
-    <col min="5" max="5" width="30.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" customWidth="1"/>
-    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.75" customWidth="1"/>
-    <col min="9" max="9" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.75" customWidth="1"/>
-    <col min="11" max="11" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.75" customWidth="1"/>
-    <col min="13" max="13" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.75" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.75" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="29.08203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.75" customWidth="1"/>
-    <col min="21" max="21" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.75" customWidth="1"/>
-    <col min="23" max="23" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.75" customWidth="1"/>
-    <col min="25" max="25" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.75" customWidth="1"/>
-    <col min="27" max="27" width="25.08203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.75" customWidth="1"/>
-    <col min="29" max="29" width="22.08203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.75" customWidth="1"/>
-    <col min="31" max="31" width="7.58203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.75" customWidth="1"/>
-    <col min="33" max="33" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" customWidth="1"/>
+    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" customWidth="1"/>
+    <col min="27" max="27" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" customWidth="1"/>
+    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.7109375" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" customWidth="1"/>
+    <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="15" customWidth="1"/>
-    <col min="37" max="37" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" s="3" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
@@ -4940,7 +4937,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4954,13 +4951,13 @@
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>140</v>
@@ -4984,31 +4981,31 @@
         <v>143</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
       <c r="S2" s="48" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>181</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
@@ -5038,7 +5035,7 @@
         <v>152</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>153</v>
@@ -5047,7 +5044,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5079,7 +5076,7 @@
         <v>158</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
@@ -5103,13 +5100,13 @@
         <v>162</v>
       </c>
       <c r="S3" s="48" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>198</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>601</v>
@@ -5133,7 +5130,7 @@
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
@@ -5160,7 +5157,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5168,19 +5165,19 @@
         <v>172</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>175</v>
@@ -5192,7 +5189,7 @@
         <v>176</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
@@ -5216,13 +5213,13 @@
         <v>180</v>
       </c>
       <c r="S4" s="48" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>232</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="5" t="s">
@@ -5268,7 +5265,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5288,7 +5285,7 @@
         <v>191</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>192</v>
@@ -5300,7 +5297,7 @@
         <v>193</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>194</v>
@@ -5324,7 +5321,7 @@
         <v>197</v>
       </c>
       <c r="S5" s="48" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="U5" s="5"/>
       <c r="W5" s="5"/>
@@ -5344,7 +5341,7 @@
         <v>202</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>203</v>
@@ -5371,7 +5368,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5379,7 +5376,7 @@
         <v>207</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -5391,7 +5388,7 @@
         <v>209</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>210</v>
@@ -5403,7 +5400,7 @@
         <v>211</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>212</v>
@@ -5415,7 +5412,7 @@
         <v>213</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>214</v>
@@ -5427,13 +5424,13 @@
         <v>215</v>
       </c>
       <c r="S6" s="48" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>260</v>
       </c>
       <c r="U6" s="9" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>217</v>
@@ -5457,7 +5454,7 @@
         <v>220</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>221</v>
@@ -5478,7 +5475,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5498,7 +5495,7 @@
         <v>226</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>227</v>
@@ -5510,7 +5507,7 @@
         <v>228</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>229</v>
@@ -5566,7 +5563,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5574,7 +5571,7 @@
         <v>238</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>239</v>
@@ -5586,7 +5583,7 @@
         <v>240</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>241</v>
@@ -5598,7 +5595,7 @@
         <v>242</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>243</v>
@@ -5618,7 +5615,7 @@
         <v>245</v>
       </c>
       <c r="S8" s="48" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="T8" s="10" t="s">
         <v>603</v>
@@ -5656,10 +5653,10 @@
         <v>251</v>
       </c>
       <c r="AK8" s="8" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5667,7 +5664,7 @@
         <v>252</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>253</v>
@@ -5679,7 +5676,7 @@
         <v>254</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>255</v>
@@ -5691,7 +5688,7 @@
         <v>256</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>257</v>
@@ -5711,7 +5708,7 @@
         <v>259</v>
       </c>
       <c r="S9" s="48" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -5747,7 +5744,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5755,7 +5752,7 @@
         <v>266</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>267</v>
@@ -5773,7 +5770,7 @@
         <v>269</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>270</v>
@@ -5799,7 +5796,7 @@
         <v>273</v>
       </c>
       <c r="S10" s="48" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>146</v>
@@ -5844,7 +5841,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5864,7 +5861,7 @@
         <v>281</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>282</v>
@@ -5876,7 +5873,7 @@
         <v>283</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>284</v>
@@ -5937,7 +5934,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5945,7 +5942,7 @@
         <v>291</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>292</v>
@@ -5957,7 +5954,7 @@
         <v>293</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>294</v>
@@ -5969,7 +5966,7 @@
         <v>295</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>296</v>
@@ -5985,13 +5982,13 @@
         <v>297</v>
       </c>
       <c r="S12" s="48" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>216</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -6022,7 +6019,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6042,19 +6039,19 @@
         <v>304</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>305</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>306</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>307</v>
@@ -6067,10 +6064,10 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="10" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="S13" s="48" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>163</v>
@@ -6103,7 +6100,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:37">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6111,31 +6108,31 @@
         <v>309</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>311</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>312</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>313</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6163,7 +6160,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6175,7 +6172,7 @@
         <v>315</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>316</v>
@@ -6187,7 +6184,7 @@
         <v>317</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -6212,7 +6209,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6224,7 +6221,7 @@
         <v>319</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>320</v>
@@ -6236,7 +6233,7 @@
         <v>321</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -6261,7 +6258,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6273,7 +6270,7 @@
         <v>323</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>324</v>
@@ -6285,7 +6282,7 @@
         <v>325</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -6310,7 +6307,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6322,7 +6319,7 @@
         <v>326</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>327</v>
@@ -6334,7 +6331,7 @@
         <v>328</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -6359,7 +6356,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6371,13 +6368,13 @@
         <v>329</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>330</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>331</v>
@@ -6410,7 +6407,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6457,7 +6454,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:37">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6469,7 +6466,7 @@
         <v>334</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>335</v>
@@ -6504,7 +6501,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:37">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6547,7 +6544,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:37">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6564,7 +6561,7 @@
         <v>577</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -6592,7 +6589,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:37">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6606,7 +6603,7 @@
         <v>338</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -6635,7 +6632,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:37" ht="75">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6677,7 +6674,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:37">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6691,10 +6688,10 @@
         <v>340</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -6722,7 +6719,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -6730,11 +6727,11 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="41" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="I27" s="41"/>
       <c r="J27" s="41" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -6762,7 +6759,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" ht="60">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -6770,11 +6767,11 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="41" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="I28" s="41"/>
       <c r="J28" s="41" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -6802,12 +6799,12 @@
         <v>643</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37">
       <c r="AJ29" s="38" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="AK29" s="9" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -6822,28 +6819,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.08203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.08203125" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.140625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="19.25" customWidth="1"/>
-    <col min="7" max="7" width="20.75" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="B1" s="15" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="B2" s="17" t="s">
         <v>341</v>
       </c>
@@ -6855,7 +6852,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6887,7 +6884,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -6901,7 +6898,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -6915,7 +6912,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -6929,7 +6926,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="57" customHeight="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -6955,7 +6952,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -6978,7 +6975,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -6995,7 +6992,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -7012,7 +7009,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -7035,7 +7032,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -7052,7 +7049,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="90">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -7063,10 +7060,10 @@
         <v>590</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -7104,7 +7101,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -7121,7 +7118,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -7138,10 +7135,10 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="17" t="s">
         <v>369</v>
       </c>
@@ -7159,7 +7156,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="138" customHeight="1">
       <c r="A19" s="23">
         <v>1</v>
       </c>
@@ -7185,7 +7182,7 @@
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
     </row>
-    <row r="20" spans="1:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="30">
       <c r="A20" s="23">
         <v>2</v>
       </c>
@@ -7211,7 +7208,7 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="30">
       <c r="A21" s="23">
         <v>3</v>
       </c>
@@ -7237,7 +7234,7 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
     </row>
-    <row r="22" spans="1:12" ht="117" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="140.25">
       <c r="A22" s="23">
         <v>4</v>
       </c>
@@ -7257,7 +7254,7 @@
         <v>692</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="22" t="s">
@@ -7271,7 +7268,7 @@
       </c>
       <c r="L22" s="28"/>
     </row>
-    <row r="23" spans="1:12" ht="117" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="140.25">
       <c r="A23" s="23">
         <v>5</v>
       </c>
@@ -7303,7 +7300,7 @@
       </c>
       <c r="L23" s="28"/>
     </row>
-    <row r="24" spans="1:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="45">
       <c r="A24" s="23">
         <v>6</v>
       </c>
@@ -7327,7 +7324,7 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
     </row>
-    <row r="25" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="105">
       <c r="A25" s="23">
         <v>7</v>
       </c>
@@ -7363,7 +7360,7 @@
       </c>
       <c r="L25" s="28"/>
     </row>
-    <row r="26" spans="1:12" ht="196" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="255">
       <c r="A26" s="23">
         <v>8</v>
       </c>
@@ -7401,7 +7398,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="117" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="127.5">
       <c r="A27" s="23">
         <v>9</v>
       </c>
@@ -7431,7 +7428,7 @@
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
     </row>
-    <row r="28" spans="1:12" ht="117" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="127.5">
       <c r="A28" s="23">
         <v>10</v>
       </c>
@@ -7463,7 +7460,7 @@
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
     </row>
-    <row r="29" spans="1:12" ht="117" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="127.5">
       <c r="A29" s="23">
         <v>11</v>
       </c>
@@ -7495,7 +7492,7 @@
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
     </row>
-    <row r="30" spans="1:12" ht="168" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="210">
       <c r="A30" s="23">
         <v>12</v>
       </c>
@@ -7513,7 +7510,7 @@
         <v>725</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="H30" s="28" t="s">
         <v>729</v>
@@ -7523,7 +7520,7 @@
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
     </row>
-    <row r="31" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="23">
         <v>13</v>
       </c>
@@ -7547,7 +7544,7 @@
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
     </row>
-    <row r="32" spans="1:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="30">
       <c r="A32" s="23">
         <v>14</v>
       </c>
@@ -7571,7 +7568,7 @@
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="2">
         <v>15</v>
       </c>
@@ -7600,26 +7597,26 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="36"/>
-    <col min="2" max="2" width="20.08203125" style="36" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="36"/>
-    <col min="4" max="4" width="34.4140625" style="36" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="36"/>
-    <col min="6" max="6" width="27.25" style="36" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="36"/>
-    <col min="8" max="8" width="29.75" style="36" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="8.08203125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="36"/>
+    <col min="2" max="2" width="20.140625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="36"/>
+    <col min="4" max="4" width="34.42578125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="36"/>
+    <col min="6" max="6" width="27.28515625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="36"/>
+    <col min="8" max="8" width="29.7109375" style="36" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="36" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30">
       <c r="A1" s="13" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="B2" s="13" t="s">
         <v>731</v>
       </c>
@@ -7631,7 +7628,7 @@
       </c>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="45">
       <c r="B3" s="13" t="s">
         <v>732</v>
       </c>
@@ -7648,7 +7645,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30">
       <c r="G4" s="36">
         <v>2</v>
       </c>
@@ -7656,7 +7653,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30">
       <c r="D5" s="37" t="s">
         <v>753</v>
       </c>
@@ -7670,7 +7667,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="90">
       <c r="D6" s="37" t="s">
         <v>754</v>
       </c>
@@ -7687,7 +7684,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="150">
       <c r="D7" s="13" t="s">
         <v>756</v>
       </c>
@@ -7701,7 +7698,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="60">
       <c r="D8" s="13" t="s">
         <v>755</v>
       </c>
@@ -7716,7 +7713,7 @@
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="105">
       <c r="D9" s="37" t="s">
         <v>757</v>
       </c>
@@ -7730,9 +7727,9 @@
         <v>747</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="60">
       <c r="D10" s="13" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>750</v>
@@ -7744,7 +7741,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30">
       <c r="F11" s="13" t="s">
         <v>740</v>
       </c>
@@ -7755,9 +7752,9 @@
         <v>749</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30">
       <c r="D12" s="13" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="G12" s="36">
         <v>10</v>
@@ -7766,18 +7763,18 @@
         <v>752</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="45">
       <c r="D13" s="13" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="45">
       <c r="F14" s="43" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
   </sheetData>
@@ -7796,18 +7793,18 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="21.95" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7826,22 +7823,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082DB092-EC3A-4409-8021-838227EE44A2}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="B1" s="7" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7849,7 +7846,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7857,7 +7854,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7865,7 +7862,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7873,7 +7870,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7881,7 +7878,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7889,7 +7886,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7897,7 +7894,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
2021.10.10 11.57 for bug修复
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbydd\IdeaProjects\micro_machinery\参考\资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FA7EE8-A5D3-4E23-BEF9-B36C676DB843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38F503A-2430-4605-BB8B-14976D9C9FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -1265,9 +1265,6 @@
     <t>破碎用转轴</t>
   </si>
   <si>
-    <t>原矿→2粉碎矿石；锭→粉；齿轮→4粉；齿轮坯→4粉；圆形铸件→9粉；块→9粉；管道→3粉；机械方块→对应板材粉末；石头→圆石；圆石→砂砾；砂砾→沙子；石英→硅粉；骨头→6骨粉；红石矿石→12红石粉+石粉；青金石矿石→8青金石+石粉；石英矿石→4石英+石粉；钻石矿石→4钻石+石粉；煤矿石→4煤粉+石粉</t>
-  </si>
-  <si>
     <t>粉碎矿石→精矿+石粉+概率金属粉</t>
   </si>
   <si>
@@ -1965,7 +1962,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1976,7 +1973,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2059,7 +2056,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2076,7 +2073,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2087,7 +2084,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2097,7 +2094,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2108,7 +2105,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2118,7 +2115,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2129,7 +2126,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2149,7 +2146,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2165,7 +2162,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2175,7 +2172,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2200,7 +2197,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2210,7 +2207,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2510,7 +2507,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2724,6 +2721,18 @@
   </si>
   <si>
     <t>conveyer_belt_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pipe_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pipe_2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>pipe_3</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -2762,7 +2771,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2772,7 +2781,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2783,7 +2792,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -2793,7 +2802,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3242,24 +3251,19 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>pipe_invar</t>
-  </si>
-  <si>
-    <t>pipe_stainless_steel</t>
-  </si>
-  <si>
-    <t>pipe_tungsten_steel</t>
+    <t>原矿→2粉碎矿石；锭→粉；齿轮→4粉；齿轮坯→4粉；圆形铸件→9粉；块→9粉；管道→3粉；机械方块→对应板材粉末；石头→圆石；圆石→砂砾；砂砾→沙子；石英→硅粉；骨头→6骨粉；红石矿石→12红石粉+沙子；青金石矿石→8青金石+沙子；石英矿石→4石英+沙子；钻石矿石→4钻石+沙子；煤矿石→4煤粉+沙子</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -3267,27 +3271,27 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3300,7 +3304,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3322,7 +3326,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3330,7 +3334,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3338,7 +3342,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3346,7 +3350,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3355,7 +3359,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -4030,31 +4034,31 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N13" sqref="N13:N15"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2:Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="24.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.08203125" customWidth="1"/>
+    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4091,55 +4095,55 @@
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
       <c r="M2" s="45" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="R2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4147,55 +4151,55 @@
         <v>18</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" s="45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N3" t="s">
         <v>24</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4203,55 +4207,55 @@
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="44" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="R4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4259,55 +4263,55 @@
         <v>36</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="45" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L5" t="s">
         <v>41</v>
       </c>
       <c r="M5" s="45" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="45" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>879</v>
+        <v>760</v>
       </c>
       <c r="R5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4315,49 +4319,49 @@
         <v>45</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J6" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L6" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="45" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P6" t="s">
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>880</v>
+        <v>761</v>
       </c>
       <c r="R6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4365,43 +4369,43 @@
         <v>53</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
       </c>
       <c r="M7" s="45" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="N7" t="s">
         <v>57</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="P7" t="s">
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>881</v>
+        <v>762</v>
       </c>
       <c r="R7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4409,43 +4413,43 @@
         <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="M8" s="45" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N8" t="s">
         <v>63</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="P8" t="s">
         <v>64</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="R8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4453,43 +4457,43 @@
         <v>66</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D9" t="s">
         <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L9" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>441</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>442</v>
       </c>
       <c r="N9" t="s">
         <v>69</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="P9" t="s">
         <v>70</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4497,37 +4501,37 @@
         <v>72</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="R10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4535,31 +4539,31 @@
         <v>77</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D11" t="s">
         <v>78</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P11" t="s">
         <v>80</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="R11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4567,31 +4571,31 @@
         <v>82</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="F12" t="s">
         <v>84</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="R12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4599,31 +4603,31 @@
         <v>86</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D13" t="s">
         <v>87</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
       <c r="G13" s="44" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="Q13" s="45" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="R13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4631,25 +4635,25 @@
         <v>90</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D14" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4657,25 +4661,25 @@
         <v>94</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D15" t="s">
         <v>95</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
       </c>
       <c r="G15" s="44" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4683,25 +4687,25 @@
         <v>98</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D16" t="s">
         <v>99</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4709,51 +4713,51 @@
         <v>102</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D17" t="s">
         <v>103</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
       </c>
       <c r="G17" s="44" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="R17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>401</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>402</v>
       </c>
       <c r="D18" t="s">
         <v>106</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
       </c>
       <c r="G18" s="44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="R18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4761,19 +4765,19 @@
         <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
       </c>
       <c r="G19" s="44" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4781,13 +4785,13 @@
         <v>112</v>
       </c>
       <c r="G20" s="44" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4795,13 +4799,13 @@
         <v>114</v>
       </c>
       <c r="G21" s="44" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="R21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4809,7 +4813,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4817,7 +4821,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4838,50 +4842,50 @@
   <dimension ref="A1:AK29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP20" sqref="AP20"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="22.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" customWidth="1"/>
+    <col min="5" max="5" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" customWidth="1"/>
+    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="9" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="11" max="11" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.75" customWidth="1"/>
+    <col min="13" max="13" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.75" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.75" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" customWidth="1"/>
-    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" customWidth="1"/>
-    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" customWidth="1"/>
-    <col min="27" max="27" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" customWidth="1"/>
-    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" customWidth="1"/>
-    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" customWidth="1"/>
-    <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.08203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.75" customWidth="1"/>
+    <col min="21" max="21" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.75" customWidth="1"/>
+    <col min="23" max="23" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.75" customWidth="1"/>
+    <col min="25" max="25" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.75" customWidth="1"/>
+    <col min="27" max="27" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.75" customWidth="1"/>
+    <col min="29" max="29" width="22.08203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.75" customWidth="1"/>
+    <col min="31" max="31" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.75" customWidth="1"/>
+    <col min="33" max="33" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.25" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="15" customWidth="1"/>
-    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="3" customFormat="1">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
@@ -4937,7 +4941,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4945,106 +4949,106 @@
         <v>137</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>140</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>141</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>142</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
       <c r="S2" s="48" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>181</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
       </c>
       <c r="AA2" s="48" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AB2" s="5" t="s">
         <v>132</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AD2" s="5" t="s">
         <v>150</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AF2" s="5" t="s">
         <v>151</v>
       </c>
       <c r="AG2" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AH2" s="5" t="s">
         <v>152</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>153</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5052,112 +5056,112 @@
         <v>154</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>155</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>156</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>157</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>158</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>160</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>161</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>162</v>
       </c>
       <c r="S3" s="48" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>198</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="V3" s="10" t="s">
+        <v>600</v>
+      </c>
+      <c r="W3" s="9" t="s">
         <v>601</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>602</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>165</v>
       </c>
       <c r="Y3" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>166</v>
       </c>
       <c r="AA3" s="48" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AB3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
       </c>
       <c r="AE3" s="8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AF3" s="5" t="s">
         <v>169</v>
       </c>
       <c r="AG3" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AH3" s="5" t="s">
         <v>170</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AJ3" s="5" t="s">
         <v>171</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5165,107 +5169,107 @@
         <v>172</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>175</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>176</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>178</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>179</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>180</v>
       </c>
       <c r="S4" s="48" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>232</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="5" t="s">
         <v>182</v>
       </c>
       <c r="Y4" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>183</v>
       </c>
       <c r="AA4" s="48" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AB4" s="5" t="s">
         <v>184</v>
       </c>
       <c r="AC4" s="8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>185</v>
       </c>
       <c r="AE4" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AF4" s="5" t="s">
         <v>186</v>
       </c>
       <c r="AG4" s="45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AH4" t="s">
         <v>187</v>
       </c>
       <c r="AI4" s="8" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AJ4" s="5" t="s">
         <v>188</v>
       </c>
       <c r="AK4" s="8" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5273,55 +5277,55 @@
         <v>189</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>191</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>193</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>194</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>195</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>196</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>197</v>
       </c>
       <c r="S5" s="48" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="U5" s="5"/>
       <c r="W5" s="5"/>
@@ -5329,46 +5333,46 @@
         <v>200</v>
       </c>
       <c r="Y5" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>201</v>
       </c>
       <c r="AA5" s="48" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>202</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>203</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AF5" s="40" t="s">
         <v>204</v>
       </c>
       <c r="AG5" s="8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AH5" t="s">
         <v>205</v>
       </c>
       <c r="AI5" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AJ5" s="5" t="s">
         <v>206</v>
       </c>
       <c r="AK5" s="45" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5376,106 +5380,106 @@
         <v>207</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>209</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>210</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>211</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>212</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N6" s="5" t="s">
         <v>213</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>214</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>215</v>
       </c>
       <c r="S6" s="48" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>260</v>
       </c>
       <c r="U6" s="9" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>217</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>218</v>
       </c>
       <c r="Y6" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>219</v>
       </c>
       <c r="AA6" s="48" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>220</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>221</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AF6" s="5" t="s">
         <v>222</v>
       </c>
       <c r="AG6" s="45" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AJ6" s="5" t="s">
         <v>223</v>
       </c>
       <c r="AK6" s="45" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5483,37 +5487,37 @@
         <v>224</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>225</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>226</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>227</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>228</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>229</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -5521,13 +5525,13 @@
         <v>230</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>231</v>
       </c>
       <c r="S7" s="48" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -5536,34 +5540,34 @@
         <v>233</v>
       </c>
       <c r="Y7" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>234</v>
       </c>
       <c r="AA7" s="48" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AB7" s="5" t="s">
         <v>235</v>
       </c>
       <c r="AC7" s="45" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="AF7" s="5" t="s">
         <v>236</v>
       </c>
       <c r="AG7" s="45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AJ7" s="5" t="s">
         <v>237</v>
       </c>
       <c r="AK7" s="8" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5571,37 +5575,37 @@
         <v>238</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>239</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>240</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>241</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>242</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>243</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -5609,19 +5613,19 @@
         <v>244</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>245</v>
       </c>
       <c r="S8" s="48" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="T8" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="U8" s="9" t="s">
         <v>603</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>604</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="9"/>
@@ -5629,34 +5633,34 @@
         <v>247</v>
       </c>
       <c r="Y8" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>248</v>
       </c>
       <c r="AA8" s="48" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>249</v>
       </c>
       <c r="AC8" s="45" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AF8" s="5" t="s">
         <v>250</v>
       </c>
       <c r="AG8" s="45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AJ8" s="5" t="s">
         <v>251</v>
       </c>
       <c r="AK8" s="8" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5664,37 +5668,37 @@
         <v>252</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>253</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>254</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>255</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>256</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>257</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
@@ -5702,13 +5706,13 @@
         <v>258</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>259</v>
       </c>
       <c r="S9" s="48" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -5717,34 +5721,34 @@
         <v>261</v>
       </c>
       <c r="Y9" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>262</v>
       </c>
       <c r="AA9" s="48" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AB9" s="5" t="s">
         <v>263</v>
       </c>
       <c r="AC9" s="45" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF9" s="5" t="s">
         <v>264</v>
       </c>
       <c r="AG9" s="45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AJ9" s="5" t="s">
         <v>265</v>
       </c>
       <c r="AK9" s="8" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5752,37 +5756,37 @@
         <v>266</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>267</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>268</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>269</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>270</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>271</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -5790,58 +5794,58 @@
         <v>272</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="R10" s="5" t="s">
         <v>273</v>
       </c>
       <c r="S10" s="48" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>146</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="V10" s="5" t="s">
         <v>147</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="X10" s="5" t="s">
         <v>274</v>
       </c>
       <c r="Y10" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="Z10" s="5" t="s">
         <v>275</v>
       </c>
       <c r="AA10" s="48" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AB10" s="5" t="s">
         <v>276</v>
       </c>
       <c r="AC10" s="45" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AF10" s="5" t="s">
         <v>277</v>
       </c>
       <c r="AG10" s="45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AJ10" s="5" t="s">
         <v>278</v>
       </c>
       <c r="AK10" s="45" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5849,37 +5853,37 @@
         <v>279</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>281</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>282</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>283</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>284</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
@@ -5887,37 +5891,37 @@
         <v>285</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="R11" s="5" t="s">
         <v>286</v>
       </c>
       <c r="S11" s="45" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>246</v>
       </c>
       <c r="U11" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="V11" s="5" t="s">
         <v>199</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>287</v>
       </c>
       <c r="Y11" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="Z11" s="5" t="s">
         <v>288</v>
       </c>
       <c r="AA11" s="45" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
@@ -5925,16 +5929,16 @@
         <v>289</v>
       </c>
       <c r="AG11" s="45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AJ11" s="5" t="s">
         <v>290</v>
       </c>
       <c r="AK11" s="45" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5942,37 +5946,37 @@
         <v>291</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>292</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>293</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>294</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>295</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>296</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
@@ -5982,13 +5986,13 @@
         <v>297</v>
       </c>
       <c r="S12" s="48" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>216</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -5996,13 +6000,13 @@
         <v>298</v>
       </c>
       <c r="Y12" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Z12" s="5" t="s">
         <v>299</v>
       </c>
       <c r="AA12" s="48" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
@@ -6010,16 +6014,16 @@
         <v>300</v>
       </c>
       <c r="AG12" s="8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AJ12" s="5" t="s">
         <v>301</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6027,59 +6031,59 @@
         <v>302</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>303</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>304</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>305</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>306</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>307</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="10" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="S13" s="48" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>163</v>
       </c>
       <c r="U13" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="V13" s="5" t="s">
         <v>164</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -6088,19 +6092,19 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AF13" s="40" t="s">
+        <v>598</v>
+      </c>
+      <c r="AG13" s="45" t="s">
         <v>599</v>
-      </c>
-      <c r="AG13" s="45" t="s">
-        <v>600</v>
       </c>
       <c r="AJ13" s="5" t="s">
         <v>308</v>
       </c>
       <c r="AK13" s="8" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6108,31 +6112,31 @@
         <v>309</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>311</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>312</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>313</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6157,10 +6161,10 @@
         <v>314</v>
       </c>
       <c r="AK14" s="8" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6172,19 +6176,19 @@
         <v>315</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>316</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>317</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -6206,10 +6210,10 @@
         <v>318</v>
       </c>
       <c r="AK15" s="8" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6221,19 +6225,19 @@
         <v>319</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>320</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>321</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -6255,10 +6259,10 @@
         <v>322</v>
       </c>
       <c r="AK16" s="45" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="17" spans="1:37">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6270,19 +6274,19 @@
         <v>323</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>324</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>325</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -6301,13 +6305,13 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AJ17" s="10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AK17" s="45" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="18" spans="1:37">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6319,19 +6323,19 @@
         <v>326</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>327</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>328</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -6350,13 +6354,13 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AJ18" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AK18" s="45" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="19" spans="1:37">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6368,19 +6372,19 @@
         <v>329</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>330</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>331</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -6401,13 +6405,13 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AJ19" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="AK19" s="45" t="s">
         <v>610</v>
       </c>
-      <c r="AK19" s="45" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="20" spans="1:37">
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6419,13 +6423,13 @@
         <v>332</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>333</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -6448,13 +6452,13 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AJ20" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AK20" s="45" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="21" spans="1:37">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6466,13 +6470,13 @@
         <v>334</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>335</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -6495,13 +6499,13 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AJ21" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="AK21" s="45" t="s">
         <v>578</v>
       </c>
-      <c r="AK21" s="45" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="22" spans="1:37">
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6515,7 +6519,7 @@
         <v>336</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -6538,13 +6542,13 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AJ22" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AK22" s="45" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6558,10 +6562,10 @@
         <v>337</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -6583,13 +6587,13 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AJ23" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AK23" s="45" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6603,7 +6607,7 @@
         <v>338</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -6626,13 +6630,13 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AJ24" s="16" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="AK24" s="45" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" ht="75">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6646,7 +6650,7 @@
         <v>339</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -6668,13 +6672,13 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AJ25" s="21" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AK25" s="9" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6688,10 +6692,10 @@
         <v>340</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -6713,13 +6717,13 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AJ26" s="16" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AK26" s="9" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="27" spans="1:37">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -6727,11 +6731,11 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="41" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="I27" s="41"/>
       <c r="J27" s="41" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -6753,13 +6757,13 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AJ27" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AK27" s="9" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="28" spans="1:37" ht="60">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -6767,11 +6771,11 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="41" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="I28" s="41"/>
       <c r="J28" s="41" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -6793,18 +6797,18 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AJ28" s="39" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="AK28" s="9" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="29" spans="1:37">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ29" s="38" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="AK29" s="9" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
     </row>
   </sheetData>
@@ -6819,28 +6823,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.08203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.08203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.08203125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.25" customWidth="1"/>
+    <col min="7" max="7" width="20.75" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>341</v>
       </c>
@@ -6852,7 +6856,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6860,10 +6864,10 @@
         <v>344</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E3" t="s">
         <v>345</v>
@@ -6881,10 +6885,10 @@
         <v>349</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -6892,13 +6896,13 @@
         <v>350</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -6906,13 +6910,13 @@
         <v>351</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -6920,13 +6924,13 @@
         <v>352</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="57" customHeight="1">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -6934,36 +6938,36 @@
         <v>353</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>612</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>613</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E8" t="s">
         <v>354</v>
@@ -6972,27 +6976,27 @@
         <v>355</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E9" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -7000,27 +7004,27 @@
         <v>357</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E10" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E11" t="s">
         <v>359</v>
@@ -7032,49 +7036,49 @@
         <v>361</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E12" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="90">
+    <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E14" t="s">
         <v>133</v>
@@ -7098,10 +7102,10 @@
         <v>364</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -7109,16 +7113,16 @@
         <v>365</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -7126,19 +7130,19 @@
         <v>367</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E16" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>369</v>
       </c>
@@ -7156,7 +7160,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="138" customHeight="1">
+    <row r="19" spans="1:12" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>1</v>
       </c>
@@ -7164,16 +7168,16 @@
         <v>373</v>
       </c>
       <c r="C19" s="25" t="s">
+        <v>677</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>678</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="E19" s="26" t="s">
         <v>679</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="F19" s="27" t="s">
         <v>680</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>681</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -7182,25 +7186,25 @@
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
     </row>
-    <row r="20" spans="1:12" ht="30">
+    <row r="20" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>2</v>
       </c>
       <c r="B20" s="46" t="s">
+        <v>681</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>682</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="D20" s="26" t="s">
         <v>683</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>684</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="27" t="s">
         <v>374</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
@@ -7208,22 +7212,22 @@
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
     </row>
-    <row r="21" spans="1:12" ht="30">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>3</v>
       </c>
       <c r="B21" s="46" t="s">
+        <v>685</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>686</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="D21" s="26" t="s">
         <v>687</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>688</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="27" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>375</v>
@@ -7234,41 +7238,41 @@
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
     </row>
-    <row r="22" spans="1:12" ht="140.25">
+    <row r="22" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>4</v>
       </c>
       <c r="B22" s="47" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D22" s="26" t="s">
+        <v>689</v>
+      </c>
+      <c r="E22" s="26" t="s">
         <v>690</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="F22" s="27" t="s">
         <v>691</v>
       </c>
-      <c r="F22" s="27" t="s">
-        <v>692</v>
-      </c>
       <c r="G22" s="30" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="J22" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="K22" s="28" t="s">
         <v>694</v>
       </c>
-      <c r="K22" s="28" t="s">
-        <v>695</v>
-      </c>
       <c r="L22" s="28"/>
     </row>
-    <row r="23" spans="1:12" ht="140.25">
+    <row r="23" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>5</v>
       </c>
@@ -7276,10 +7280,10 @@
         <v>376</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>695</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>696</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>697</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="23"/>
@@ -7287,35 +7291,35 @@
         <v>377</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I23" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="J23" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="K23" s="28" t="s">
         <v>694</v>
       </c>
-      <c r="K23" s="28" t="s">
-        <v>695</v>
-      </c>
       <c r="L23" s="28"/>
     </row>
-    <row r="24" spans="1:12" ht="45">
+    <row r="24" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>6</v>
       </c>
       <c r="B24" s="33" t="s">
+        <v>698</v>
+      </c>
+      <c r="C24" s="25" t="s">
         <v>699</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="D24" s="22" t="s">
         <v>700</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>701</v>
       </c>
       <c r="E24" s="34"/>
       <c r="F24" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -7324,217 +7328,217 @@
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
     </row>
-    <row r="25" spans="1:12" ht="105">
+    <row r="25" spans="1:12" ht="84" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>7</v>
       </c>
       <c r="B25" s="46" t="s">
+        <v>702</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>703</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="D25" s="22" t="s">
         <v>704</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="E25" s="26" t="s">
         <v>705</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="F25" s="23" t="s">
         <v>706</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="G25" s="32" t="s">
         <v>707</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="H25" s="26" t="s">
         <v>708</v>
       </c>
-      <c r="H25" s="26" t="s">
-        <v>709</v>
-      </c>
       <c r="I25" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="J25" s="22" t="s">
         <v>671</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="K25" s="22" t="s">
         <v>672</v>
       </c>
-      <c r="K25" s="22" t="s">
-        <v>673</v>
-      </c>
       <c r="L25" s="28"/>
     </row>
-    <row r="26" spans="1:12" ht="255">
+    <row r="26" spans="1:12" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
         <v>8</v>
       </c>
       <c r="B26" s="31" t="s">
+        <v>709</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>710</v>
       </c>
-      <c r="C26" s="25" t="s">
-        <v>711</v>
-      </c>
       <c r="D26" s="26" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>378</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>379</v>
+        <v>881</v>
       </c>
       <c r="H26" s="27" t="s">
+        <v>673</v>
+      </c>
+      <c r="I26" s="27" t="s">
         <v>674</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>675</v>
-      </c>
       <c r="J26" s="22" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="127.5">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A27" s="23">
         <v>9</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="23" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H27" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="I27" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="J27" s="28" t="s">
         <v>694</v>
-      </c>
-      <c r="J27" s="28" t="s">
-        <v>695</v>
       </c>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
     </row>
-    <row r="28" spans="1:12" ht="127.5">
+    <row r="28" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A28" s="23">
         <v>10</v>
       </c>
       <c r="B28" s="46" t="s">
+        <v>714</v>
+      </c>
+      <c r="C28" s="25" t="s">
         <v>715</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="D28" s="26" t="s">
         <v>716</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>717</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="23" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H28" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="I28" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="J28" s="28" t="s">
         <v>694</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>695</v>
       </c>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
     </row>
-    <row r="29" spans="1:12" ht="127.5">
+    <row r="29" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A29" s="23">
         <v>11</v>
       </c>
       <c r="B29" s="29" t="s">
+        <v>718</v>
+      </c>
+      <c r="C29" s="25" t="s">
         <v>719</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="D29" s="26" t="s">
         <v>720</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>721</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="23" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H29" s="22" t="s">
+        <v>692</v>
+      </c>
+      <c r="I29" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="J29" s="28" t="s">
         <v>694</v>
-      </c>
-      <c r="J29" s="28" t="s">
-        <v>695</v>
       </c>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
     </row>
-    <row r="30" spans="1:12" ht="210">
+    <row r="30" spans="1:12" ht="168" x14ac:dyDescent="0.3">
       <c r="A30" s="23">
         <v>12</v>
       </c>
       <c r="B30" s="29" t="s">
+        <v>722</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>723</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>724</v>
-      </c>
       <c r="D30" s="26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="23" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
     </row>
-    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="23">
         <v>13</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -7544,21 +7548,21 @@
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
     </row>
-    <row r="32" spans="1:12" ht="30">
+    <row r="32" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="23">
         <v>14</v>
       </c>
       <c r="B32" s="29" t="s">
+        <v>726</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>594</v>
+      </c>
+      <c r="D32" s="26" t="s">
         <v>727</v>
       </c>
-      <c r="C32" s="25" t="s">
-        <v>595</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>728</v>
-      </c>
       <c r="E32" s="34" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
@@ -7568,18 +7572,18 @@
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>15</v>
       </c>
       <c r="B33" s="35" t="s">
+        <v>665</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>666</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="14" t="s">
         <v>667</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -7597,184 +7601,184 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="36"/>
-    <col min="2" max="2" width="20.140625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="36"/>
-    <col min="4" max="4" width="34.42578125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="36"/>
-    <col min="6" max="6" width="27.28515625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="36"/>
-    <col min="8" max="8" width="29.7109375" style="36" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="36" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="36"/>
+    <col min="2" max="2" width="20.08203125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="36"/>
+    <col min="4" max="4" width="34.4140625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="36"/>
+    <col min="6" max="6" width="27.25" style="36" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="36"/>
+    <col min="8" max="8" width="29.75" style="36" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="36" customWidth="1"/>
+    <col min="10" max="10" width="8.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="B2" s="13" t="s">
+      <c r="D2" s="13" t="s">
+        <v>732</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>734</v>
+      </c>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
         <v>731</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>733</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>735</v>
-      </c>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" ht="45">
-      <c r="B3" s="13" t="s">
-        <v>732</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>734</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>736</v>
       </c>
       <c r="G3" s="36">
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="G4" s="36">
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D5" s="37" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G5" s="36">
         <v>3</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="90">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
       <c r="D6" s="37" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G6" s="36">
         <v>4</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="150">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G7" s="36">
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G8" s="36">
         <v>6</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" ht="105">
+    <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="D9" s="37" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G9" s="36">
         <v>7</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D10" s="13" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G10" s="36">
         <v>8</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="F11" s="13" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G11" s="36">
         <v>9</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D12" s="13" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="G12" s="36">
         <v>10</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="45">
+    <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="F14" s="43" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -7793,23 +7797,23 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.95" customHeight="1">
+    <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -7823,83 +7827,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082DB092-EC3A-4409-8021-838227EE44A2}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new pipe 2022.8.6 11.10
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbydd\IdeaProjects\micro_machinery\参考\资料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E990BFAD-F0F6-459B-A6E3-7FDE6019FB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A5157-2AC0-4060-B71A-B4F18F7D9EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方块列表" sheetId="6" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="888">
   <si>
     <t>矿石</t>
   </si>
@@ -1288,19 +1288,19 @@
   </si>
   <si>
     <t>orecopper</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>oresilver</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>orepyrolusite</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>oregraphite</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>orechromite</t>
@@ -1334,7 +1334,7 @@
   </si>
   <si>
     <t>下界钒铁矿</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>orenolanite_nether</t>
@@ -1359,19 +1359,19 @@
   </si>
   <si>
     <t>casing_3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>casing_4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>oretin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>oreilmenite</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>molten_copper_discarded</t>
@@ -1435,23 +1435,23 @@
   </si>
   <si>
     <t>熔融金</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>module_transmission_2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>module_transmission_3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>module_transmission_4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>module_transmission_5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>pcm</t>
@@ -1464,14 +1464,14 @@
   </si>
   <si>
     <t>强化玻璃</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>stalinite</t>
   </si>
   <si>
     <t>graphite_crucible</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>stone_hammer</t>
@@ -1616,7 +1616,7 @@
   </si>
   <si>
     <t>circle_casting_gold</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_tungsten_steel</t>
@@ -1779,19 +1779,19 @@
   </si>
   <si>
     <t>motor_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>motor_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>motor_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>motor_5</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ore_tin_concentrate</t>
@@ -1825,15 +1825,15 @@
   </si>
   <si>
     <t>锭模具</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>杆模具</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>剑模具</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>cast_ingot</t>
@@ -1885,66 +1885,66 @@
   </si>
   <si>
     <t>青铜剑刃</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>bronze_sword0</t>
   </si>
   <si>
     <t>klin</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>lathe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>cutter</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>anvil_stone</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>anvil_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>anvil_pigiron</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>etcher</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>electrolysis</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>centrifuge</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>atomization</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>pump</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>weld</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>hand_generator</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>generator</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>spherical_tank</t>
@@ -1963,7 +1963,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1974,80 +1974,80 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>键3次，产出成品，空手右键取下</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>杆→线</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>勘矿镐</t>
   </si>
   <si>
     <t>prospector</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>钢辊</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>roll_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>钴轴</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>axis_cobalt</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>copper_cable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>nickel_cable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>aluminum_cable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>tungsten_cable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>cobalt_cable</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>齿轮坯模具</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>cast_gear_blank</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>齿轮坯→齿轮（钻削，镗孔</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>锭→杆（刨削，磨削</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>轴→辊（钻削，车削</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2057,14 +2057,14 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>铣削，车削</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2074,7 +2074,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2085,8 +2085,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>个模板，可以熔炼青铜合金【锭160mb、杆80mb、</t>
@@ -2095,7 +2095,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2106,8 +2106,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>mb、</t>
@@ -2116,7 +2116,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2127,17 +2127,17 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>】</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>车削加工，选择加工项目：齿轮、杆、辊、螺丝，根据加工项目收取材料）钻削-5，车削-10，铣削-7，磨削-2，刨削-4，镗孔-3，车床最大电容量40000fe，每次加工消耗6400fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2147,13 +2147,13 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>fe</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2163,8 +2163,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0000fe，每tick消耗</t>
@@ -2173,206 +2173,206 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>4096fe</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>最大电容量120000fe，每tick消耗1024fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>最大电容量40000fe，每tick消耗128fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>切断整材，最大电容量40000fe，每tick消耗128fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>海绵状铁</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>灼热的铁锭</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>灼热的钢锭（未完工）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>sponge_iron</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>hot_iron_ingot</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>hot_steel_ingot</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>风箱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>最大电容40000fe，每tick发电200fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>每tick发电16fe</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>离心机</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>切割机</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>金属管</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>钢制飞轮（用于制作便携式飞轮电池和放置在大型飞轮蓄电器内）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>碳素飞轮</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>超材料飞轮</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>便携式飞轮电池（蓄电量为单个碳素飞轮的存储量）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>flying_wheel_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>flying_wheel_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>flying_wheel_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>flywheel_battery</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>熔炉和高炉不可以烧铁矿石、金矿石、铜矿石</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>配置文件</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>能量生产效率（0.1-10）数字为倍率</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>飞轮储能效率（0.1-10）数字为倍率</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>苹果汁持续时间系数（0.1-10）数字为倍率</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>开/关 火电站最低水量限制</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>锯片效率（0.2-5）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>矿产密度（0-0.05）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>激光钻头伤害（0-∞）</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>球形储罐容量（256000</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>激光蚀刻机（无gui</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>金属雾化器</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>焊接室</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>etched_wafer</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>refined_slag_vanadium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_copper</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>单晶硅→4晶圆</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>monocrystalline_silicon</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>gear_blank_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>gear_blank_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>电动泵（无gui</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>集装箱</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>container</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>拥有8个格子，每个格子可以存放同类物品4096个</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>tank_block</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>thickener</t>
@@ -2421,9 +2421,6 @@
     <t>所有工作时间相同（便于动画效果实现）正在运行的配方将会把物品渲染在操作台上，然后锤头压下去完成工作</t>
   </si>
   <si>
-    <t>圆形铸件→1轴；锭→板；4板→1管道</t>
-  </si>
-  <si>
     <t>浇注机</t>
   </si>
   <si>
@@ -2434,9 +2431,6 @@
   </si>
   <si>
     <t>钢包、浇筑流体块</t>
-  </si>
-  <si>
-    <t>共有四个按钮，对应四种生产类型，按下会让按钮移动1/16个方块，其他按钮恢复原位，刚建造的时候默认板材</t>
   </si>
   <si>
     <t>容量指示</t>
@@ -2477,7 +2471,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2571,167 +2565,155 @@
   </si>
   <si>
     <t>管道设置</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>导线类</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>能量管道，根据不同等级区分最大传输速率</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>流体管道</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>类似能量管道</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>传送带</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>传送带的连接方式类似原版铁轨</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>掉落物落在传送带上会被插入传送带</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>拿着物品，对着传送带右键可以放上物品</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>传送带仅有一个出口</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>用锤子可以断开传送带之间的连接</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>传送带放置时，可以和四周任何方向的传送带相连（除非是跨高度的）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>锤子右键传送带的连接处可以断开连接</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>传送带的中间应当有方向指示器</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>有连接端点的方向无法连接传送带</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>端点朝向的连接范围是</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>空手shift右键传送带的长边可以拖出一个连接端点，右键一个容器或者另一个传送带，可以完成连接（连接容器没有另一个端点，接连传送带会产生另一个端点</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>空手shift右键端点可以断开连接</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>端点运输速度为1米/秒</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>空手右键端点可以打开过滤器gui</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>不同等级的传送带具有不同的运载速度：1x，4x，16x（每一格传送带同时能运送的物品堆叠数</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>端点建立完成之后会生成一个线缆，抓钩沿着线缆运动</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>跨高度传送带会被对角线的实心方块切断</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>流体管道也是按tick向周围的流体管道传输流体</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>只会传输给其中容纳的流体数量比自身少的管道，每个流体管道都会尝试使周围的管道和自身的管道中内含的流体量持平（简而言之，流体量就是液压，流体从高的传输给低的）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>堵塞物会被推动，在以上的情况下当装有B流体的管道继续发送B流体时就会将堵塞物推向对面的管道（如果对面没有管道那就不推动）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>当一个已经装有A流体的管道被传入B流体时就会发生堵塞（根据配方消耗一定数量的A和B产生堵塞物，如果没有对应的配方或者数量不够就产生普通的管道堵塞物），堵塞的管道无法主动向外传输流体，也不会向其他液体容器输出液体，但是依然可以接收液体，被堵塞的管道中仍然会残留有余下的流体（有液压）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>使用扳手（？）锤子(?)右键管道可以将管道打开，打开的一侧所对应的方块，如果是空气方块那么当液体量足够时输会尝试放置液体方块，同时堵塞物可被从打开的一侧推出（掉落物形式）（液体加农炮可能性存疑）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>漏斗可以和传送带互动</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>空手shift右键可以取下物品</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>conveyer_belt_1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>pipe_1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>pipe_2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>pipe_3</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>单向阀</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>check_valve</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>过滤器标记</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>filter</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>过滤器标记可以快速复制过滤器给管道或者传送带端点</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>单向阀能够从容器或者管道内抽取液体到另一侧，并且不允许反向，仅有相对的两个接口（可以配置过滤器*白名单*和速度限制）</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>手持过滤器标记，shift+右键复制指向的单向阀或者传送带端点，右键单向阀或者传送带端点即可复制</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2741,8 +2723,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>，每</t>
@@ -2751,7 +2733,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2762,8 +2744,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>消耗50</t>
@@ -2772,457 +2754,457 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>fe</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>8铁粉+1碳粉→8钢锭；2铁粉+1镍粉→3殷钢锭；4碳粉+4钨粉+1钴粉→5钨钢锭；3铜粉+1锡粉→4青铜锭；4钢粉+3镍粉+2铬粉→5镍铬合金锭；2钢粉+1不锈钢添加剂→2不锈钢锭；6钢粉+1镍粉+1铬粉+1锰粉→9不锈钢锭；3钨钢粉+5钢粉+1高速钢添加剂→9高速钢锭</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>dust_chromium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>dust_manganese</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>dust_tungsten_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>dust_ncalloy</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>铬4钒1锰1萤石粉1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>dust_ferrochrome</t>
   </si>
   <si>
     <t>锰铬镍</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>钛合金粉</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>钒1铝1钛7</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>记忆合金</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>钛镍下界合金</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>漏斗可以从机器中的输出格中取出物品；漏斗可以向机器的输入格中输入物品</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>传送带端点在无过滤器时行为和漏斗一致，有过滤器时，可以访问机器的所有库存</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>steel_scaffolding</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>screw_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>string_copper</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>resistor</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>module_transmission_1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>gear_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>复杂传动装置</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>module_generator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>coilcopper</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>module_heat_sink</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>ingot_graphite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>module_pressure_bearing</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>slag_concrete</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>bellow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>高速钢圆形铸件</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_titanium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_hss</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>axis_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>axis_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>axis_iron</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>axis_invar</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>axis_titanium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_tin</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_ss</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_nickel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_invar</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_tungsten_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_silver</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_chromium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_titanium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_aluminum</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_ncalloy</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_gold</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_iron</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>plate_silicon</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_copper</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_bronze</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_ss</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_tungsten</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_nickel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_invar</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_hss</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_silver</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_manganese</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_chromium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_vanadium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_cobalt</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_titanium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_aluminum</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ingot_ncalloy</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>blockcopper</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocktin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockbronze</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocksteel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockss</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocktungsten</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocknickel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockinvar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockhss</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocksilver</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockchromium</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockvanadium</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockcobalt</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocktitanium</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockaluminum</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockncalloy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blockmanganese</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>blocktungsten_steel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_steel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_iron</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_silver</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_invar</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_aluminum</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_nickel</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>circle_casting_ss</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>板150mb；杆75mb；线75mb；管600mb；</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>screw_titanium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>apple_drops</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ore_copper_concentrate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ore_ilmenite_concentrate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_chromite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_ilmenite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>slag_titanium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_pyrolusite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_bauxite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_ferromanganese</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>slag_manganese</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_nolanite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>slag_vanadium</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>crushed_tunstite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ore_tunstite_concentrate</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>ss_additive</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>原矿→2粉碎矿石；锭→粉；齿轮→4粉；齿轮坯→4粉；圆形铸件→9粉；块→9粉；管道→3粉；机械方块→对应板材粉末；石头→圆石；圆石→砂砾；砂砾→沙子；石英→硅粉；骨头→6骨粉；红石矿石→12红石粉+沙子；青金石矿石→8青金石+沙子；石英矿石→4石英+沙子；钻石矿石→4钻石+沙子；煤矿石→4煤粉+沙子</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -3232,8 +3214,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="等线"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0000fe，每tick消耗</t>
@@ -3242,7 +3224,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -3265,44 +3247,157 @@
   <si>
     <t>能量输出接口</t>
   </si>
+  <si>
+    <t>pipe_invar</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>pipe_stainless_steel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>pipe_tungsten_steel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>流体管道现在存在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>connect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>arm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>shell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>三个组件</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>shell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>需要管道连接数超过2</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆形铸件→1轴；锭→板；4板→1传送带</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>共有四个按钮，对应四种生产类型，按下会让按钮移动3/16个方块，其他按钮恢复原位，刚建造的时候默认板材</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3315,7 +3410,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3337,7 +3432,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3345,7 +3440,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3353,7 +3448,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3361,7 +3456,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3370,7 +3465,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3379,6 +3474,20 @@
       <sz val="9.8000000000000007"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3496,135 +3605,141 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4089,34 +4204,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N4" sqref="N4"/>
+      <selection pane="topRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="12.75" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
+    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4141,11 +4257,11 @@
       <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4159,7 +4275,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -4177,7 +4293,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -4189,19 +4305,20 @@
         <v>15</v>
       </c>
       <c r="O2" s="44" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>757</v>
-      </c>
-      <c r="R2" t="s">
+        <v>755</v>
+      </c>
+      <c r="R2" s="8"/>
+      <c r="S2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4215,7 +4332,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -4245,19 +4362,20 @@
         <v>24</v>
       </c>
       <c r="O3" s="44" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>757</v>
-      </c>
-      <c r="R3" t="s">
+        <v>755</v>
+      </c>
+      <c r="R3" s="8"/>
+      <c r="S3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4271,7 +4389,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -4295,25 +4413,26 @@
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="44" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>757</v>
-      </c>
-      <c r="R4" t="s">
+        <v>755</v>
+      </c>
+      <c r="R4" s="8"/>
+      <c r="S4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19" ht="39.5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4327,7 +4446,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
@@ -4357,19 +4476,22 @@
         <v>42</v>
       </c>
       <c r="O5" s="44" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>758</v>
-      </c>
-      <c r="R5" t="s">
+        <v>881</v>
+      </c>
+      <c r="R5" s="51" t="s">
+        <v>884</v>
+      </c>
+      <c r="S5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19" ht="26.5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4383,7 +4505,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -4401,7 +4523,7 @@
         <v>49</v>
       </c>
       <c r="M6" s="44" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
@@ -4413,13 +4535,16 @@
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>759</v>
-      </c>
-      <c r="R6" t="s">
+        <v>882</v>
+      </c>
+      <c r="R6" s="52" t="s">
+        <v>885</v>
+      </c>
+      <c r="S6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4433,7 +4558,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
@@ -4457,13 +4582,14 @@
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>760</v>
-      </c>
-      <c r="R7" t="s">
+        <v>883</v>
+      </c>
+      <c r="R7" s="8"/>
+      <c r="S7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4477,7 +4603,7 @@
         <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
@@ -4486,7 +4612,7 @@
         <v>418</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="M8" s="44" t="s">
         <v>437</v>
@@ -4503,11 +4629,12 @@
       <c r="Q8" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="8"/>
+      <c r="S8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4521,7 +4648,7 @@
         <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
@@ -4547,11 +4674,12 @@
       <c r="Q9" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="8"/>
+      <c r="S9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4565,7 +4693,7 @@
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
@@ -4577,7 +4705,7 @@
         <v>628</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
@@ -4585,11 +4713,12 @@
       <c r="Q10" s="8" t="s">
         <v>606</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="8"/>
+      <c r="S10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4603,7 +4732,7 @@
         <v>78</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
@@ -4617,11 +4746,12 @@
       <c r="Q11" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="8"/>
+      <c r="S11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4635,7 +4765,7 @@
         <v>83</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="F12" t="s">
         <v>84</v>
@@ -4644,7 +4774,7 @@
         <v>421</v>
       </c>
       <c r="N12" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
@@ -4652,11 +4782,12 @@
       <c r="Q12" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="8"/>
+      <c r="S12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4670,7 +4801,7 @@
         <v>87</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
@@ -4679,19 +4810,20 @@
         <v>424</v>
       </c>
       <c r="N13" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="Q13" s="44" t="s">
-        <v>762</v>
-      </c>
-      <c r="R13" t="s">
+        <v>757</v>
+      </c>
+      <c r="R13" s="44"/>
+      <c r="S13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4705,7 +4837,7 @@
         <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -4714,13 +4846,13 @@
         <v>425</v>
       </c>
       <c r="N14" t="s">
-        <v>885</v>
-      </c>
-      <c r="R14" t="s">
+        <v>880</v>
+      </c>
+      <c r="S14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4734,7 +4866,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -4742,11 +4874,11 @@
       <c r="G15" s="43" t="s">
         <v>426</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4760,7 +4892,7 @@
         <v>99</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -4768,11 +4900,11 @@
       <c r="G16" s="43" t="s">
         <v>427</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4786,7 +4918,7 @@
         <v>103</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
@@ -4794,11 +4926,11 @@
       <c r="G17" s="43" t="s">
         <v>428</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4812,7 +4944,7 @@
         <v>106</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
@@ -4820,11 +4952,11 @@
       <c r="G18" s="43" t="s">
         <v>429</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4832,7 +4964,7 @@
         <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
@@ -4840,11 +4972,11 @@
       <c r="G19" s="43" t="s">
         <v>431</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4854,11 +4986,11 @@
       <c r="G20" s="43" t="s">
         <v>422</v>
       </c>
-      <c r="R20" s="7" t="s">
+      <c r="S20" s="7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4868,36 +5000,36 @@
       <c r="G21" s="43" t="s">
         <v>423</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -4913,46 +5045,46 @@
       <selection pane="topRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" customWidth="1"/>
+    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="9" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="11" max="11" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.75" customWidth="1"/>
+    <col min="13" max="13" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.75" customWidth="1"/>
+    <col min="15" max="15" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.75" customWidth="1"/>
+    <col min="17" max="17" width="15.25" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" customWidth="1"/>
-    <col min="23" max="23" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" customWidth="1"/>
-    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" customWidth="1"/>
-    <col min="27" max="27" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" customWidth="1"/>
-    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" customWidth="1"/>
-    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" customWidth="1"/>
-    <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.75" customWidth="1"/>
+    <col min="21" max="21" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.75" customWidth="1"/>
+    <col min="23" max="23" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.75" customWidth="1"/>
+    <col min="25" max="25" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.75" customWidth="1"/>
+    <col min="27" max="27" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.75" customWidth="1"/>
+    <col min="29" max="29" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.75" customWidth="1"/>
+    <col min="31" max="31" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.75" customWidth="1"/>
+    <col min="33" max="33" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.25" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="15" customWidth="1"/>
-    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="3" customFormat="1">
+    <row r="1" spans="1:37" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
@@ -5008,7 +5140,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5022,13 +5154,13 @@
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>140</v>
@@ -5052,31 +5184,31 @@
         <v>143</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
       <c r="S2" s="47" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>181</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
@@ -5106,7 +5238,7 @@
         <v>152</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>153</v>
@@ -5115,7 +5247,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5147,7 +5279,7 @@
         <v>158</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
@@ -5171,13 +5303,13 @@
         <v>162</v>
       </c>
       <c r="S3" s="47" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>198</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>600</v>
@@ -5201,7 +5333,7 @@
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
@@ -5228,7 +5360,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5236,19 +5368,19 @@
         <v>172</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>175</v>
@@ -5260,7 +5392,7 @@
         <v>176</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
@@ -5284,13 +5416,13 @@
         <v>180</v>
       </c>
       <c r="S4" s="47" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>232</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="5" t="s">
@@ -5336,7 +5468,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5356,7 +5488,7 @@
         <v>191</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>192</v>
@@ -5368,7 +5500,7 @@
         <v>193</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>194</v>
@@ -5392,7 +5524,7 @@
         <v>197</v>
       </c>
       <c r="S5" s="47" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="U5" s="5"/>
       <c r="W5" s="5"/>
@@ -5412,7 +5544,7 @@
         <v>202</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>203</v>
@@ -5439,7 +5571,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5447,7 +5579,7 @@
         <v>207</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>208</v>
@@ -5459,7 +5591,7 @@
         <v>209</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>210</v>
@@ -5471,7 +5603,7 @@
         <v>211</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>212</v>
@@ -5483,7 +5615,7 @@
         <v>213</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>214</v>
@@ -5495,13 +5627,13 @@
         <v>215</v>
       </c>
       <c r="S6" s="47" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>260</v>
       </c>
       <c r="U6" s="9" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>217</v>
@@ -5525,7 +5657,7 @@
         <v>220</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>221</v>
@@ -5546,7 +5678,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5566,7 +5698,7 @@
         <v>226</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>227</v>
@@ -5578,7 +5710,7 @@
         <v>228</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>229</v>
@@ -5634,7 +5766,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5642,7 +5774,7 @@
         <v>238</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>239</v>
@@ -5654,7 +5786,7 @@
         <v>240</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>241</v>
@@ -5666,7 +5798,7 @@
         <v>242</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>243</v>
@@ -5686,7 +5818,7 @@
         <v>245</v>
       </c>
       <c r="S8" s="47" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="T8" s="10" t="s">
         <v>602</v>
@@ -5724,10 +5856,10 @@
         <v>251</v>
       </c>
       <c r="AK8" s="8" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5735,7 +5867,7 @@
         <v>252</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>253</v>
@@ -5747,7 +5879,7 @@
         <v>254</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>255</v>
@@ -5759,7 +5891,7 @@
         <v>256</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>257</v>
@@ -5779,7 +5911,7 @@
         <v>259</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -5815,7 +5947,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5823,7 +5955,7 @@
         <v>266</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>267</v>
@@ -5841,7 +5973,7 @@
         <v>269</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>270</v>
@@ -5867,7 +5999,7 @@
         <v>273</v>
       </c>
       <c r="S10" s="47" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>146</v>
@@ -5912,7 +6044,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5932,7 +6064,7 @@
         <v>281</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>282</v>
@@ -5944,7 +6076,7 @@
         <v>283</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>284</v>
@@ -6005,7 +6137,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6013,7 +6145,7 @@
         <v>291</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>292</v>
@@ -6025,7 +6157,7 @@
         <v>293</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>294</v>
@@ -6037,7 +6169,7 @@
         <v>295</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>296</v>
@@ -6053,13 +6185,13 @@
         <v>297</v>
       </c>
       <c r="S12" s="47" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>216</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -6090,7 +6222,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6110,19 +6242,19 @@
         <v>304</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>305</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>306</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>307</v>
@@ -6135,10 +6267,10 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="10" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="S13" s="47" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>163</v>
@@ -6171,7 +6303,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6179,31 +6311,31 @@
         <v>309</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>311</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>312</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>313</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6231,7 +6363,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6243,7 +6375,7 @@
         <v>315</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>316</v>
@@ -6255,7 +6387,7 @@
         <v>317</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -6280,7 +6412,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6292,7 +6424,7 @@
         <v>319</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>320</v>
@@ -6304,7 +6436,7 @@
         <v>321</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -6329,7 +6461,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6341,7 +6473,7 @@
         <v>323</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>324</v>
@@ -6353,7 +6485,7 @@
         <v>325</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -6378,7 +6510,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6390,7 +6522,7 @@
         <v>326</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>327</v>
@@ -6402,7 +6534,7 @@
         <v>328</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -6427,7 +6559,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6439,13 +6571,13 @@
         <v>329</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>330</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>331</v>
@@ -6478,7 +6610,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6525,7 +6657,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6537,7 +6669,7 @@
         <v>334</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>335</v>
@@ -6572,7 +6704,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6615,7 +6747,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6632,7 +6764,7 @@
         <v>576</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -6660,7 +6792,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6674,7 +6806,7 @@
         <v>338</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -6703,7 +6835,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="75">
+    <row r="25" spans="1:37" ht="70" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6745,7 +6877,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6759,10 +6891,10 @@
         <v>340</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -6790,7 +6922,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -6798,11 +6930,11 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="40" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="I27" s="40"/>
       <c r="J27" s="40" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -6830,7 +6962,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="60">
+    <row r="28" spans="1:37" ht="56" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -6838,11 +6970,11 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="40" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="I28" s="40"/>
       <c r="J28" s="40" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -6870,16 +7002,16 @@
         <v>641</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ29" s="37" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="AK29" s="9" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6890,28 +7022,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.1640625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.25" customWidth="1"/>
+    <col min="7" max="7" width="20.75" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>341</v>
       </c>
@@ -6923,7 +7055,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -6955,7 +7087,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -6969,7 +7101,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -6983,7 +7115,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -6997,7 +7129,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57" customHeight="1">
+    <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -7023,7 +7155,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -7046,7 +7178,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -7063,7 +7195,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -7080,7 +7212,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="11" spans="1:12" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -7103,7 +7235,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:12" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -7114,13 +7246,13 @@
         <v>588</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="E12" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="90">
+    <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -7131,10 +7263,10 @@
         <v>589</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -7172,7 +7304,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -7189,7 +7321,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -7206,10 +7338,10 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>369</v>
       </c>
@@ -7227,7 +7359,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="150">
+    <row r="19" spans="1:12" ht="112" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>1</v>
       </c>
@@ -7253,7 +7385,7 @@
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
     </row>
-    <row r="20" spans="1:12" ht="30">
+    <row r="20" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="22">
         <v>2</v>
       </c>
@@ -7271,7 +7403,7 @@
         <v>374</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>682</v>
+        <v>886</v>
       </c>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
@@ -7279,22 +7411,22 @@
       <c r="K20" s="27"/>
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="1:12" ht="30">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="22">
         <v>3</v>
       </c>
       <c r="B21" s="45" t="s">
+        <v>682</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>683</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="D21" s="25" t="s">
         <v>684</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>685</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="26" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G21" s="29" t="s">
         <v>375</v>
@@ -7305,7 +7437,7 @@
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
     </row>
-    <row r="22" spans="1:12" ht="140.25">
+    <row r="22" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A22" s="22">
         <v>4</v>
       </c>
@@ -7316,30 +7448,30 @@
         <v>595</v>
       </c>
       <c r="D22" s="25" t="s">
+        <v>887</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>687</v>
       </c>
-      <c r="E22" s="25" t="s">
-        <v>688</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>689</v>
-      </c>
       <c r="G22" s="29" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>689</v>
+      </c>
+      <c r="K22" s="27" t="s">
         <v>690</v>
       </c>
-      <c r="J22" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>692</v>
-      </c>
       <c r="L22" s="27"/>
     </row>
-    <row r="23" spans="1:12" ht="140.25">
+    <row r="23" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <v>5</v>
       </c>
@@ -7347,10 +7479,10 @@
         <v>376</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="22"/>
@@ -7358,35 +7490,35 @@
         <v>377</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="I23" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>689</v>
+      </c>
+      <c r="K23" s="27" t="s">
         <v>690</v>
       </c>
-      <c r="J23" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="K23" s="27" t="s">
-        <v>692</v>
-      </c>
       <c r="L23" s="27"/>
     </row>
-    <row r="24" spans="1:12" ht="45">
+    <row r="24" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="22">
         <v>6</v>
       </c>
       <c r="B24" s="32" t="s">
+        <v>694</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>695</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>696</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>697</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>698</v>
       </c>
       <c r="E24" s="33"/>
       <c r="F24" s="22" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
@@ -7395,30 +7527,30 @@
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
     </row>
-    <row r="25" spans="1:12" ht="105">
+    <row r="25" spans="1:12" ht="84" x14ac:dyDescent="0.3">
       <c r="A25" s="22">
         <v>7</v>
       </c>
       <c r="B25" s="45" t="s">
+        <v>698</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>699</v>
+      </c>
+      <c r="D25" s="21" t="s">
         <v>700</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="E25" s="25" t="s">
         <v>701</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="F25" s="22" t="s">
         <v>702</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="G25" s="31" t="s">
         <v>703</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="H25" s="25" t="s">
         <v>704</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>705</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>706</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>668</v>
@@ -7431,15 +7563,15 @@
       </c>
       <c r="L25" s="27"/>
     </row>
-    <row r="26" spans="1:12" ht="255">
+    <row r="26" spans="1:12" ht="196" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <v>8</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>673</v>
@@ -7451,7 +7583,7 @@
         <v>378</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>671</v>
@@ -7460,21 +7592,21 @@
         <v>672</v>
       </c>
       <c r="J26" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="K26" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="L26" s="27" t="s">
         <v>690</v>
       </c>
-      <c r="K26" s="21" t="s">
-        <v>709</v>
-      </c>
-      <c r="L26" s="27" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="127.5">
+    </row>
+    <row r="27" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A27" s="22">
         <v>9</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>667</v>
@@ -7482,121 +7614,121 @@
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
       <c r="F27" s="22" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G27" s="31" t="s">
         <v>379</v>
       </c>
       <c r="H27" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>689</v>
+      </c>
+      <c r="J27" s="27" t="s">
         <v>690</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="J27" s="27" t="s">
-        <v>692</v>
       </c>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
     </row>
-    <row r="28" spans="1:12" ht="127.5">
+    <row r="28" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A28" s="22">
         <v>10</v>
       </c>
       <c r="B28" s="45" t="s">
+        <v>710</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>712</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>713</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>714</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="22" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G28" s="31" t="s">
         <v>380</v>
       </c>
       <c r="H28" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>689</v>
+      </c>
+      <c r="J28" s="27" t="s">
         <v>690</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="J28" s="27" t="s">
-        <v>692</v>
       </c>
       <c r="K28" s="27"/>
       <c r="L28" s="27"/>
     </row>
-    <row r="29" spans="1:12" ht="127.5">
+    <row r="29" spans="1:12" ht="117" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <v>11</v>
       </c>
       <c r="B29" s="28" t="s">
+        <v>714</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>715</v>
+      </c>
+      <c r="D29" s="25" t="s">
         <v>716</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>717</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>718</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="22" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G29" s="31" t="s">
         <v>381</v>
       </c>
       <c r="H29" s="21" t="s">
+        <v>688</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>689</v>
+      </c>
+      <c r="J29" s="27" t="s">
         <v>690</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>691</v>
-      </c>
-      <c r="J29" s="27" t="s">
-        <v>692</v>
       </c>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
     </row>
-    <row r="30" spans="1:12" ht="210">
+    <row r="30" spans="1:12" ht="168" x14ac:dyDescent="0.3">
       <c r="A30" s="22">
         <v>12</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>382</v>
       </c>
       <c r="E30" s="25"/>
       <c r="F30" s="22" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G30" s="31" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
       <c r="L30" s="27"/>
     </row>
-    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22">
         <v>13</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>593</v>
@@ -7605,7 +7737,7 @@
         <v>383</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
@@ -7615,18 +7747,18 @@
       <c r="K31" s="27"/>
       <c r="L31" s="27"/>
     </row>
-    <row r="32" spans="1:12" ht="30">
+    <row r="32" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <v>14</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>594</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>384</v>
@@ -7639,7 +7771,7 @@
       <c r="K32" s="27"/>
       <c r="L32" s="27"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>15</v>
       </c>
@@ -7654,7 +7786,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7668,188 +7800,188 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="35"/>
-    <col min="2" max="2" width="20.140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="35"/>
-    <col min="4" max="4" width="34.42578125" style="35" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="35"/>
-    <col min="6" max="6" width="27.28515625" style="35" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="35"/>
-    <col min="8" max="8" width="29.7109375" style="35" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="35" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.75" style="35"/>
+    <col min="2" max="2" width="20.1640625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="8.75" style="35"/>
+    <col min="4" max="4" width="34.4140625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="8.75" style="35"/>
+    <col min="6" max="6" width="27.25" style="35" customWidth="1"/>
+    <col min="7" max="7" width="8.75" style="35"/>
+    <col min="8" max="8" width="29.75" style="35" customWidth="1"/>
+    <col min="9" max="9" width="12.75" style="35" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>728</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>730</v>
+      </c>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="B2" s="13" t="s">
-        <v>728</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>730</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>732</v>
-      </c>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" ht="45">
-      <c r="B3" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>729</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>731</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>733</v>
       </c>
       <c r="G3" s="35">
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="G4" s="35">
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D5" s="36" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G5" s="35">
         <v>3</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="90">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
       <c r="D6" s="36" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G6" s="35">
         <v>4</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="150">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G7" s="35">
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G8" s="35">
         <v>6</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9" ht="105">
+    <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="D9" s="36" t="s">
+        <v>752</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>754</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>756</v>
       </c>
       <c r="G9" s="35">
         <v>7</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D10" s="13" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G10" s="35">
         <v>8</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="F11" s="13" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G11" s="35">
         <v>9</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D12" s="13" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="G12" s="35">
         <v>10</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="45">
+    <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="F14" s="42" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -7864,18 +7996,18 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.95" customHeight="1">
+    <row r="1" spans="1:2" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7884,7 +8016,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7898,18 +8030,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7917,7 +8049,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7925,7 +8057,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7933,7 +8065,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7941,7 +8073,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7949,7 +8081,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7957,7 +8089,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7965,7 +8097,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7974,7 +8106,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7988,14 +8120,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
something new（pump 2022.9.7 19.13
</commit_message>
<xml_diff>
--- a/参考/资料/企划20200806.xlsx
+++ b/参考/资料/企划20200806.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\micro_machinery\参考\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89FB860-53B6-408C-BD1E-79CB28915517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02042D5C-03EE-41C6-A682-FBB233CE813E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,6 +56,30 @@
 物流管道应当全部删除；
 新增三个等级的传送带；
 流体管道模型应当重置（dbydd有一些疯狂的想法）；</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{221D5BB2-6383-4012-974D-420536EE51DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>hqyzsy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+传动模块待删除，仅保留复杂传动模块</t>
         </r>
       </text>
     </comment>
@@ -1955,9 +1979,6 @@
     <t>cast_sword</t>
   </si>
   <si>
-    <t>wafer</t>
-  </si>
-  <si>
     <t>i7_8700k</t>
   </si>
   <si>
@@ -3844,12 +3865,16 @@
     <t>每tick发电40fe</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>wafer</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4001,6 +4026,19 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
@@ -4741,8 +4779,8 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H4" sqref="H4:I4"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4795,7 +4833,7 @@
         <v>8</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -4812,7 +4850,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -4830,7 +4868,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -4842,13 +4880,13 @@
         <v>15</v>
       </c>
       <c r="O2" s="44" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="R2" s="8"/>
       <c r="S2" t="s">
@@ -4872,7 +4910,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -4902,13 +4940,13 @@
         <v>24</v>
       </c>
       <c r="O3" s="44" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="P3" t="s">
         <v>25</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" t="s">
@@ -4932,7 +4970,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -4956,19 +4994,19 @@
         <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="N4" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="44" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="R4" s="8"/>
       <c r="S4" t="s">
@@ -4992,7 +5030,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
@@ -5016,22 +5054,22 @@
         <v>41</v>
       </c>
       <c r="M5" s="44" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="44" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="P5" t="s">
         <v>43</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="R5" s="50" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="S5" t="s">
         <v>44</v>
@@ -5054,7 +5092,7 @@
         <v>46</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -5072,7 +5110,7 @@
         <v>49</v>
       </c>
       <c r="M6" s="44" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N6" t="s">
         <v>50</v>
@@ -5084,10 +5122,10 @@
         <v>51</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="R6" s="51" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="S6" t="s">
         <v>52</v>
@@ -5110,7 +5148,7 @@
         <v>54</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F7" t="s">
         <v>55</v>
@@ -5134,7 +5172,7 @@
         <v>58</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="R7" s="8"/>
       <c r="S7" t="s">
@@ -5158,7 +5196,7 @@
         <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F8" t="s">
         <v>62</v>
@@ -5167,7 +5205,7 @@
         <v>408</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="M8" s="44" t="s">
         <v>427</v>
@@ -5182,7 +5220,7 @@
         <v>64</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="R8" s="8"/>
       <c r="S8" t="s">
@@ -5206,7 +5244,7 @@
         <v>67</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
@@ -5230,7 +5268,7 @@
         <v>70</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="R9" s="8"/>
       <c r="S9" t="s">
@@ -5254,7 +5292,7 @@
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
@@ -5263,16 +5301,16 @@
         <v>409</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="P10" t="s">
         <v>75</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R10" s="8"/>
       <c r="S10" t="s">
@@ -5296,7 +5334,7 @@
         <v>78</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F11" t="s">
         <v>79</v>
@@ -5308,7 +5346,7 @@
         <v>80</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" t="s">
@@ -5332,7 +5370,7 @@
         <v>83</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F12" t="s">
         <v>84</v>
@@ -5341,13 +5379,13 @@
         <v>411</v>
       </c>
       <c r="N12" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="R12" s="8"/>
       <c r="S12" t="s">
@@ -5371,7 +5409,7 @@
         <v>87</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
@@ -5380,13 +5418,13 @@
         <v>414</v>
       </c>
       <c r="N13" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="P13" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="Q13" s="44" t="s">
         <v>707</v>
-      </c>
-      <c r="Q13" s="44" t="s">
-        <v>708</v>
       </c>
       <c r="R13" s="44"/>
       <c r="S13" t="s">
@@ -5410,7 +5448,7 @@
         <v>91</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F14" t="s">
         <v>92</v>
@@ -5419,7 +5457,7 @@
         <v>415</v>
       </c>
       <c r="N14" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="S14" t="s">
         <v>97</v>
@@ -5442,7 +5480,7 @@
         <v>95</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F15" t="s">
         <v>96</v>
@@ -5471,7 +5509,7 @@
         <v>99</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F16" t="s">
         <v>100</v>
@@ -5480,7 +5518,7 @@
         <v>417</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="S16" t="s">
         <v>105</v>
@@ -5503,7 +5541,7 @@
         <v>103</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F17" t="s">
         <v>104</v>
@@ -5512,10 +5550,10 @@
         <v>418</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="S17" t="s">
         <v>108</v>
@@ -5538,7 +5576,7 @@
         <v>106</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F18" t="s">
         <v>107</v>
@@ -5547,10 +5585,10 @@
         <v>419</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="S18" t="s">
         <v>111</v>
@@ -5567,7 +5605,7 @@
         <v>109</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
@@ -5663,7 +5701,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ32" sqref="AJ32"/>
+      <selection pane="topRight" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5775,13 +5813,13 @@
         <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>140</v>
@@ -5793,7 +5831,7 @@
         <v>141</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>142</v>
@@ -5805,37 +5843,37 @@
         <v>143</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>144</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>145</v>
       </c>
       <c r="S2" s="46" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>181</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>149</v>
       </c>
       <c r="AA2" s="46" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AB2" s="5" t="s">
         <v>132</v>
@@ -5859,13 +5897,13 @@
         <v>152</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="AJ2" s="5" t="s">
         <v>153</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.3">
@@ -5900,7 +5938,7 @@
         <v>158</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>159</v>
@@ -5924,19 +5962,19 @@
         <v>162</v>
       </c>
       <c r="S3" s="46" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>197</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="V3" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="W3" s="9" t="s">
         <v>587</v>
-      </c>
-      <c r="W3" s="9" t="s">
-        <v>588</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>165</v>
@@ -5948,13 +5986,13 @@
         <v>166</v>
       </c>
       <c r="AA3" s="46" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AB3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>168</v>
@@ -5978,7 +6016,7 @@
         <v>171</v>
       </c>
       <c r="AK3" s="8" t="s">
-        <v>554</v>
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
@@ -5989,19 +6027,19 @@
         <v>172</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>174</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>175</v>
@@ -6013,7 +6051,7 @@
         <v>176</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>177</v>
@@ -6037,13 +6075,13 @@
         <v>180</v>
       </c>
       <c r="S4" s="46" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>231</v>
       </c>
       <c r="U4" s="9" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="W4" s="5"/>
       <c r="X4" s="5" t="s">
@@ -6086,7 +6124,7 @@
         <v>205</v>
       </c>
       <c r="AK4" s="44" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.3">
@@ -6109,7 +6147,7 @@
         <v>190</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>191</v>
@@ -6121,7 +6159,7 @@
         <v>192</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>193</v>
@@ -6145,7 +6183,7 @@
         <v>196</v>
       </c>
       <c r="S5" s="46" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="U5" s="5"/>
       <c r="W5" s="5"/>
@@ -6165,7 +6203,7 @@
         <v>201</v>
       </c>
       <c r="AC5" s="8" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>202</v>
@@ -6186,10 +6224,10 @@
         <v>445</v>
       </c>
       <c r="AJ5" s="16" t="s">
+        <v>834</v>
+      </c>
+      <c r="AK5" s="8" t="s">
         <v>835</v>
-      </c>
-      <c r="AK5" s="8" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
@@ -6200,7 +6238,7 @@
         <v>206</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>207</v>
@@ -6212,7 +6250,7 @@
         <v>208</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>209</v>
@@ -6224,7 +6262,7 @@
         <v>210</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>211</v>
@@ -6236,7 +6274,7 @@
         <v>212</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>213</v>
@@ -6248,13 +6286,13 @@
         <v>214</v>
       </c>
       <c r="S6" s="46" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>257</v>
       </c>
       <c r="U6" s="9" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>216</v>
@@ -6278,7 +6316,7 @@
         <v>219</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>220</v>
@@ -6293,10 +6331,10 @@
         <v>437</v>
       </c>
       <c r="AJ6" s="16" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="AK6" s="8" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -6319,7 +6357,7 @@
         <v>225</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>226</v>
@@ -6331,7 +6369,7 @@
         <v>227</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>228</v>
@@ -6372,7 +6410,7 @@
         <v>234</v>
       </c>
       <c r="AC7" s="44" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AF7" s="5" t="s">
         <v>235</v>
@@ -6384,7 +6422,7 @@
         <v>262</v>
       </c>
       <c r="AK7" s="8" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -6395,7 +6433,7 @@
         <v>236</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>237</v>
@@ -6407,7 +6445,7 @@
         <v>238</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>239</v>
@@ -6419,7 +6457,7 @@
         <v>240</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>241</v>
@@ -6439,13 +6477,13 @@
         <v>243</v>
       </c>
       <c r="S8" s="46" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="T8" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="U8" s="9" t="s">
         <v>589</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>590</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="9"/>
@@ -6477,7 +6515,7 @@
         <v>275</v>
       </c>
       <c r="AK8" s="44" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -6488,7 +6526,7 @@
         <v>249</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>250</v>
@@ -6500,7 +6538,7 @@
         <v>251</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>252</v>
@@ -6512,7 +6550,7 @@
         <v>253</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>254</v>
@@ -6532,7 +6570,7 @@
         <v>256</v>
       </c>
       <c r="S9" s="46" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
@@ -6565,7 +6603,7 @@
         <v>287</v>
       </c>
       <c r="AK9" s="44" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -6576,7 +6614,7 @@
         <v>263</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>264</v>
@@ -6594,7 +6632,7 @@
         <v>266</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>267</v>
@@ -6620,7 +6658,7 @@
         <v>270</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>146</v>
@@ -6662,7 +6700,7 @@
         <v>298</v>
       </c>
       <c r="AK10" s="8" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -6685,7 +6723,7 @@
         <v>278</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>279</v>
@@ -6697,7 +6735,7 @@
         <v>280</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>281</v>
@@ -6755,7 +6793,7 @@
         <v>305</v>
       </c>
       <c r="AK11" s="8" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
@@ -6766,7 +6804,7 @@
         <v>288</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>289</v>
@@ -6778,7 +6816,7 @@
         <v>290</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>291</v>
@@ -6790,7 +6828,7 @@
         <v>292</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>293</v>
@@ -6806,13 +6844,13 @@
         <v>294</v>
       </c>
       <c r="S12" s="46" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>215</v>
       </c>
       <c r="U12" s="9" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -6840,7 +6878,7 @@
         <v>311</v>
       </c>
       <c r="AK12" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
@@ -6863,19 +6901,19 @@
         <v>301</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>302</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>303</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>304</v>
@@ -6888,10 +6926,10 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="10" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="S13" s="46" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="T13" s="5" t="s">
         <v>163</v>
@@ -6912,16 +6950,16 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AF13" s="39" t="s">
+        <v>584</v>
+      </c>
+      <c r="AG13" s="44" t="s">
         <v>585</v>
-      </c>
-      <c r="AG13" s="44" t="s">
-        <v>586</v>
       </c>
       <c r="AJ13" s="5" t="s">
         <v>315</v>
       </c>
       <c r="AK13" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
@@ -6932,31 +6970,31 @@
         <v>306</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>307</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>308</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>309</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>310</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -6981,7 +7019,7 @@
         <v>319</v>
       </c>
       <c r="AK14" s="44" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
@@ -6996,7 +7034,7 @@
         <v>312</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>313</v>
@@ -7008,7 +7046,7 @@
         <v>314</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -7045,7 +7083,7 @@
         <v>316</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>317</v>
@@ -7057,7 +7095,7 @@
         <v>318</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -7094,7 +7132,7 @@
         <v>320</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>321</v>
@@ -7106,7 +7144,7 @@
         <v>322</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
@@ -7125,10 +7163,10 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AJ17" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="AK17" s="44" t="s">
         <v>596</v>
-      </c>
-      <c r="AK17" s="44" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.3">
@@ -7143,7 +7181,7 @@
         <v>323</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>324</v>
@@ -7155,7 +7193,7 @@
         <v>325</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
@@ -7192,13 +7230,13 @@
         <v>326</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>327</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>328</v>
@@ -7225,10 +7263,10 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AJ19" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="AK19" s="44" t="s">
         <v>565</v>
-      </c>
-      <c r="AK19" s="44" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -7272,10 +7310,10 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AJ20" s="10" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AK20" s="44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -7290,7 +7328,7 @@
         <v>331</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>332</v>
@@ -7319,10 +7357,10 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AJ21" s="10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AK21" s="44" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.3">
@@ -7362,10 +7400,10 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AJ22" s="16" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AK22" s="44" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="23" spans="1:37" ht="70" x14ac:dyDescent="0.3">
@@ -7382,10 +7420,10 @@
         <v>334</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -7407,10 +7445,10 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AJ23" s="20" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AK23" s="9" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.3">
@@ -7427,7 +7465,7 @@
         <v>335</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -7450,10 +7488,10 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AJ24" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AK24" s="9" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.3">
@@ -7492,10 +7530,10 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AJ25" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AK25" s="9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="26" spans="1:37" ht="56" x14ac:dyDescent="0.3">
@@ -7512,10 +7550,10 @@
         <v>337</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -7537,10 +7575,10 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AJ26" s="38" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AK26" s="9" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.3">
@@ -7551,11 +7589,11 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="40" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I27" s="40"/>
       <c r="J27" s="40" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -7577,10 +7615,10 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AJ27" s="37" t="s">
+        <v>708</v>
+      </c>
+      <c r="AK27" s="9" t="s">
         <v>709</v>
-      </c>
-      <c r="AK27" s="9" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.3">
@@ -7591,11 +7629,11 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="40" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="I28" s="40"/>
       <c r="J28" s="40" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -7619,23 +7657,23 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ29" s="7" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ30" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="AK30" s="9" t="s">
         <v>860</v>
-      </c>
-      <c r="AK30" s="9" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AJ31" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="AK31" s="9" t="s">
         <v>863</v>
-      </c>
-      <c r="AK31" s="9" t="s">
-        <v>864</v>
       </c>
     </row>
   </sheetData>
@@ -7650,8 +7688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7668,7 +7706,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7691,10 +7729,10 @@
         <v>341</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E3" t="s">
         <v>342</v>
@@ -7712,7 +7750,7 @@
         <v>346</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7723,10 +7761,10 @@
         <v>347</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7737,10 +7775,10 @@
         <v>348</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7751,10 +7789,10 @@
         <v>349</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -7765,22 +7803,22 @@
         <v>350</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>598</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>600</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7788,13 +7826,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E8" t="s">
         <v>351</v>
@@ -7803,7 +7841,7 @@
         <v>352</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7814,10 +7852,10 @@
         <v>353</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E9" t="s">
         <v>354</v>
@@ -7828,13 +7866,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="47" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E10" t="s">
         <v>355</v>
@@ -7851,13 +7889,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E11" t="s">
         <v>358</v>
@@ -7868,13 +7906,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7882,13 +7920,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E13" t="s">
         <v>133</v>
@@ -7912,7 +7950,7 @@
         <v>360</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7923,10 +7961,10 @@
         <v>361</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7937,10 +7975,10 @@
         <v>362</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -7955,10 +7993,10 @@
         <v>364</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>840</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>841</v>
       </c>
       <c r="G17" t="s">
         <v>340</v>
@@ -7972,16 +8010,16 @@
         <v>365</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D18" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>848</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>847</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>849</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>848</v>
       </c>
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
@@ -7995,22 +8033,22 @@
         <v>2</v>
       </c>
       <c r="B19" s="45" t="s">
+        <v>646</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>923</v>
+      </c>
+      <c r="D19" s="25" t="s">
         <v>647</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>924</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>648</v>
-      </c>
       <c r="E19" s="25" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>366</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
@@ -8023,19 +8061,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="45" t="s">
+        <v>648</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>924</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>649</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>925</v>
-      </c>
-      <c r="D20" s="25" t="s">
+      <c r="E20" s="25" t="s">
+        <v>849</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>650</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>850</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>651</v>
       </c>
       <c r="G20" s="29" t="s">
         <v>367</v>
@@ -8051,30 +8089,30 @@
         <v>4</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F21" s="26"/>
       <c r="G21" s="31" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="K21" s="27" t="s">
         <v>652</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>913</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>653</v>
       </c>
       <c r="L21" s="27"/>
     </row>
@@ -8086,29 +8124,29 @@
         <v>368</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="31" t="s">
         <v>369</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I22" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="K22" s="27" t="s">
         <v>652</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>913</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>653</v>
       </c>
       <c r="L22" s="27"/>
     </row>
@@ -8117,17 +8155,17 @@
         <v>6</v>
       </c>
       <c r="B23" s="32" t="s">
+        <v>655</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>656</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="D23" s="21" t="s">
         <v>657</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>658</v>
       </c>
       <c r="E23" s="33"/>
       <c r="F23" s="22" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -8141,32 +8179,32 @@
         <v>7</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="31" t="s">
+        <v>660</v>
+      </c>
+      <c r="H24" s="25" t="s">
         <v>661</v>
       </c>
-      <c r="H24" s="25" t="s">
-        <v>662</v>
-      </c>
       <c r="I24" s="21" t="s">
+        <v>641</v>
+      </c>
+      <c r="J24" s="21" t="s">
         <v>642</v>
       </c>
-      <c r="J24" s="21" t="s">
-        <v>643</v>
-      </c>
       <c r="K24" s="21" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="L24" s="27"/>
     </row>
@@ -8175,37 +8213,37 @@
         <v>8</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F25" s="22" t="s">
         <v>370</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J25" s="21" t="s">
+        <v>913</v>
+      </c>
+      <c r="K25" s="21" t="s">
         <v>914</v>
       </c>
-      <c r="K25" s="21" t="s">
-        <v>915</v>
-      </c>
       <c r="L25" s="27" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="104" x14ac:dyDescent="0.3">
@@ -8213,31 +8251,31 @@
         <v>9</v>
       </c>
       <c r="B26" s="30" t="s">
+        <v>663</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>928</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>844</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>842</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>664</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>929</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>845</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>843</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>665</v>
       </c>
       <c r="G26" s="31" t="s">
         <v>371</v>
       </c>
       <c r="I26" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="K26" s="27" t="s">
         <v>652</v>
-      </c>
-      <c r="J26" s="21" t="s">
-        <v>913</v>
-      </c>
-      <c r="K26" s="27" t="s">
-        <v>653</v>
       </c>
       <c r="L26" s="27"/>
     </row>
@@ -8246,29 +8284,29 @@
         <v>10</v>
       </c>
       <c r="B27" s="45" t="s">
+        <v>665</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>929</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>666</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>930</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>667</v>
-      </c>
       <c r="E27" s="25" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="31" t="s">
         <v>372</v>
       </c>
       <c r="I27" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="K27" s="27" t="s">
         <v>652</v>
-      </c>
-      <c r="J27" s="21" t="s">
-        <v>913</v>
-      </c>
-      <c r="K27" s="27" t="s">
-        <v>653</v>
       </c>
       <c r="L27" s="27"/>
     </row>
@@ -8277,13 +8315,13 @@
         <v>11</v>
       </c>
       <c r="B28" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>668</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="D28" s="25" t="s">
         <v>669</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>670</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="22"/>
@@ -8291,13 +8329,13 @@
         <v>373</v>
       </c>
       <c r="I28" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="K28" s="27" t="s">
         <v>652</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>913</v>
-      </c>
-      <c r="K28" s="27" t="s">
-        <v>653</v>
       </c>
       <c r="L28" s="27"/>
     </row>
@@ -8306,21 +8344,21 @@
         <v>12</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="25" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="31" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
@@ -8332,16 +8370,16 @@
         <v>13</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>374</v>
       </c>
       <c r="E30" s="33" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F30" s="27"/>
       <c r="G30" s="27"/>
@@ -8356,13 +8394,13 @@
         <v>14</v>
       </c>
       <c r="B31" s="28" t="s">
+        <v>672</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>673</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>581</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>674</v>
       </c>
       <c r="E31" s="33"/>
       <c r="F31" s="27"/>
@@ -8378,99 +8416,99 @@
         <v>15</v>
       </c>
       <c r="B32" s="34" t="s">
+        <v>638</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>639</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>839</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="59" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B35" s="56" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="59"/>
       <c r="B36" s="57"/>
       <c r="C36" s="52" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="59"/>
       <c r="B37" s="57"/>
       <c r="C37" s="52" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>892</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>893</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="59"/>
       <c r="B38" s="57"/>
       <c r="C38" s="52" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="59"/>
       <c r="B39" s="57"/>
       <c r="C39" s="52" t="s">
+        <v>869</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>870</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="59"/>
       <c r="B40" s="57"/>
       <c r="C40" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>872</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="59"/>
       <c r="B41" s="57"/>
       <c r="C41" s="56" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -8478,7 +8516,7 @@
       <c r="B42" s="57"/>
       <c r="C42" s="56"/>
       <c r="D42" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -8486,27 +8524,27 @@
       <c r="B43" s="57"/>
       <c r="C43" s="56"/>
       <c r="D43" s="7" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="59"/>
       <c r="B44" s="57"/>
       <c r="C44" s="53" t="s">
+        <v>879</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>880</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="59"/>
       <c r="B45" s="57"/>
       <c r="C45" s="53" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -8517,98 +8555,98 @@
     <row r="47" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="59"/>
       <c r="B47" s="58" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C47" s="53" t="s">
+        <v>881</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>882</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="59"/>
       <c r="B48" s="58"/>
       <c r="C48" s="53" t="s">
+        <v>883</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>884</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>885</v>
-      </c>
       <c r="E48" s="7" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="59"/>
       <c r="B49" s="58"/>
       <c r="C49" s="53" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="59"/>
       <c r="B50" s="58"/>
       <c r="C50" s="53" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="59"/>
       <c r="B51" s="58"/>
       <c r="C51" s="53" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="59"/>
       <c r="B52" s="58"/>
       <c r="C52" s="53" t="s">
+        <v>894</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>895</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="59"/>
       <c r="B53" s="58"/>
       <c r="D53" s="7" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="59"/>
       <c r="B54" s="58"/>
       <c r="D54" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D56" s="7" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D57" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D58" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -8649,36 +8687,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G3" s="35">
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.3">
@@ -8686,131 +8724,131 @@
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D5" s="36" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G5" s="35">
         <v>3</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="70" x14ac:dyDescent="0.3">
       <c r="D6" s="36" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G6" s="35">
         <v>4</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.3">
       <c r="D7" s="13" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G7" s="35">
         <v>5</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D8" s="13" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G8" s="35">
         <v>6</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="D9" s="36" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="G9" s="35">
         <v>7</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="56" x14ac:dyDescent="0.3">
       <c r="D10" s="13" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G10" s="35">
         <v>8</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="F11" s="13" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G11" s="35">
         <v>9</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28" x14ac:dyDescent="0.3">
       <c r="D12" s="13" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G12" s="35">
         <v>10</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="D13" s="13" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="F14" s="42" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>
@@ -8845,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>
@@ -8860,7 +8898,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8871,7 +8909,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -8879,7 +8917,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8887,7 +8925,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8895,7 +8933,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -8903,7 +8941,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -8911,7 +8949,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -8919,7 +8957,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -8927,7 +8965,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -8935,7 +8973,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -8957,7 +8995,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>